<commit_message>
Update equations and log
</commit_message>
<xml_diff>
--- a/Simulation_log_key.xlsx
+++ b/Simulation_log_key.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\Documents\R\working_directory\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zeus\Documents\R\working_directory\LemonSharkCKMR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91E399B0-55D8-4647-AD40-9F0C9BAD6A7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9682CCB3-614B-4A93-81D8-A7129EE64B08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5085" yWindow="-11640" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="1" xr2:uid="{24E2991C-2C0C-4843-9426-0DC9EB9B25FD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="2" xr2:uid="{24E2991C-2C0C-4843-9426-0DC9EB9B25FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Bayesian_model_validation" sheetId="3" state="hidden" r:id="rId1"/>
@@ -2725,33 +2725,33 @@
       <selection pane="topRight" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="59.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="59.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.33203125" customWidth="1"/>
-    <col min="5" max="5" width="39.5546875" customWidth="1"/>
-    <col min="6" max="6" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="15" width="31.5546875" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" customWidth="1"/>
+    <col min="5" max="5" width="39.5703125" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="15" width="31.5703125" customWidth="1"/>
     <col min="16" max="16" width="51" customWidth="1"/>
-    <col min="17" max="17" width="49.6640625" style="39" customWidth="1"/>
-    <col min="18" max="21" width="19.5546875" customWidth="1"/>
-    <col min="22" max="23" width="25.33203125" customWidth="1"/>
+    <col min="17" max="17" width="49.7109375" style="39" customWidth="1"/>
+    <col min="18" max="21" width="19.5703125" customWidth="1"/>
+    <col min="22" max="23" width="25.28515625" customWidth="1"/>
     <col min="24" max="24" width="16" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="33.109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="33.140625" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="16" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="33.109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="33.140625" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="16" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="33.109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="33.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="99" t="s">
         <v>105</v>
       </c>
@@ -2840,7 +2840,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:29" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:29" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="100" t="s">
         <v>106</v>
       </c>
@@ -2891,7 +2891,7 @@
       <c r="AB2" s="63"/>
       <c r="AC2" s="64"/>
     </row>
-    <row r="3" spans="1:29" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:29" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="103" t="s">
         <v>107</v>
       </c>
@@ -2942,7 +2942,7 @@
       <c r="AB3" s="65"/>
       <c r="AC3" s="66"/>
     </row>
-    <row r="4" spans="1:29" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:29" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="103" t="s">
         <v>108</v>
       </c>
@@ -2993,7 +2993,7 @@
       <c r="AB4" s="65"/>
       <c r="AC4" s="66"/>
     </row>
-    <row r="5" spans="1:29" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:29" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="91" t="s">
         <v>115</v>
       </c>
@@ -3042,7 +3042,7 @@
       <c r="AB5" s="65"/>
       <c r="AC5" s="66"/>
     </row>
-    <row r="6" spans="1:29" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:29" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="91" t="s">
         <v>116</v>
       </c>
@@ -3095,7 +3095,7 @@
       <c r="AB6" s="65"/>
       <c r="AC6" s="66"/>
     </row>
-    <row r="7" spans="1:29" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:29" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="91" t="s">
         <v>117</v>
       </c>
@@ -3142,7 +3142,7 @@
       <c r="AB7" s="65"/>
       <c r="AC7" s="66"/>
     </row>
-    <row r="8" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="91" t="s">
         <v>128</v>
       </c>
@@ -3175,7 +3175,7 @@
       <c r="AB8" s="65"/>
       <c r="AC8" s="66"/>
     </row>
-    <row r="9" spans="1:29" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:29" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="91" t="s">
         <v>129</v>
       </c>
@@ -3222,7 +3222,7 @@
       <c r="AB9" s="67"/>
       <c r="AC9" s="68"/>
     </row>
-    <row r="10" spans="1:29" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:29" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="91" t="s">
         <v>131</v>
       </c>
@@ -3279,7 +3279,7 @@
       <c r="AB10" s="67"/>
       <c r="AC10" s="68"/>
     </row>
-    <row r="11" spans="1:29" ht="72" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:29" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="91" t="s">
         <v>144</v>
       </c>
@@ -3332,7 +3332,7 @@
       <c r="AB11" s="67"/>
       <c r="AC11" s="68"/>
     </row>
-    <row r="12" spans="1:29" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:29" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="90" t="s">
         <v>146</v>
       </c>
@@ -3391,7 +3391,7 @@
       <c r="AB12" s="67"/>
       <c r="AC12" s="68"/>
     </row>
-    <row r="13" spans="1:29" ht="72" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:29" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="90" t="s">
         <v>152</v>
       </c>
@@ -3452,7 +3452,7 @@
       <c r="AB13" s="67"/>
       <c r="AC13" s="68"/>
     </row>
-    <row r="14" spans="1:29" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:29" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="90" t="s">
         <v>178</v>
       </c>
@@ -3511,7 +3511,7 @@
       <c r="AB14" s="69"/>
       <c r="AC14" s="70"/>
     </row>
-    <row r="15" spans="1:29" ht="72" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:29" ht="90" x14ac:dyDescent="0.25">
       <c r="A15" s="90" t="s">
         <v>134</v>
       </c>
@@ -3572,7 +3572,7 @@
       <c r="AB15" s="67"/>
       <c r="AC15" s="68"/>
     </row>
-    <row r="16" spans="1:29" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:29" ht="105" x14ac:dyDescent="0.25">
       <c r="A16" s="90" t="s">
         <v>134</v>
       </c>
@@ -3633,7 +3633,7 @@
       <c r="AB16" s="69"/>
       <c r="AC16" s="70"/>
     </row>
-    <row r="17" spans="1:29" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:29" ht="180" x14ac:dyDescent="0.25">
       <c r="A17" s="91" t="s">
         <v>193</v>
       </c>
@@ -3696,7 +3696,7 @@
       <c r="AB17" s="69"/>
       <c r="AC17" s="70"/>
     </row>
-    <row r="18" spans="1:29" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:29" ht="120" x14ac:dyDescent="0.25">
       <c r="A18" s="91" t="s">
         <v>202</v>
       </c>
@@ -3745,7 +3745,7 @@
       <c r="AB18" s="69"/>
       <c r="AC18" s="70"/>
     </row>
-    <row r="19" spans="1:29" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:29" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="91" t="s">
         <v>202</v>
       </c>
@@ -3794,7 +3794,7 @@
       <c r="AB19" s="69"/>
       <c r="AC19" s="70"/>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A20" s="91" t="s">
         <v>205</v>
       </c>
@@ -3829,7 +3829,7 @@
       <c r="AB20" s="69"/>
       <c r="AC20" s="70"/>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A21" s="91"/>
       <c r="B21" s="91"/>
       <c r="C21" s="103"/>
@@ -3860,7 +3860,7 @@
       <c r="AB21" s="69"/>
       <c r="AC21" s="70"/>
     </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A22" s="91"/>
       <c r="B22" s="91"/>
       <c r="C22" s="103"/>
@@ -3891,7 +3891,7 @@
       <c r="AB22" s="69"/>
       <c r="AC22" s="70"/>
     </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A23" s="91"/>
       <c r="B23" s="91"/>
       <c r="C23" s="103"/>
@@ -3922,7 +3922,7 @@
       <c r="AB23" s="69"/>
       <c r="AC23" s="70"/>
     </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A24" s="91"/>
       <c r="B24" s="91"/>
       <c r="C24" s="103"/>
@@ -3953,7 +3953,7 @@
       <c r="AB24" s="69"/>
       <c r="AC24" s="70"/>
     </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A25" s="91"/>
       <c r="B25" s="91"/>
       <c r="C25" s="103"/>
@@ -3984,7 +3984,7 @@
       <c r="AB25" s="69"/>
       <c r="AC25" s="70"/>
     </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A26" s="91"/>
       <c r="B26" s="91"/>
       <c r="C26" s="103"/>
@@ -4015,7 +4015,7 @@
       <c r="AB26" s="69"/>
       <c r="AC26" s="70"/>
     </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A27" s="91"/>
       <c r="B27" s="91"/>
       <c r="C27" s="103"/>
@@ -4046,7 +4046,7 @@
       <c r="AB27" s="69"/>
       <c r="AC27" s="70"/>
     </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A28" s="91"/>
       <c r="B28" s="91"/>
       <c r="C28" s="103"/>
@@ -4077,7 +4077,7 @@
       <c r="AB28" s="69"/>
       <c r="AC28" s="70"/>
     </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A29" s="91"/>
       <c r="B29" s="91"/>
       <c r="C29" s="103"/>
@@ -4108,7 +4108,7 @@
       <c r="AB29" s="69"/>
       <c r="AC29" s="70"/>
     </row>
-    <row r="30" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A30" s="91"/>
       <c r="B30" s="91"/>
       <c r="C30" s="103"/>
@@ -4139,7 +4139,7 @@
       <c r="AB30" s="69"/>
       <c r="AC30" s="70"/>
     </row>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A31" s="91"/>
       <c r="B31" s="91"/>
       <c r="C31" s="103"/>
@@ -4170,7 +4170,7 @@
       <c r="AB31" s="69"/>
       <c r="AC31" s="70"/>
     </row>
-    <row r="32" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A32" s="91"/>
       <c r="B32" s="91"/>
       <c r="C32" s="103"/>
@@ -4201,7 +4201,7 @@
       <c r="AB32" s="69"/>
       <c r="AC32" s="70"/>
     </row>
-    <row r="33" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A33" s="91"/>
       <c r="B33" s="91"/>
       <c r="C33" s="103"/>
@@ -4232,7 +4232,7 @@
       <c r="AB33" s="69"/>
       <c r="AC33" s="70"/>
     </row>
-    <row r="34" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A34" s="91"/>
       <c r="B34" s="91"/>
       <c r="C34" s="103"/>
@@ -4263,7 +4263,7 @@
       <c r="AB34" s="69"/>
       <c r="AC34" s="70"/>
     </row>
-    <row r="35" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A35" s="91"/>
       <c r="B35" s="91"/>
       <c r="C35" s="103"/>
@@ -4294,7 +4294,7 @@
       <c r="AB35" s="69"/>
       <c r="AC35" s="70"/>
     </row>
-    <row r="36" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A36" s="91"/>
       <c r="B36" s="91"/>
       <c r="C36" s="103"/>
@@ -4325,7 +4325,7 @@
       <c r="AB36" s="69"/>
       <c r="AC36" s="70"/>
     </row>
-    <row r="37" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A37" s="91"/>
       <c r="B37" s="91"/>
       <c r="C37" s="103"/>
@@ -4356,7 +4356,7 @@
       <c r="AB37" s="69"/>
       <c r="AC37" s="70"/>
     </row>
-    <row r="38" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A38" s="91"/>
       <c r="B38" s="91"/>
       <c r="C38" s="103"/>
@@ -4387,7 +4387,7 @@
       <c r="AB38" s="69"/>
       <c r="AC38" s="70"/>
     </row>
-    <row r="39" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A39" s="104"/>
       <c r="B39" s="91"/>
       <c r="C39" s="103"/>
@@ -4418,7 +4418,7 @@
       <c r="AB39" s="69"/>
       <c r="AC39" s="70"/>
     </row>
-    <row r="40" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A40" s="104"/>
       <c r="B40" s="91"/>
       <c r="C40" s="103"/>
@@ -4449,7 +4449,7 @@
       <c r="AB40" s="69"/>
       <c r="AC40" s="70"/>
     </row>
-    <row r="41" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A41" s="104"/>
       <c r="B41" s="91"/>
       <c r="C41" s="103"/>
@@ -4480,7 +4480,7 @@
       <c r="AB41" s="69"/>
       <c r="AC41" s="70"/>
     </row>
-    <row r="42" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A42" s="104"/>
       <c r="B42" s="91"/>
       <c r="C42" s="103"/>
@@ -4511,7 +4511,7 @@
       <c r="AB42" s="69"/>
       <c r="AC42" s="70"/>
     </row>
-    <row r="43" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A43" s="104"/>
       <c r="B43" s="91"/>
       <c r="C43" s="103"/>
@@ -4542,7 +4542,7 @@
       <c r="AB43" s="69"/>
       <c r="AC43" s="70"/>
     </row>
-    <row r="44" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="105"/>
       <c r="B44" s="94"/>
       <c r="C44" s="106"/>
@@ -4597,28 +4597,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D1FDC4A-298A-4ACF-A50A-BBA01C5BF255}">
   <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.44140625" customWidth="1"/>
-    <col min="2" max="2" width="48.33203125" customWidth="1"/>
-    <col min="3" max="3" width="10.5546875" customWidth="1"/>
+    <col min="1" max="1" width="24.42578125" customWidth="1"/>
+    <col min="2" max="2" width="48.28515625" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" customWidth="1"/>
     <col min="4" max="4" width="32" customWidth="1"/>
-    <col min="5" max="5" width="10.5546875" customWidth="1"/>
-    <col min="6" max="6" width="38.5546875" customWidth="1"/>
-    <col min="7" max="7" width="48.33203125" customWidth="1"/>
-    <col min="8" max="8" width="12.33203125" customWidth="1"/>
-    <col min="9" max="10" width="14.88671875" customWidth="1"/>
-    <col min="11" max="11" width="24.6640625" customWidth="1"/>
-    <col min="12" max="12" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" customWidth="1"/>
+    <col min="6" max="6" width="38.5703125" customWidth="1"/>
+    <col min="7" max="7" width="48.28515625" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" customWidth="1"/>
+    <col min="9" max="10" width="14.85546875" customWidth="1"/>
+    <col min="11" max="11" width="24.7109375" customWidth="1"/>
+    <col min="12" max="12" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="14" max="16" width="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>330</v>
       </c>
@@ -4659,7 +4659,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>333</v>
       </c>
@@ -4682,7 +4682,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>334</v>
       </c>
@@ -4701,7 +4701,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>335</v>
       </c>
@@ -4714,7 +4714,7 @@
       <c r="F4" s="39"/>
       <c r="G4" s="39"/>
     </row>
-    <row r="5" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>336</v>
       </c>
@@ -4727,7 +4727,7 @@
       <c r="F5" s="39"/>
       <c r="G5" s="39"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B6" s="39"/>
       <c r="C6" s="39"/>
       <c r="D6" s="39"/>
@@ -4735,7 +4735,7 @@
       <c r="F6" s="39"/>
       <c r="G6" s="39"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B7" s="39"/>
       <c r="C7" s="39"/>
       <c r="D7" s="39"/>
@@ -4743,7 +4743,7 @@
       <c r="F7" s="39"/>
       <c r="G7" s="39"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B8" s="39"/>
       <c r="C8" s="39"/>
       <c r="D8" s="39"/>
@@ -4751,7 +4751,7 @@
       <c r="F8" s="39"/>
       <c r="G8" s="39"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B9" s="39"/>
       <c r="C9" s="39"/>
       <c r="D9" s="39"/>
@@ -4759,7 +4759,7 @@
       <c r="F9" s="39"/>
       <c r="G9" s="39"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B10" s="39"/>
       <c r="C10" s="39"/>
       <c r="D10" s="39"/>
@@ -4767,7 +4767,7 @@
       <c r="F10" s="39"/>
       <c r="G10" s="39"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B11" s="39"/>
       <c r="C11" s="39"/>
       <c r="D11" s="39"/>
@@ -4775,7 +4775,7 @@
       <c r="F11" s="39"/>
       <c r="G11" s="39"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B12" s="39"/>
       <c r="C12" s="39"/>
       <c r="D12" s="39"/>
@@ -4783,7 +4783,7 @@
       <c r="F12" s="39"/>
       <c r="G12" s="39"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B13" s="39"/>
       <c r="C13" s="39"/>
       <c r="D13" s="39"/>
@@ -4801,19 +4801,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{062A0465-36AA-48A3-BB7A-61F0737D9C02}">
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="3" width="34.6640625" customWidth="1"/>
-    <col min="4" max="5" width="73.88671875" customWidth="1"/>
-    <col min="6" max="6" width="41.88671875" customWidth="1"/>
+    <col min="2" max="3" width="34.7109375" customWidth="1"/>
+    <col min="4" max="5" width="73.85546875" customWidth="1"/>
+    <col min="6" max="6" width="41.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="149" t="s">
         <v>306</v>
       </c>
@@ -4833,7 +4833,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="147">
         <v>1</v>
       </c>
@@ -4849,7 +4849,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="147">
         <v>2.1</v>
       </c>
@@ -4865,7 +4865,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="147">
         <v>2.2000000000000002</v>
       </c>
@@ -4881,7 +4881,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="147">
         <v>3</v>
       </c>
@@ -4894,7 +4894,7 @@
       </c>
       <c r="E5" s="150"/>
     </row>
-    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="147">
         <v>4</v>
       </c>
@@ -4907,217 +4907,217 @@
       </c>
       <c r="E6" s="150"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="147"/>
       <c r="B7" s="147"/>
       <c r="C7" s="147"/>
       <c r="D7" s="150"/>
       <c r="E7" s="150"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="147"/>
       <c r="B8" s="147"/>
       <c r="C8" s="147"/>
       <c r="D8" s="150"/>
       <c r="E8" s="150"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="147"/>
       <c r="B9" s="147"/>
       <c r="C9" s="147"/>
       <c r="D9" s="150"/>
       <c r="E9" s="150"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="147"/>
       <c r="B10" s="147"/>
       <c r="C10" s="147"/>
       <c r="D10" s="150"/>
       <c r="E10" s="150"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="147"/>
       <c r="B11" s="147"/>
       <c r="C11" s="147"/>
       <c r="D11" s="150"/>
       <c r="E11" s="150"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="147"/>
       <c r="B12" s="147"/>
       <c r="C12" s="147"/>
       <c r="D12" s="150"/>
       <c r="E12" s="150"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="147"/>
       <c r="B13" s="147"/>
       <c r="C13" s="147"/>
       <c r="D13" s="150"/>
       <c r="E13" s="150"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="147"/>
       <c r="B14" s="147"/>
       <c r="C14" s="147"/>
       <c r="D14" s="150"/>
       <c r="E14" s="150"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="147"/>
       <c r="B15" s="147"/>
       <c r="C15" s="147"/>
       <c r="D15" s="150"/>
       <c r="E15" s="150"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="147"/>
       <c r="B16" s="147"/>
       <c r="C16" s="147"/>
       <c r="D16" s="150"/>
       <c r="E16" s="150"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="147"/>
       <c r="B17" s="147"/>
       <c r="C17" s="147"/>
       <c r="D17" s="150"/>
       <c r="E17" s="150"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="147"/>
       <c r="B18" s="147"/>
       <c r="C18" s="147"/>
       <c r="D18" s="150"/>
       <c r="E18" s="150"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="147"/>
       <c r="B19" s="147"/>
       <c r="C19" s="147"/>
       <c r="D19" s="150"/>
       <c r="E19" s="150"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="147"/>
       <c r="B20" s="147"/>
       <c r="C20" s="147"/>
       <c r="D20" s="150"/>
       <c r="E20" s="150"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="147"/>
       <c r="B21" s="147"/>
       <c r="C21" s="147"/>
       <c r="D21" s="150"/>
       <c r="E21" s="150"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="147"/>
       <c r="B22" s="147"/>
       <c r="C22" s="147"/>
       <c r="D22" s="150"/>
       <c r="E22" s="150"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="147"/>
       <c r="B23" s="147"/>
       <c r="C23" s="147"/>
       <c r="D23" s="150"/>
       <c r="E23" s="150"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="147"/>
       <c r="B24" s="147"/>
       <c r="C24" s="147"/>
       <c r="D24" s="150"/>
       <c r="E24" s="150"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D25" s="39"/>
       <c r="E25" s="39"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D26" s="39"/>
       <c r="E26" s="39"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D27" s="39"/>
       <c r="E27" s="39"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D28" s="39"/>
       <c r="E28" s="39"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D29" s="39"/>
       <c r="E29" s="39"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D30" s="39"/>
       <c r="E30" s="39"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D31" s="39"/>
       <c r="E31" s="39"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D32" s="39"/>
       <c r="E32" s="39"/>
     </row>
-    <row r="33" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D33" s="39"/>
       <c r="E33" s="39"/>
     </row>
-    <row r="34" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D34" s="39"/>
       <c r="E34" s="39"/>
     </row>
-    <row r="35" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D35" s="39"/>
       <c r="E35" s="39"/>
     </row>
-    <row r="36" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D36" s="39"/>
       <c r="E36" s="39"/>
     </row>
-    <row r="37" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D37" s="39"/>
       <c r="E37" s="39"/>
     </row>
-    <row r="38" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D38" s="39"/>
       <c r="E38" s="39"/>
     </row>
-    <row r="39" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D39" s="39"/>
       <c r="E39" s="39"/>
     </row>
-    <row r="40" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D40" s="39"/>
       <c r="E40" s="39"/>
     </row>
-    <row r="41" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D41" s="39"/>
       <c r="E41" s="39"/>
     </row>
-    <row r="42" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D42" s="39"/>
       <c r="E42" s="39"/>
     </row>
-    <row r="43" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D43" s="39"/>
       <c r="E43" s="39"/>
     </row>
-    <row r="44" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D44" s="39"/>
       <c r="E44" s="39"/>
     </row>
-    <row r="45" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D45" s="39"/>
       <c r="E45" s="39"/>
     </row>
-    <row r="46" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D46" s="39"/>
       <c r="E46" s="39"/>
     </row>
@@ -5135,13 +5135,13 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="107.6640625" customWidth="1"/>
+    <col min="1" max="1" width="34.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="107.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>161</v>
       </c>
@@ -5149,7 +5149,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>280</v>
       </c>
@@ -5157,7 +5157,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>308</v>
       </c>
@@ -5165,16 +5165,16 @@
         <v>309</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" s="39"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" s="39"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" s="39"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" s="39"/>
     </row>
   </sheetData>
@@ -5191,32 +5191,32 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="59.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="59.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.109375" customWidth="1"/>
-    <col min="5" max="5" width="20.33203125" customWidth="1"/>
-    <col min="6" max="6" width="39.5546875" customWidth="1"/>
-    <col min="7" max="7" width="13.6640625" customWidth="1"/>
-    <col min="8" max="8" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.6640625" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" customWidth="1"/>
+    <col min="6" max="6" width="39.5703125" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" customWidth="1"/>
     <col min="11" max="11" width="51" customWidth="1"/>
-    <col min="12" max="12" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="16" width="31.5546875" customWidth="1"/>
-    <col min="17" max="20" width="19.5546875" customWidth="1"/>
-    <col min="21" max="22" width="25.33203125" customWidth="1"/>
+    <col min="12" max="12" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="16" width="31.5703125" customWidth="1"/>
+    <col min="17" max="20" width="19.5703125" customWidth="1"/>
+    <col min="21" max="22" width="25.28515625" customWidth="1"/>
     <col min="23" max="23" width="16" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="33.109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="33.140625" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="16" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="33.109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="33.140625" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="16" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="33.109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="33.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="99" t="s">
         <v>105</v>
       </c>
@@ -5302,7 +5302,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:28" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="90" t="s">
         <v>268</v>
       </c>
@@ -5350,7 +5350,7 @@
       <c r="AA2" s="67"/>
       <c r="AB2" s="68"/>
     </row>
-    <row r="3" spans="1:28" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="90" t="s">
         <v>274</v>
       </c>
@@ -5400,7 +5400,7 @@
       <c r="AA3" s="69"/>
       <c r="AB3" s="70"/>
     </row>
-    <row r="4" spans="1:28" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="91" t="s">
         <v>298</v>
       </c>
@@ -5448,7 +5448,7 @@
       <c r="AA4" s="69"/>
       <c r="AB4" s="70"/>
     </row>
-    <row r="5" spans="1:28" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="91" t="s">
         <v>299</v>
       </c>
@@ -5496,7 +5496,7 @@
       <c r="AA5" s="69"/>
       <c r="AB5" s="70"/>
     </row>
-    <row r="6" spans="1:28" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="91" t="s">
         <v>294</v>
       </c>
@@ -5544,7 +5544,7 @@
       <c r="AA6" s="69"/>
       <c r="AB6" s="70"/>
     </row>
-    <row r="7" spans="1:28" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:28" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="91" t="s">
         <v>296</v>
       </c>
@@ -5592,7 +5592,7 @@
       <c r="AA7" s="69"/>
       <c r="AB7" s="70"/>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" s="91"/>
       <c r="B8" s="91"/>
       <c r="C8" s="103"/>
@@ -5622,7 +5622,7 @@
       <c r="AA8" s="69"/>
       <c r="AB8" s="70"/>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9" s="91"/>
       <c r="B9" s="91"/>
       <c r="C9" s="103"/>
@@ -5652,7 +5652,7 @@
       <c r="AA9" s="69"/>
       <c r="AB9" s="70"/>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10" s="91"/>
       <c r="B10" s="91"/>
       <c r="C10" s="103"/>
@@ -5682,7 +5682,7 @@
       <c r="AA10" s="69"/>
       <c r="AB10" s="70"/>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" s="91"/>
       <c r="B11" s="91"/>
       <c r="C11" s="103"/>
@@ -5712,7 +5712,7 @@
       <c r="AA11" s="69"/>
       <c r="AB11" s="70"/>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12" s="91"/>
       <c r="B12" s="91"/>
       <c r="C12" s="103"/>
@@ -5742,7 +5742,7 @@
       <c r="AA12" s="69"/>
       <c r="AB12" s="70"/>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13" s="91"/>
       <c r="B13" s="91"/>
       <c r="C13" s="103"/>
@@ -5772,7 +5772,7 @@
       <c r="AA13" s="69"/>
       <c r="AB13" s="70"/>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14" s="91"/>
       <c r="B14" s="91"/>
       <c r="C14" s="103"/>
@@ -5802,7 +5802,7 @@
       <c r="AA14" s="69"/>
       <c r="AB14" s="70"/>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15" s="91"/>
       <c r="B15" s="91"/>
       <c r="C15" s="103"/>
@@ -5832,7 +5832,7 @@
       <c r="AA15" s="69"/>
       <c r="AB15" s="70"/>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16" s="91"/>
       <c r="B16" s="91"/>
       <c r="C16" s="103"/>
@@ -5862,7 +5862,7 @@
       <c r="AA16" s="69"/>
       <c r="AB16" s="70"/>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A17" s="91"/>
       <c r="B17" s="91"/>
       <c r="C17" s="103"/>
@@ -5892,7 +5892,7 @@
       <c r="AA17" s="69"/>
       <c r="AB17" s="70"/>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A18" s="91"/>
       <c r="B18" s="91"/>
       <c r="C18" s="103"/>
@@ -5922,7 +5922,7 @@
       <c r="AA18" s="69"/>
       <c r="AB18" s="70"/>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A19" s="91"/>
       <c r="B19" s="91"/>
       <c r="C19" s="103"/>
@@ -5952,7 +5952,7 @@
       <c r="AA19" s="69"/>
       <c r="AB19" s="70"/>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20" s="91"/>
       <c r="B20" s="91"/>
       <c r="C20" s="103"/>
@@ -5982,7 +5982,7 @@
       <c r="AA20" s="69"/>
       <c r="AB20" s="70"/>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A21" s="91"/>
       <c r="B21" s="91"/>
       <c r="C21" s="103"/>
@@ -6012,7 +6012,7 @@
       <c r="AA21" s="69"/>
       <c r="AB21" s="70"/>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A22" s="91"/>
       <c r="B22" s="91"/>
       <c r="C22" s="103"/>
@@ -6042,7 +6042,7 @@
       <c r="AA22" s="69"/>
       <c r="AB22" s="70"/>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A23" s="91"/>
       <c r="B23" s="91"/>
       <c r="C23" s="103"/>
@@ -6072,7 +6072,7 @@
       <c r="AA23" s="69"/>
       <c r="AB23" s="70"/>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A24" s="91"/>
       <c r="B24" s="91"/>
       <c r="C24" s="103"/>
@@ -6102,7 +6102,7 @@
       <c r="AA24" s="69"/>
       <c r="AB24" s="70"/>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A25" s="91"/>
       <c r="B25" s="91"/>
       <c r="C25" s="103"/>
@@ -6132,7 +6132,7 @@
       <c r="AA25" s="69"/>
       <c r="AB25" s="70"/>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A26" s="104"/>
       <c r="B26" s="91"/>
       <c r="C26" s="103"/>
@@ -6162,7 +6162,7 @@
       <c r="AA26" s="69"/>
       <c r="AB26" s="70"/>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A27" s="104"/>
       <c r="B27" s="91"/>
       <c r="C27" s="103"/>
@@ -6192,7 +6192,7 @@
       <c r="AA27" s="69"/>
       <c r="AB27" s="70"/>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A28" s="104"/>
       <c r="B28" s="91"/>
       <c r="C28" s="103"/>
@@ -6222,7 +6222,7 @@
       <c r="AA28" s="69"/>
       <c r="AB28" s="70"/>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A29" s="104"/>
       <c r="B29" s="91"/>
       <c r="C29" s="103"/>
@@ -6252,7 +6252,7 @@
       <c r="AA29" s="69"/>
       <c r="AB29" s="70"/>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A30" s="104"/>
       <c r="B30" s="91"/>
       <c r="C30" s="103"/>
@@ -6282,7 +6282,7 @@
       <c r="AA30" s="69"/>
       <c r="AB30" s="70"/>
     </row>
-    <row r="31" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="105"/>
       <c r="B31" s="94"/>
       <c r="C31" s="106"/>
@@ -6312,77 +6312,77 @@
       <c r="AA31" s="71"/>
       <c r="AB31" s="72"/>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
       <c r="K32" s="39"/>
       <c r="M32" s="39"/>
       <c r="N32" s="39"/>
       <c r="O32" s="39"/>
       <c r="P32" s="39"/>
     </row>
-    <row r="33" spans="11:16" x14ac:dyDescent="0.3">
+    <row r="33" spans="11:16" x14ac:dyDescent="0.25">
       <c r="K33" s="39"/>
       <c r="M33" s="39"/>
       <c r="N33" s="39"/>
       <c r="O33" s="39"/>
       <c r="P33" s="39"/>
     </row>
-    <row r="34" spans="11:16" x14ac:dyDescent="0.3">
+    <row r="34" spans="11:16" x14ac:dyDescent="0.25">
       <c r="K34" s="39"/>
       <c r="M34" s="39"/>
       <c r="N34" s="39"/>
       <c r="O34" s="39"/>
       <c r="P34" s="39"/>
     </row>
-    <row r="35" spans="11:16" x14ac:dyDescent="0.3">
+    <row r="35" spans="11:16" x14ac:dyDescent="0.25">
       <c r="K35" s="39"/>
       <c r="M35" s="39"/>
       <c r="N35" s="39"/>
       <c r="O35" s="39"/>
       <c r="P35" s="39"/>
     </row>
-    <row r="36" spans="11:16" x14ac:dyDescent="0.3">
+    <row r="36" spans="11:16" x14ac:dyDescent="0.25">
       <c r="K36" s="39"/>
       <c r="M36" s="39"/>
       <c r="N36" s="39"/>
       <c r="O36" s="39"/>
       <c r="P36" s="39"/>
     </row>
-    <row r="37" spans="11:16" x14ac:dyDescent="0.3">
+    <row r="37" spans="11:16" x14ac:dyDescent="0.25">
       <c r="K37" s="39"/>
       <c r="M37" s="39"/>
       <c r="N37" s="39"/>
       <c r="O37" s="39"/>
       <c r="P37" s="39"/>
     </row>
-    <row r="38" spans="11:16" x14ac:dyDescent="0.3">
+    <row r="38" spans="11:16" x14ac:dyDescent="0.25">
       <c r="K38" s="39"/>
       <c r="M38" s="39"/>
       <c r="N38" s="39"/>
       <c r="O38" s="39"/>
       <c r="P38" s="39"/>
     </row>
-    <row r="39" spans="11:16" x14ac:dyDescent="0.3">
+    <row r="39" spans="11:16" x14ac:dyDescent="0.25">
       <c r="K39" s="39"/>
       <c r="M39" s="39"/>
       <c r="N39" s="39"/>
       <c r="O39" s="39"/>
       <c r="P39" s="39"/>
     </row>
-    <row r="40" spans="11:16" x14ac:dyDescent="0.3">
+    <row r="40" spans="11:16" x14ac:dyDescent="0.25">
       <c r="K40" s="39"/>
       <c r="M40" s="39"/>
       <c r="N40" s="39"/>
       <c r="O40" s="39"/>
       <c r="P40" s="39"/>
     </row>
-    <row r="41" spans="11:16" x14ac:dyDescent="0.3">
+    <row r="41" spans="11:16" x14ac:dyDescent="0.25">
       <c r="K41" s="39"/>
       <c r="M41" s="39"/>
       <c r="N41" s="39"/>
       <c r="O41" s="39"/>
       <c r="P41" s="39"/>
     </row>
-    <row r="42" spans="11:16" x14ac:dyDescent="0.3">
+    <row r="42" spans="11:16" x14ac:dyDescent="0.25">
       <c r="K42" s="39"/>
       <c r="M42" s="39"/>
       <c r="N42" s="39"/>
@@ -6408,32 +6408,32 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="59.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="59.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" hidden="1" customWidth="1"/>
-    <col min="3" max="4" width="20.109375" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="20.33203125" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="39.5546875" customWidth="1"/>
-    <col min="7" max="7" width="39.5546875" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="13.6640625" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="12.33203125" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="16.5546875" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="16.6640625" hidden="1" customWidth="1"/>
+    <col min="3" max="4" width="20.140625" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="39.5703125" customWidth="1"/>
+    <col min="7" max="7" width="39.5703125" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="16.5703125" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="16.7109375" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="51" customWidth="1"/>
-    <col min="13" max="13" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="17" width="31.5546875" customWidth="1"/>
-    <col min="18" max="21" width="19.5546875" customWidth="1"/>
-    <col min="22" max="23" width="25.33203125" customWidth="1"/>
+    <col min="13" max="13" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="17" width="31.5703125" customWidth="1"/>
+    <col min="18" max="21" width="19.5703125" customWidth="1"/>
+    <col min="22" max="23" width="25.28515625" customWidth="1"/>
     <col min="24" max="24" width="16" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="33.109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="33.140625" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="16" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="33.109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="33.140625" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="16" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="33.109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="33.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="99" t="s">
         <v>105</v>
       </c>
@@ -6522,7 +6522,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:29" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="100" t="s">
         <v>213</v>
       </c>
@@ -6583,7 +6583,7 @@
       <c r="AB2" s="63"/>
       <c r="AC2" s="64"/>
     </row>
-    <row r="3" spans="1:29" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:29" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="103" t="s">
         <v>221</v>
       </c>
@@ -6644,7 +6644,7 @@
       <c r="AB3" s="65"/>
       <c r="AC3" s="66"/>
     </row>
-    <row r="4" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:29" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="103" t="s">
         <v>220</v>
       </c>
@@ -6705,7 +6705,7 @@
       <c r="AB4" s="65"/>
       <c r="AC4" s="66"/>
     </row>
-    <row r="5" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:29" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="91" t="s">
         <v>219</v>
       </c>
@@ -6766,7 +6766,7 @@
       <c r="AB5" s="65"/>
       <c r="AC5" s="66"/>
     </row>
-    <row r="6" spans="1:29" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:29" ht="150" x14ac:dyDescent="0.25">
       <c r="A6" s="91" t="s">
         <v>213</v>
       </c>
@@ -6829,7 +6829,7 @@
       <c r="AB6" s="65"/>
       <c r="AC6" s="66"/>
     </row>
-    <row r="7" spans="1:29" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:29" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="91" t="s">
         <v>242</v>
       </c>
@@ -6892,7 +6892,7 @@
       <c r="AB7" s="65"/>
       <c r="AC7" s="66"/>
     </row>
-    <row r="8" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:29" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="91" t="s">
         <v>221</v>
       </c>
@@ -6955,7 +6955,7 @@
       <c r="AB8" s="65"/>
       <c r="AC8" s="66"/>
     </row>
-    <row r="9" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:29" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="91" t="s">
         <v>213</v>
       </c>
@@ -7008,7 +7008,7 @@
       <c r="AB9" s="65"/>
       <c r="AC9" s="66"/>
     </row>
-    <row r="10" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:29" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="91" t="s">
         <v>242</v>
       </c>
@@ -7061,7 +7061,7 @@
       <c r="AB10" s="65"/>
       <c r="AC10" s="66"/>
     </row>
-    <row r="11" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:29" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="91" t="s">
         <v>221</v>
       </c>
@@ -7114,7 +7114,7 @@
       <c r="AB11" s="65"/>
       <c r="AC11" s="66"/>
     </row>
-    <row r="12" spans="1:29" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:29" ht="135" x14ac:dyDescent="0.25">
       <c r="A12" s="91" t="s">
         <v>260</v>
       </c>
@@ -7169,7 +7169,7 @@
       <c r="AB12" s="67"/>
       <c r="AC12" s="68"/>
     </row>
-    <row r="13" spans="1:29" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:29" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="90" t="s">
         <v>269</v>
       </c>
@@ -7222,7 +7222,7 @@
       <c r="AB13" s="67"/>
       <c r="AC13" s="68"/>
     </row>
-    <row r="14" spans="1:29" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:29" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="90" t="s">
         <v>270</v>
       </c>
@@ -7275,7 +7275,7 @@
       <c r="AB14" s="69"/>
       <c r="AC14" s="70"/>
     </row>
-    <row r="15" spans="1:29" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:29" ht="90" x14ac:dyDescent="0.25">
       <c r="A15" s="91" t="s">
         <v>271</v>
       </c>
@@ -7328,7 +7328,7 @@
       <c r="AB15" s="67"/>
       <c r="AC15" s="68"/>
     </row>
-    <row r="16" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:29" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="91" t="s">
         <v>275</v>
       </c>
@@ -7379,7 +7379,7 @@
       <c r="AB16" s="69"/>
       <c r="AC16" s="70"/>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A17" s="91"/>
       <c r="B17" s="91"/>
       <c r="C17" s="103"/>
@@ -7410,7 +7410,7 @@
       <c r="AB17" s="69"/>
       <c r="AC17" s="70"/>
     </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A18" s="91"/>
       <c r="B18" s="91"/>
       <c r="C18" s="103"/>
@@ -7441,7 +7441,7 @@
       <c r="AB18" s="69"/>
       <c r="AC18" s="70"/>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A19" s="91"/>
       <c r="B19" s="91"/>
       <c r="C19" s="103"/>
@@ -7472,7 +7472,7 @@
       <c r="AB19" s="69"/>
       <c r="AC19" s="70"/>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A20" s="91"/>
       <c r="B20" s="91"/>
       <c r="C20" s="103"/>
@@ -7503,7 +7503,7 @@
       <c r="AB20" s="69"/>
       <c r="AC20" s="70"/>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A21" s="91"/>
       <c r="B21" s="91"/>
       <c r="C21" s="103"/>
@@ -7534,7 +7534,7 @@
       <c r="AB21" s="69"/>
       <c r="AC21" s="70"/>
     </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A22" s="91"/>
       <c r="B22" s="91"/>
       <c r="C22" s="103"/>
@@ -7565,7 +7565,7 @@
       <c r="AB22" s="69"/>
       <c r="AC22" s="70"/>
     </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A23" s="91"/>
       <c r="B23" s="91"/>
       <c r="C23" s="103"/>
@@ -7596,7 +7596,7 @@
       <c r="AB23" s="69"/>
       <c r="AC23" s="70"/>
     </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A24" s="91"/>
       <c r="B24" s="91"/>
       <c r="C24" s="103"/>
@@ -7627,7 +7627,7 @@
       <c r="AB24" s="69"/>
       <c r="AC24" s="70"/>
     </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A25" s="91"/>
       <c r="B25" s="91"/>
       <c r="C25" s="103"/>
@@ -7658,7 +7658,7 @@
       <c r="AB25" s="69"/>
       <c r="AC25" s="70"/>
     </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A26" s="91"/>
       <c r="B26" s="91"/>
       <c r="C26" s="103"/>
@@ -7689,7 +7689,7 @@
       <c r="AB26" s="69"/>
       <c r="AC26" s="70"/>
     </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A27" s="91"/>
       <c r="B27" s="91"/>
       <c r="C27" s="103"/>
@@ -7720,7 +7720,7 @@
       <c r="AB27" s="69"/>
       <c r="AC27" s="70"/>
     </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A28" s="91"/>
       <c r="B28" s="91"/>
       <c r="C28" s="103"/>
@@ -7751,7 +7751,7 @@
       <c r="AB28" s="69"/>
       <c r="AC28" s="70"/>
     </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A29" s="91"/>
       <c r="B29" s="91"/>
       <c r="C29" s="103"/>
@@ -7782,7 +7782,7 @@
       <c r="AB29" s="69"/>
       <c r="AC29" s="70"/>
     </row>
-    <row r="30" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A30" s="91"/>
       <c r="B30" s="91"/>
       <c r="C30" s="103"/>
@@ -7813,7 +7813,7 @@
       <c r="AB30" s="69"/>
       <c r="AC30" s="70"/>
     </row>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A31" s="91"/>
       <c r="B31" s="91"/>
       <c r="C31" s="103"/>
@@ -7844,7 +7844,7 @@
       <c r="AB31" s="69"/>
       <c r="AC31" s="70"/>
     </row>
-    <row r="32" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A32" s="91"/>
       <c r="B32" s="91"/>
       <c r="C32" s="103"/>
@@ -7875,7 +7875,7 @@
       <c r="AB32" s="69"/>
       <c r="AC32" s="70"/>
     </row>
-    <row r="33" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A33" s="91"/>
       <c r="B33" s="91"/>
       <c r="C33" s="103"/>
@@ -7906,7 +7906,7 @@
       <c r="AB33" s="69"/>
       <c r="AC33" s="70"/>
     </row>
-    <row r="34" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A34" s="91"/>
       <c r="B34" s="91"/>
       <c r="C34" s="103"/>
@@ -7937,7 +7937,7 @@
       <c r="AB34" s="69"/>
       <c r="AC34" s="70"/>
     </row>
-    <row r="35" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A35" s="91"/>
       <c r="B35" s="91"/>
       <c r="C35" s="103"/>
@@ -7968,7 +7968,7 @@
       <c r="AB35" s="69"/>
       <c r="AC35" s="70"/>
     </row>
-    <row r="36" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A36" s="91"/>
       <c r="B36" s="91"/>
       <c r="C36" s="103"/>
@@ -7999,7 +7999,7 @@
       <c r="AB36" s="69"/>
       <c r="AC36" s="70"/>
     </row>
-    <row r="37" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A37" s="91"/>
       <c r="B37" s="91"/>
       <c r="C37" s="103"/>
@@ -8030,7 +8030,7 @@
       <c r="AB37" s="69"/>
       <c r="AC37" s="70"/>
     </row>
-    <row r="38" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A38" s="104"/>
       <c r="B38" s="91"/>
       <c r="C38" s="103"/>
@@ -8061,7 +8061,7 @@
       <c r="AB38" s="69"/>
       <c r="AC38" s="70"/>
     </row>
-    <row r="39" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A39" s="104"/>
       <c r="B39" s="91"/>
       <c r="C39" s="103"/>
@@ -8092,7 +8092,7 @@
       <c r="AB39" s="69"/>
       <c r="AC39" s="70"/>
     </row>
-    <row r="40" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A40" s="104"/>
       <c r="B40" s="91"/>
       <c r="C40" s="103"/>
@@ -8123,7 +8123,7 @@
       <c r="AB40" s="69"/>
       <c r="AC40" s="70"/>
     </row>
-    <row r="41" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A41" s="104"/>
       <c r="B41" s="91"/>
       <c r="C41" s="103"/>
@@ -8154,7 +8154,7 @@
       <c r="AB41" s="69"/>
       <c r="AC41" s="70"/>
     </row>
-    <row r="42" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A42" s="104"/>
       <c r="B42" s="91"/>
       <c r="C42" s="103"/>
@@ -8185,7 +8185,7 @@
       <c r="AB42" s="69"/>
       <c r="AC42" s="70"/>
     </row>
-    <row r="43" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="105"/>
       <c r="B43" s="94"/>
       <c r="C43" s="106"/>
@@ -8216,77 +8216,77 @@
       <c r="AB43" s="71"/>
       <c r="AC43" s="72"/>
     </row>
-    <row r="44" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:29" x14ac:dyDescent="0.25">
       <c r="L44" s="39"/>
       <c r="N44" s="39"/>
       <c r="O44" s="39"/>
       <c r="P44" s="39"/>
       <c r="Q44" s="39"/>
     </row>
-    <row r="45" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:29" x14ac:dyDescent="0.25">
       <c r="L45" s="39"/>
       <c r="N45" s="39"/>
       <c r="O45" s="39"/>
       <c r="P45" s="39"/>
       <c r="Q45" s="39"/>
     </row>
-    <row r="46" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:29" x14ac:dyDescent="0.25">
       <c r="L46" s="39"/>
       <c r="N46" s="39"/>
       <c r="O46" s="39"/>
       <c r="P46" s="39"/>
       <c r="Q46" s="39"/>
     </row>
-    <row r="47" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:29" x14ac:dyDescent="0.25">
       <c r="L47" s="39"/>
       <c r="N47" s="39"/>
       <c r="O47" s="39"/>
       <c r="P47" s="39"/>
       <c r="Q47" s="39"/>
     </row>
-    <row r="48" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:29" x14ac:dyDescent="0.25">
       <c r="L48" s="39"/>
       <c r="N48" s="39"/>
       <c r="O48" s="39"/>
       <c r="P48" s="39"/>
       <c r="Q48" s="39"/>
     </row>
-    <row r="49" spans="12:17" x14ac:dyDescent="0.3">
+    <row r="49" spans="12:17" x14ac:dyDescent="0.25">
       <c r="L49" s="39"/>
       <c r="N49" s="39"/>
       <c r="O49" s="39"/>
       <c r="P49" s="39"/>
       <c r="Q49" s="39"/>
     </row>
-    <row r="50" spans="12:17" x14ac:dyDescent="0.3">
+    <row r="50" spans="12:17" x14ac:dyDescent="0.25">
       <c r="L50" s="39"/>
       <c r="N50" s="39"/>
       <c r="O50" s="39"/>
       <c r="P50" s="39"/>
       <c r="Q50" s="39"/>
     </row>
-    <row r="51" spans="12:17" x14ac:dyDescent="0.3">
+    <row r="51" spans="12:17" x14ac:dyDescent="0.25">
       <c r="L51" s="39"/>
       <c r="N51" s="39"/>
       <c r="O51" s="39"/>
       <c r="P51" s="39"/>
       <c r="Q51" s="39"/>
     </row>
-    <row r="52" spans="12:17" x14ac:dyDescent="0.3">
+    <row r="52" spans="12:17" x14ac:dyDescent="0.25">
       <c r="L52" s="39"/>
       <c r="N52" s="39"/>
       <c r="O52" s="39"/>
       <c r="P52" s="39"/>
       <c r="Q52" s="39"/>
     </row>
-    <row r="53" spans="12:17" x14ac:dyDescent="0.3">
+    <row r="53" spans="12:17" x14ac:dyDescent="0.25">
       <c r="L53" s="39"/>
       <c r="N53" s="39"/>
       <c r="O53" s="39"/>
       <c r="P53" s="39"/>
       <c r="Q53" s="39"/>
     </row>
-    <row r="54" spans="12:17" x14ac:dyDescent="0.3">
+    <row r="54" spans="12:17" x14ac:dyDescent="0.25">
       <c r="L54" s="39"/>
       <c r="N54" s="39"/>
       <c r="O54" s="39"/>
@@ -8314,15 +8314,15 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.33203125" customWidth="1"/>
-    <col min="3" max="3" width="96.109375" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" customWidth="1"/>
+    <col min="3" max="3" width="96.140625" customWidth="1"/>
     <col min="4" max="4" width="45" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="99" t="s">
         <v>0</v>
       </c>
@@ -8339,7 +8339,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="102">
         <v>44578</v>
       </c>
@@ -8353,7 +8353,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="103">
         <v>44582</v>
       </c>
@@ -8370,241 +8370,241 @@
         <v>198</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="103"/>
       <c r="B4" s="120"/>
       <c r="C4" s="128"/>
       <c r="D4" s="40"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="103"/>
       <c r="B5" s="120"/>
       <c r="C5" s="128"/>
       <c r="D5" s="41"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="103"/>
       <c r="B6" s="120"/>
       <c r="C6" s="128"/>
       <c r="D6" s="41"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="103"/>
       <c r="B7" s="120"/>
       <c r="C7" s="128"/>
       <c r="D7" s="41"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="103"/>
       <c r="B8" s="120"/>
       <c r="C8" s="128"/>
       <c r="D8" s="41"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="103"/>
       <c r="B9" s="120"/>
       <c r="C9" s="128"/>
       <c r="D9" s="41"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="103"/>
       <c r="B10" s="120"/>
       <c r="C10" s="128"/>
       <c r="D10" s="41"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="103"/>
       <c r="B11" s="120"/>
       <c r="C11" s="128"/>
       <c r="D11" s="41"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="103"/>
       <c r="B12" s="120"/>
       <c r="C12" s="128"/>
       <c r="D12" s="42"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="103"/>
       <c r="B13" s="120"/>
       <c r="C13" s="128"/>
       <c r="D13" s="42"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="103"/>
       <c r="B14" s="120"/>
       <c r="C14" s="128"/>
       <c r="D14" s="42"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="103"/>
       <c r="B15" s="120"/>
       <c r="C15" s="128"/>
       <c r="D15" s="42"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="103"/>
       <c r="B16" s="120"/>
       <c r="C16" s="128"/>
       <c r="D16" s="42"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="103"/>
       <c r="B17" s="120"/>
       <c r="C17" s="128"/>
       <c r="D17" s="42"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="103"/>
       <c r="B18" s="120"/>
       <c r="C18" s="128"/>
       <c r="D18" s="42"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="103"/>
       <c r="B19" s="120"/>
       <c r="C19" s="128"/>
       <c r="D19" s="42"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="103"/>
       <c r="B20" s="120"/>
       <c r="C20" s="128"/>
       <c r="D20" s="42"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="103"/>
       <c r="B21" s="120"/>
       <c r="C21" s="128"/>
       <c r="D21" s="42"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="103"/>
       <c r="B22" s="120"/>
       <c r="C22" s="128"/>
       <c r="D22" s="42"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="103"/>
       <c r="B23" s="120"/>
       <c r="C23" s="128"/>
       <c r="D23" s="42"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="103"/>
       <c r="B24" s="120"/>
       <c r="C24" s="128"/>
       <c r="D24" s="42"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="103"/>
       <c r="B25" s="120"/>
       <c r="C25" s="128"/>
       <c r="D25" s="42"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="103"/>
       <c r="B26" s="120"/>
       <c r="C26" s="128"/>
       <c r="D26" s="42"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="103"/>
       <c r="B27" s="120"/>
       <c r="C27" s="128"/>
       <c r="D27" s="42"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="103"/>
       <c r="B28" s="120"/>
       <c r="C28" s="128"/>
       <c r="D28" s="42"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="103"/>
       <c r="B29" s="120"/>
       <c r="C29" s="128"/>
       <c r="D29" s="42"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="103"/>
       <c r="B30" s="120"/>
       <c r="C30" s="128"/>
       <c r="D30" s="42"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="103"/>
       <c r="B31" s="120"/>
       <c r="C31" s="128"/>
       <c r="D31" s="42"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="103"/>
       <c r="B32" s="120"/>
       <c r="C32" s="128"/>
       <c r="D32" s="42"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="103"/>
       <c r="B33" s="120"/>
       <c r="C33" s="128"/>
       <c r="D33" s="42"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="103"/>
       <c r="B34" s="120"/>
       <c r="C34" s="128"/>
       <c r="D34" s="42"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="103"/>
       <c r="B35" s="120"/>
       <c r="C35" s="128"/>
       <c r="D35" s="42"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="103"/>
       <c r="B36" s="120"/>
       <c r="C36" s="128"/>
       <c r="D36" s="42"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="103"/>
       <c r="B37" s="120"/>
       <c r="C37" s="128"/>
       <c r="D37" s="42"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="103"/>
       <c r="B38" s="120"/>
       <c r="C38" s="128"/>
       <c r="D38" s="42"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="103"/>
       <c r="B39" s="120"/>
       <c r="C39" s="128"/>
       <c r="D39" s="42"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="103"/>
       <c r="B40" s="120"/>
       <c r="C40" s="128"/>
       <c r="D40" s="42"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="103"/>
       <c r="B41" s="120"/>
       <c r="C41" s="128"/>
       <c r="D41" s="42"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="103"/>
       <c r="B42" s="120"/>
       <c r="C42" s="128"/>
       <c r="D42" s="42"/>
     </row>
-    <row r="43" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="106"/>
       <c r="B43" s="121"/>
       <c r="C43" s="129"/>
@@ -8626,20 +8626,20 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.5546875" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="77.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="118.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="53.6640625" customWidth="1"/>
-    <col min="8" max="8" width="39.6640625" customWidth="1"/>
-    <col min="9" max="9" width="49.6640625" customWidth="1"/>
+    <col min="1" max="1" width="19.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="77.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="118.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="53.7109375" customWidth="1"/>
+    <col min="8" max="8" width="39.7109375" customWidth="1"/>
+    <col min="9" max="9" width="49.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="26" t="s">
         <v>39</v>
       </c>
@@ -8668,7 +8668,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A2" s="27"/>
       <c r="B2" s="27"/>
       <c r="C2" s="18" t="s">
@@ -8691,7 +8691,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="27"/>
       <c r="B3" s="27"/>
       <c r="C3" s="19" t="s">
@@ -8714,7 +8714,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="27"/>
       <c r="B4" s="27"/>
       <c r="C4" s="19" t="s">
@@ -8735,7 +8735,7 @@
       </c>
       <c r="I4" s="11"/>
     </row>
-    <row r="5" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>38</v>
       </c>
@@ -8762,7 +8762,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>38</v>
       </c>
@@ -8787,7 +8787,7 @@
       <c r="H6" s="14"/>
       <c r="I6" s="15"/>
     </row>
-    <row r="7" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>38</v>
       </c>
@@ -8812,7 +8812,7 @@
       </c>
       <c r="I7" s="15"/>
     </row>
-    <row r="8" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>38</v>
       </c>
@@ -8841,7 +8841,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>40</v>
       </c>
@@ -8868,7 +8868,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>40</v>
       </c>
@@ -8891,7 +8891,7 @@
       <c r="H10" s="14"/>
       <c r="I10" s="15"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>40</v>
       </c>
@@ -8914,7 +8914,7 @@
       <c r="H11" s="14"/>
       <c r="I11" s="15"/>
     </row>
-    <row r="12" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="22" t="s">
         <v>38</v>
       </c>
@@ -8939,7 +8939,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="22"/>
       <c r="B13" s="29"/>
       <c r="C13" s="23"/>
@@ -8950,7 +8950,7 @@
       <c r="H13" s="14"/>
       <c r="I13" s="15"/>
     </row>
-    <row r="14" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
         <v>40</v>
       </c>
@@ -8975,7 +8975,7 @@
       <c r="H14" s="14"/>
       <c r="I14" s="15"/>
     </row>
-    <row r="15" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
         <v>40</v>
       </c>
@@ -9002,7 +9002,7 @@
       </c>
       <c r="I15" s="15"/>
     </row>
-    <row r="16" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
         <v>40</v>
       </c>
@@ -9029,7 +9029,7 @@
       </c>
       <c r="I16" s="15"/>
     </row>
-    <row r="17" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
         <v>40</v>
       </c>
@@ -9054,7 +9054,7 @@
       <c r="H17" s="14"/>
       <c r="I17" s="15"/>
     </row>
-    <row r="18" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
         <v>40</v>
       </c>
@@ -9081,7 +9081,7 @@
       </c>
       <c r="I18" s="38"/>
     </row>
-    <row r="19" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="31" t="s">
         <v>40</v>
       </c>
@@ -9108,7 +9108,7 @@
       </c>
       <c r="I19" s="38"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="31" t="s">
         <v>40</v>
       </c>
@@ -9131,7 +9131,7 @@
       <c r="H20" s="37"/>
       <c r="I20" s="38"/>
     </row>
-    <row r="21" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="31" t="s">
         <v>40</v>
       </c>
@@ -9156,7 +9156,7 @@
       </c>
       <c r="I21" s="38"/>
     </row>
-    <row r="22" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="31" t="s">
         <v>40</v>
       </c>
@@ -9179,7 +9179,7 @@
       <c r="H22" s="37"/>
       <c r="I22" s="38"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="31"/>
       <c r="B23" s="32"/>
       <c r="C23" s="33"/>
@@ -9190,7 +9190,7 @@
       <c r="H23" s="37"/>
       <c r="I23" s="38"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="31"/>
       <c r="B24" s="32"/>
       <c r="C24" s="33"/>
@@ -9201,7 +9201,7 @@
       <c r="H24" s="37"/>
       <c r="I24" s="38"/>
     </row>
-    <row r="25" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="24"/>
       <c r="B25" s="30"/>
       <c r="C25" s="25"/>
@@ -9226,14 +9226,14 @@
       <selection activeCell="A2" sqref="A2:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="105.88671875" customWidth="1"/>
-    <col min="2" max="2" width="28.88671875" customWidth="1"/>
+    <col min="1" max="1" width="105.85546875" customWidth="1"/>
+    <col min="2" max="2" width="28.85546875" customWidth="1"/>
     <col min="3" max="3" width="48" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -9244,7 +9244,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="39" t="s">
         <v>93</v>
       </c>
@@ -9255,7 +9255,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>62</v>
       </c>
@@ -9263,7 +9263,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>64</v>
       </c>
@@ -9271,7 +9271,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>86</v>
       </c>
@@ -9279,19 +9279,19 @@
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C6" s="39"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C7" s="39"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C8" s="39"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C9" s="39"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C10" s="39"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update simulations and sample proportions of the population, rather than absolute numbers.
Also archive old scripts
</commit_message>
<xml_diff>
--- a/Simulation_log_key.xlsx
+++ b/Simulation_log_key.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\Documents\R\working_directory\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\Documents\R\working_directory\LemonSharkCKMR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91E399B0-55D8-4647-AD40-9F0C9BAD6A7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{141BAA86-8F8C-4F20-BB8D-998B4FD21EDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5085" yWindow="-11640" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="1" xr2:uid="{24E2991C-2C0C-4843-9426-0DC9EB9B25FD}"/>
+    <workbookView xWindow="5085" yWindow="-11640" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="3" xr2:uid="{24E2991C-2C0C-4843-9426-0DC9EB9B25FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Bayesian_model_validation" sheetId="3" state="hidden" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="350">
   <si>
     <t>Date run</t>
   </si>
@@ -1307,6 +1307,15 @@
   </si>
   <si>
     <t>1D</t>
+  </si>
+  <si>
+    <t>skipped-breeding was in the simulation</t>
+  </si>
+  <si>
+    <t>AB</t>
+  </si>
+  <si>
+    <t>annual breeding</t>
   </si>
 </sst>
 </file>
@@ -4597,7 +4606,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D1FDC4A-298A-4ACF-A50A-BBA01C5BF255}">
   <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -5131,8 +5140,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C0E03EF-3489-4384-AA19-0C78DA3254C7}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5166,10 +5175,20 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B4" s="39"/>
+      <c r="A4" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" s="39" t="s">
+        <v>347</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B5" s="39"/>
+      <c r="A5" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="B5" s="39" t="s">
+        <v>349</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B6" s="39"/>

</xml_diff>

<commit_message>
Update Objective 1 and 2 scripts
</commit_message>
<xml_diff>
--- a/Simulation_log_key.xlsx
+++ b/Simulation_log_key.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zeus\Documents\R\working_directory\LemonSharkCKMR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\Documents\R\working_directory\LemonSharkCKMR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{2AD4F4A9-8495-4142-9181-D56F1B1E47AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FDDDFFD-C43E-4739-82DB-6E06BE1D5A12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="5085" yWindow="-11640" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Simulation_log_key" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="44">
   <si>
     <t>Objective</t>
   </si>
@@ -79,9 +79,6 @@
     <t>Lambda in PopSim; not in model</t>
   </si>
   <si>
-    <t>Obj2.2</t>
-  </si>
-  <si>
     <t>all three</t>
   </si>
   <si>
@@ -137,12 +134,30 @@
   </si>
   <si>
     <t>Can try estimating abundance in three different years: 1 year in the past, 5 years, 10 years.</t>
+  </si>
+  <si>
+    <t>Obj2.2.1</t>
+  </si>
+  <si>
+    <t>Obj2.2.2</t>
+  </si>
+  <si>
+    <t>iteratively fixed</t>
+  </si>
+  <si>
+    <t>Obj1.2</t>
+  </si>
+  <si>
+    <t>Initial model validation w/ uninformed priors</t>
+  </si>
+  <si>
+    <t>beta w/ 10% CV</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -979,26 +994,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="44.5703125" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="43.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="72.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.5546875" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="43.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="72.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1021,13 +1036,13 @@
         <v>5</v>
       </c>
       <c r="H1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1035,7 +1050,7 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1047,53 +1062,53 @@
         <v>17</v>
       </c>
       <c r="G2" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="H2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
-      <c r="E3" t="s">
-        <v>9</v>
+      <c r="E3">
+        <v>1</v>
       </c>
       <c r="F3" t="s">
         <v>17</v>
       </c>
       <c r="G3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
         <v>19</v>
-      </c>
-      <c r="B4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" t="s">
-        <v>20</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -1102,24 +1117,27 @@
         <v>9</v>
       </c>
       <c r="F4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" t="s">
         <v>21</v>
       </c>
-      <c r="G4" t="s">
-        <v>22</v>
-      </c>
       <c r="H4" t="s">
-        <v>32</v>
+        <v>30</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -1128,96 +1146,148 @@
         <v>9</v>
       </c>
       <c r="F5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" t="s">
         <v>21</v>
       </c>
-      <c r="G5" t="s">
-        <v>22</v>
-      </c>
       <c r="H5" t="s">
-        <v>32</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="B6" t="s">
         <v>24</v>
       </c>
       <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" t="s">
         <v>20</v>
       </c>
-      <c r="D6">
+      <c r="G7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8">
         <v>2</v>
       </c>
-      <c r="E6">
+      <c r="E8">
         <v>1</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" t="s">
         <v>21</v>
       </c>
-      <c r="G6" t="s">
-        <v>22</v>
-      </c>
-      <c r="H6" t="s">
+      <c r="H8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H9" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" t="s">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>27</v>
       </c>
-      <c r="C7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7">
-        <v>2</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" t="s">
-        <v>22</v>
-      </c>
-      <c r="H7" t="s">
-        <v>33</v>
+      <c r="B10" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" t="s">
-        <v>29</v>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>11</v>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>12</v>
-      </c>
-      <c r="B22" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>14</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B25" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update simulation and model log, and objective 2
</commit_message>
<xml_diff>
--- a/Simulation_log_key.xlsx
+++ b/Simulation_log_key.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zeus\Documents\R\working_directory\LemonSharkCKMR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{122226A2-D73B-4434-AF25-C2681FDF9B8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E79C9A2-F18B-4B81-BE2B-ED0BDADEBD46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="48">
   <si>
     <t>Objective</t>
   </si>
@@ -127,9 +127,6 @@
     <t>Will need to comment on the "true" value. It'll be the mean over the cohort years, but how well does this reflect the abundance in a given year?</t>
   </si>
   <si>
-    <t>Obj2.3?</t>
-  </si>
-  <si>
     <t>Lambda in PopSim; lambda in model; vary year of abundance estimation? Try 10, 5, 1 year in the past?</t>
   </si>
   <si>
@@ -155,6 +152,18 @@
   </si>
   <si>
     <t>Pin this for later. I could try estimating abundance in three different years relative to the present: 1 year in the past, 5 years (current), and 10 years. This could show if there are any differences in model performance based on the year of estimation.</t>
+  </si>
+  <si>
+    <t>Obj2.2.3</t>
+  </si>
+  <si>
+    <t>Obj2.4?</t>
+  </si>
+  <si>
+    <t>variable; stable</t>
+  </si>
+  <si>
+    <t>Change the year of estimation to make it further and closer</t>
   </si>
 </sst>
 </file>
@@ -1008,10 +1017,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1075,7 +1084,7 @@
         <v>17</v>
       </c>
       <c r="G2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H2" t="s">
         <v>30</v>
@@ -1086,10 +1095,10 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" t="s">
         <v>40</v>
-      </c>
-      <c r="B3" t="s">
-        <v>41</v>
       </c>
       <c r="C3" t="s">
         <v>19</v>
@@ -1144,7 +1153,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B5" t="s">
         <v>24</v>
@@ -1156,7 +1165,7 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>9</v>
+        <v>46</v>
       </c>
       <c r="F5" t="s">
         <v>20</v>
@@ -1168,41 +1177,41 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B6" s="2" t="s">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6">
         <v>1</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="G6" s="2" t="s">
+      <c r="F6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" t="s">
         <v>21</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H6" t="s">
         <v>31</v>
       </c>
-      <c r="I6" s="3" t="s">
-        <v>43</v>
+      <c r="I6" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>36</v>
+        <v>44</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>19</v>
@@ -1214,7 +1223,7 @@
         <v>9</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>21</v>
@@ -1223,41 +1232,44 @@
         <v>31</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" t="s">
+    <row r="8" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D8">
-        <v>2</v>
-      </c>
-      <c r="E8">
+      <c r="D8" s="2">
         <v>1</v>
       </c>
-      <c r="F8" t="s">
+      <c r="E8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="2" t="s">
         <v>31</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s">
         <v>19</v>
@@ -1275,35 +1287,61 @@
         <v>21</v>
       </c>
       <c r="H9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>27</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>12</v>
-      </c>
-      <c r="B24" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>14</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B26" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update data viz and analysis file
</commit_message>
<xml_diff>
--- a/Simulation_log_key.xlsx
+++ b/Simulation_log_key.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zeus\Documents\R\working_directory\LemonSharkCKMR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E79C9A2-F18B-4B81-BE2B-ED0BDADEBD46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5D810C7-2077-4D7E-8E7A-53862A969762}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1019,8 +1019,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1191,7 +1191,7 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>9</v>
+        <v>46</v>
       </c>
       <c r="F6" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
Lots of Data viz updates
</commit_message>
<xml_diff>
--- a/Simulation_log_key.xlsx
+++ b/Simulation_log_key.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zeus\Documents\R\working_directory\LemonSharkCKMR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\Documents\R\working_directory\LemonSharkCKMR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5D810C7-2077-4D7E-8E7A-53862A969762}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFB6AF96-E211-4A5E-A582-184EAE071A9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5085" yWindow="-11640" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Simulation_log_key" sheetId="1" r:id="rId1"/>
+    <sheet name="Objective_key" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="67">
   <si>
     <t>Objective</t>
   </si>
@@ -43,18 +44,12 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>Obj1.1</t>
-  </si>
-  <si>
     <t>Initial model validation w/ informed priors</t>
   </si>
   <si>
     <t>variable</t>
   </si>
   <si>
-    <t>Obj2.1</t>
-  </si>
-  <si>
     <t>Potential supplemental simulations</t>
   </si>
   <si>
@@ -88,24 +83,15 @@
     <t>Uniform 0.5-0.95</t>
   </si>
   <si>
-    <t>Obj3.1</t>
-  </si>
-  <si>
     <t>Skipped-breeding (SB) in PopSim; not in model</t>
   </si>
   <si>
     <t>Lambda in PopSim; lambda in model</t>
   </si>
   <si>
-    <t>Obj3.2</t>
-  </si>
-  <si>
     <t>SB in PopSim; SB in model</t>
   </si>
   <si>
-    <t>Obj4.1</t>
-  </si>
-  <si>
     <t>Aging error</t>
   </si>
   <si>
@@ -127,21 +113,9 @@
     <t>Will need to comment on the "true" value. It'll be the mean over the cohort years, but how well does this reflect the abundance in a given year?</t>
   </si>
   <si>
-    <t>Lambda in PopSim; lambda in model; vary year of abundance estimation? Try 10, 5, 1 year in the past?</t>
-  </si>
-  <si>
-    <t>Obj2.2.1</t>
-  </si>
-  <si>
-    <t>Obj2.2.2</t>
-  </si>
-  <si>
     <t>iteratively fixed</t>
   </si>
   <si>
-    <t>Obj1.2</t>
-  </si>
-  <si>
     <t>Initial model validation w/ uninformed priors</t>
   </si>
   <si>
@@ -151,19 +125,103 @@
     <t>I can run this later if we want … but for now I'm gonna proceed linearly and skip this step, since it is a little time intensive and I want to get the major results first.</t>
   </si>
   <si>
-    <t>Pin this for later. I could try estimating abundance in three different years relative to the present: 1 year in the past, 5 years (current), and 10 years. This could show if there are any differences in model performance based on the year of estimation.</t>
-  </si>
-  <si>
-    <t>Obj2.2.3</t>
-  </si>
-  <si>
-    <t>Obj2.4?</t>
-  </si>
-  <si>
     <t>variable; stable</t>
   </si>
   <si>
     <t>Change the year of estimation to make it further and closer</t>
+  </si>
+  <si>
+    <t>scenario</t>
+  </si>
+  <si>
+    <t>scenario_1.1</t>
+  </si>
+  <si>
+    <t>scenario_1.2</t>
+  </si>
+  <si>
+    <t>scenario_2.1</t>
+  </si>
+  <si>
+    <t>scenario_2.2.1</t>
+  </si>
+  <si>
+    <t>scenario_2.2.2</t>
+  </si>
+  <si>
+    <t>scenario_2.2.3</t>
+  </si>
+  <si>
+    <t>scenario_3.1</t>
+  </si>
+  <si>
+    <t>scenario_3.2</t>
+  </si>
+  <si>
+    <t>scenario_4.1</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Scenario 1</t>
+  </si>
+  <si>
+    <t>Scenario 2</t>
+  </si>
+  <si>
+    <t>Scenario 3</t>
+  </si>
+  <si>
+    <t>Validate model with informed and diffuse prior for survival</t>
+  </si>
+  <si>
+    <t>obj1</t>
+  </si>
+  <si>
+    <t>obj2.1</t>
+  </si>
+  <si>
+    <t>Compare naïve model vs lambda model w/ population growth and a range of estimation years</t>
+  </si>
+  <si>
+    <t>model validation; informed prior on survival</t>
+  </si>
+  <si>
+    <t>model validation; diffuse prior on survival</t>
+  </si>
+  <si>
+    <t>Scenario 1 relevance</t>
+  </si>
+  <si>
+    <t>Scenario 2 relevance</t>
+  </si>
+  <si>
+    <t>Scenario 3 relevance</t>
+  </si>
+  <si>
+    <t>neutral population growth; no prior on lambda</t>
+  </si>
+  <si>
+    <t>variable population growth; no lambda</t>
+  </si>
+  <si>
+    <t>Scenario 4</t>
+  </si>
+  <si>
+    <t>Scenario 4 relevance</t>
+  </si>
+  <si>
+    <t>scenario2.2.1</t>
+  </si>
+  <si>
+    <t>scenario _2.2.2</t>
+  </si>
+  <si>
+    <t>neutral + variable population growth; lambda prior; estimate year 85</t>
+  </si>
+  <si>
+    <t>neutral + variable population growth; lambda prior; estimate years 80 and 90</t>
   </si>
 </sst>
 </file>
@@ -1017,332 +1075,418 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:I25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.5546875" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="43.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="72.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="2">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" t="s">
+        <v>19</v>
+      </c>
+      <c r="H9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{412D6C35-5CAD-470C-B537-E441B956C3CF}">
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="44.5703125" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="43.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="72.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.77734375" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.44140625" customWidth="1"/>
+    <col min="7" max="7" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.109375" customWidth="1"/>
+    <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="34.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>46</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>47</v>
       </c>
       <c r="D1" t="s">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>48</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>57</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>49</v>
       </c>
       <c r="H1" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
       <c r="I1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="J1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>50</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
+        <v>37</v>
+      </c>
+      <c r="D2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" t="s">
+        <v>38</v>
       </c>
       <c r="F2" t="s">
-        <v>17</v>
+        <v>55</v>
       </c>
       <c r="G2" t="s">
-        <v>41</v>
-      </c>
-      <c r="H2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E3" t="s">
         <v>39</v>
       </c>
-      <c r="B3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
       <c r="F3" t="s">
-        <v>17</v>
+        <v>60</v>
       </c>
       <c r="G3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" t="s">
-        <v>30</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" t="s">
-        <v>21</v>
-      </c>
-      <c r="H4" t="s">
-        <v>30</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5" t="s">
-        <v>46</v>
-      </c>
-      <c r="F5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" t="s">
-        <v>21</v>
-      </c>
-      <c r="H5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6" t="s">
-        <v>46</v>
-      </c>
-      <c r="F6" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" t="s">
-        <v>21</v>
-      </c>
-      <c r="H6" t="s">
-        <v>31</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="2">
-        <v>1</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="2">
-        <v>1</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9">
-        <v>2</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G9" t="s">
-        <v>21</v>
-      </c>
-      <c r="H9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10">
-        <v>2</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10" t="s">
-        <v>20</v>
-      </c>
-      <c r="G10" t="s">
-        <v>21</v>
-      </c>
-      <c r="H10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>12</v>
-      </c>
-      <c r="B25" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>14</v>
-      </c>
-      <c r="B26" t="s">
-        <v>15</v>
+        <v>63</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="I3" t="s">
+        <v>64</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Lots and lots of updates
</commit_message>
<xml_diff>
--- a/Simulation_log_key.xlsx
+++ b/Simulation_log_key.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\Documents\R\working_directory\LemonSharkCKMR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFB6AF96-E211-4A5E-A582-184EAE071A9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79D1D6F4-B945-4001-AD84-C165F1AE8570}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5085" yWindow="-11640" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5085" yWindow="-11640" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Simulation_log_key" sheetId="1" r:id="rId1"/>
-    <sheet name="Objective_key" sheetId="2" r:id="rId2"/>
+    <sheet name="Simulation_log_old_7.24.22" sheetId="3" r:id="rId2"/>
+    <sheet name="Objective_key" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="78">
   <si>
     <t>Objective</t>
   </si>
@@ -222,6 +223,39 @@
   </si>
   <si>
     <t>neutral + variable population growth; lambda prior; estimate years 80 and 90</t>
+  </si>
+  <si>
+    <t>small variations</t>
+  </si>
+  <si>
+    <t>bigger variations</t>
+  </si>
+  <si>
+    <t>scenario_3.1.1</t>
+  </si>
+  <si>
+    <t>Skipped-breeding (SB) in PopSim; not in model; no lambda in model</t>
+  </si>
+  <si>
+    <t>Skipped-breeding (SB) in PopSim; not in model; lambda in model</t>
+  </si>
+  <si>
+    <t>scenario_3.1.2</t>
+  </si>
+  <si>
+    <t>scenario_3.2.1</t>
+  </si>
+  <si>
+    <t>scenario_3.2.2</t>
+  </si>
+  <si>
+    <t>SB in PopSim; SB in model; lambda in model</t>
+  </si>
+  <si>
+    <t>SB in PopSim; SB in model; no lambda in model</t>
+  </si>
+  <si>
+    <t>Liz's derivation (minus lambda)</t>
   </si>
 </sst>
 </file>
@@ -1075,10 +1109,343 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="56.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="43.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="72.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>68</v>
+      </c>
+      <c r="F6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>73</v>
+      </c>
+      <c r="B9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" t="s">
+        <v>19</v>
+      </c>
+      <c r="H9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>74</v>
+      </c>
+      <c r="B10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" t="s">
+        <v>19</v>
+      </c>
+      <c r="H10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB1D795D-554E-4B31-8732-D7CC78219987}">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1380,11 +1747,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{412D6C35-5CAD-470C-B537-E441B956C3CF}">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -1457,7 +1824,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>52</v>
       </c>

</xml_diff>

<commit_message>
Update simulation log and add population simulations for refined juvenile sampling, and model simulations for psi=1, a=2 and lambda prior of 0.8 - 1.2.
</commit_message>
<xml_diff>
--- a/Simulation_log_key.xlsx
+++ b/Simulation_log_key.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\Documents\R\working_directory\LemonSharkCKMR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zeus\Documents\R\working_directory\LemonSharkCKMR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6767413-DA5B-40F6-B03C-32FAA57F0061}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8749CD5-9C3F-45D9-8ADB-3D6F3AEE4085}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5085" yWindow="-11640" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-15480" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Simulation_log_key" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="83">
   <si>
     <t>Objective</t>
   </si>
@@ -262,6 +262,15 @@
   </si>
   <si>
     <t>scenario_2.1.2</t>
+  </si>
+  <si>
+    <t>scenario_3.3.1</t>
+  </si>
+  <si>
+    <t>scenario_3.3.2</t>
+  </si>
+  <si>
+    <t>Non-conformists</t>
   </si>
 </sst>
 </file>
@@ -751,7 +760,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -760,6 +769,7 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1115,26 +1125,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="56.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5546875" customWidth="1"/>
-    <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="72.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.5703125" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="16.5703125" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="72.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>36</v>
       </c>
@@ -1148,22 +1158,25 @@
         <v>14</v>
       </c>
       <c r="E1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>24</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -1177,22 +1190,25 @@
         <v>1</v>
       </c>
       <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
         <v>15</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>32</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>25</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -1206,22 +1222,25 @@
         <v>1</v>
       </c>
       <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
         <v>15</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>19</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>78</v>
       </c>
@@ -1234,23 +1253,26 @@
       <c r="D4">
         <v>1</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4" t="s">
         <v>67</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>15</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>19</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>25</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>79</v>
       </c>
@@ -1263,23 +1285,26 @@
       <c r="D5">
         <v>1</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5" t="s">
         <v>68</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>15</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>19</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>25</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -1292,23 +1317,26 @@
       <c r="D6">
         <v>1</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6" t="s">
         <v>67</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>18</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>19</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>26</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>41</v>
       </c>
@@ -1321,23 +1349,26 @@
       <c r="D7">
         <v>1</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7" t="s">
         <v>68</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>18</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>19</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>26</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="J7" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>69</v>
       </c>
@@ -1350,20 +1381,23 @@
       <c r="D8">
         <v>2</v>
       </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="F8" t="s">
+      <c r="E8" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8" t="s">
         <v>15</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>19</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>72</v>
       </c>
@@ -1376,20 +1410,23 @@
       <c r="D9">
         <v>2</v>
       </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9" t="s">
+      <c r="E9" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9" t="s">
         <v>18</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>19</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>73</v>
       </c>
@@ -1402,20 +1439,23 @@
       <c r="D10">
         <v>2</v>
       </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10" t="s">
+      <c r="E10" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10" t="s">
         <v>15</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>19</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>74</v>
       </c>
@@ -1428,45 +1468,106 @@
       <c r="D11">
         <v>2</v>
       </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-      <c r="F11" t="s">
+      <c r="E11" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11" t="s">
         <v>18</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>19</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>80</v>
+      </c>
+      <c r="B12" t="s">
+        <v>76</v>
+      </c>
+      <c r="C12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12" s="4">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12" t="s">
+        <v>19</v>
+      </c>
+      <c r="I12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>81</v>
+      </c>
+      <c r="B13" t="s">
+        <v>75</v>
+      </c>
+      <c r="C13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13" s="4">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13" t="s">
+        <v>18</v>
+      </c>
+      <c r="H13" t="s">
+        <v>19</v>
+      </c>
+      <c r="I13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>45</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B14" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>10</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B28" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>12</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B29" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1483,20 +1584,20 @@
       <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.5546875" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5546875" customWidth="1"/>
-    <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="72.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.5703125" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="72.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>36</v>
       </c>
@@ -1525,7 +1626,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -1554,7 +1655,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -1583,7 +1684,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -1612,7 +1713,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>40</v>
       </c>
@@ -1638,7 +1739,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>41</v>
       </c>
@@ -1667,7 +1768,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>42</v>
       </c>
@@ -1696,7 +1797,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>43</v>
       </c>
@@ -1722,7 +1823,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>44</v>
       </c>
@@ -1748,7 +1849,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>45</v>
       </c>
@@ -1756,12 +1857,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>10</v>
       </c>
@@ -1769,7 +1870,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>12</v>
       </c>
@@ -1790,21 +1891,21 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.77734375" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.44140625" customWidth="1"/>
-    <col min="7" max="7" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.109375" customWidth="1"/>
-    <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="34.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.140625" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="34.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1836,7 +1937,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>51</v>
       </c>
@@ -1859,7 +1960,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>52</v>
       </c>

</xml_diff>

<commit_message>
Update simulation log objects and add scenario 3.3.3
</commit_message>
<xml_diff>
--- a/Simulation_log_key.xlsx
+++ b/Simulation_log_key.xlsx
@@ -5,24 +5,25 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zeus\Documents\R\working_directory\LemonSharkCKMR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\Documents\R\working_directory\LemonSharkCKMR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8749CD5-9C3F-45D9-8ADB-3D6F3AEE4085}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83640C46-6A68-4AD2-8FCF-DA17C74B6039}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-15480" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5085" yWindow="-11640" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Simulation_log_key" sheetId="1" r:id="rId1"/>
     <sheet name="Simulation_log_old_7.24.22" sheetId="3" r:id="rId2"/>
-    <sheet name="Objective_key" sheetId="2" r:id="rId3"/>
+    <sheet name="model_settings_old" sheetId="4" r:id="rId3"/>
+    <sheet name="Objective_key" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="167">
   <si>
     <t>Objective</t>
   </si>
@@ -271,6 +272,258 @@
   </si>
   <si>
     <t>Non-conformists</t>
+  </si>
+  <si>
+    <t>Uniform(0.80, 1.0)</t>
+  </si>
+  <si>
+    <t>Uniform(0.80, 1.20)</t>
+  </si>
+  <si>
+    <t>Minimal population growth; estimate abundance in three different years.</t>
+  </si>
+  <si>
+    <t>More extreme population decline; estimate abundance in three different years; set a lambda prior that reflects knowledge that the population is declining.</t>
+  </si>
+  <si>
+    <t>More extreme population decline; estimate abundance in three different years; set a lambda prior that does not assume knowledge about the direction of annual population change.</t>
+  </si>
+  <si>
+    <t>script_name</t>
+  </si>
+  <si>
+    <t>primary_goal</t>
+  </si>
+  <si>
+    <t>question1</t>
+  </si>
+  <si>
+    <t>question2</t>
+  </si>
+  <si>
+    <t>question3</t>
+  </si>
+  <si>
+    <t>purpose</t>
+  </si>
+  <si>
+    <t>date.of.simulation</t>
+  </si>
+  <si>
+    <t>target.YOY</t>
+  </si>
+  <si>
+    <t>down_sample</t>
+  </si>
+  <si>
+    <t>max.HSPs</t>
+  </si>
+  <si>
+    <t>max.POPs</t>
+  </si>
+  <si>
+    <t>HS.only</t>
+  </si>
+  <si>
+    <t>PO.only</t>
+  </si>
+  <si>
+    <t>fixed.parameters</t>
+  </si>
+  <si>
+    <t>estimated.parameters</t>
+  </si>
+  <si>
+    <t>seeds</t>
+  </si>
+  <si>
+    <t>thinning_rate</t>
+  </si>
+  <si>
+    <t>posterior_samples</t>
+  </si>
+  <si>
+    <t>burn_in</t>
+  </si>
+  <si>
+    <t>survival.prior.info</t>
+  </si>
+  <si>
+    <t>lambda.prior.info</t>
+  </si>
+  <si>
+    <t>psi.prior</t>
+  </si>
+  <si>
+    <t>abundance.prior</t>
+  </si>
+  <si>
+    <t>Obj1.1_model.validation_Target.YOY.R</t>
+  </si>
+  <si>
+    <t>Validate iniitial model</t>
+  </si>
+  <si>
+    <t>Does the model perform as expected in a simplified base-case scenario with an informed prior on survival?</t>
+  </si>
+  <si>
+    <t>Obj1.1_model.validation_Target.YOY</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>Nf,Nm,survival</t>
+  </si>
+  <si>
+    <t>Seeds2022.04.15</t>
+  </si>
+  <si>
+    <t>diffuse Normal w diffuse Uniform hyperprior</t>
+  </si>
+  <si>
+    <t>Obj1.1_model.validation_sample.all.juvenile.ages.R</t>
+  </si>
+  <si>
+    <t>Obj1.1_model.validation_sample.all.juvenile.ages</t>
+  </si>
+  <si>
+    <t>Obj1.1_model.validation_sample.ALL.ages.R</t>
+  </si>
+  <si>
+    <t>Obj1.1_model.validation_sample.ALL.ages</t>
+  </si>
+  <si>
+    <t>Obj1.2_model.validation_Target.YOY.R</t>
+  </si>
+  <si>
+    <t>Does the model perform as expected in a simplified base-case scenario with a diffuse prior on survival?</t>
+  </si>
+  <si>
+    <t>Obj1.2_model.validation_Target.YOY</t>
+  </si>
+  <si>
+    <t>Obj1.2_model.validation_sample.all.juvenile.ages.R</t>
+  </si>
+  <si>
+    <t>Obj1.2_model.validation_sample.all.juvenile.ages</t>
+  </si>
+  <si>
+    <t>Obj1.2_model.validation_sample.ALL.ages.R</t>
+  </si>
+  <si>
+    <t>Obj1.2_model.validation_sample.ALL.ages</t>
+  </si>
+  <si>
+    <t>Obj2.1_lambda.trial_Target.YOY.R</t>
+  </si>
+  <si>
+    <t>Test model performance with changing population size</t>
+  </si>
+  <si>
+    <t>How does a base-case CKMR model perform with changing population size?</t>
+  </si>
+  <si>
+    <t>Do we need to account for this in a CKMR model for elasmobranchs?</t>
+  </si>
+  <si>
+    <t>Obj2.1_lambda.trial_Target.YOY</t>
+  </si>
+  <si>
+    <t>Obj2.1_lambda.trial_sample.all.juvenile.ages.R</t>
+  </si>
+  <si>
+    <t>Obj2.1_lambda.trial_sample.all.juvenile.ages</t>
+  </si>
+  <si>
+    <t>Obj2.1_lambda.trial_sample.ALL.ages.R</t>
+  </si>
+  <si>
+    <t>Obj2.1_lambda.trial_sample.ALL.ages</t>
+  </si>
+  <si>
+    <t>Obj2.2.1_lambda.trial_sample.ALL.ages_stablePopSimLambda.R</t>
+  </si>
+  <si>
+    <t>Obj2.2.1_lambda.trial_sample.ALL.ages_stablePopSimLambda</t>
+  </si>
+  <si>
+    <t>Nf,Nm,survival,lambda</t>
+  </si>
+  <si>
+    <t>Obj2.2.1_lambda.trial_Target.YOY_stablePopSimLambda.R</t>
+  </si>
+  <si>
+    <t>Obj2.2.1_lambda.trial_Target.YOY_stablePopSimLambda</t>
+  </si>
+  <si>
+    <t>Obj2.2.1_lambda.trial_Target.YOY_variablePopSimLambda.R</t>
+  </si>
+  <si>
+    <t>Obj2.2.1_lambda.trial_Target.YOY_variablePopSimLambda</t>
+  </si>
+  <si>
+    <t>Obj2.2.1_lambda.trial_sample.all.juvenile.ages_stablePopSimLambda.R</t>
+  </si>
+  <si>
+    <t>Obj2.2.1_lambda.trial_sample.all.juvenile.ages_stablePopSimLambda</t>
+  </si>
+  <si>
+    <t>Obj2.2.1_lambda.trial_sample.all.juvenile.ages_variablePopSimLambda.R</t>
+  </si>
+  <si>
+    <t>Obj2.2.1_lambda.trial_sample.all.juvenile.ages_variablePopSimLambda</t>
+  </si>
+  <si>
+    <t>Obj2.2.1_lambda.trial_sample.ALL.ages_variablePopSimLambda.R</t>
+  </si>
+  <si>
+    <t>Obj2.2.1_lambda.trial_sample.ALL.ages_variablePopSimLambda</t>
+  </si>
+  <si>
+    <t>Obj2.2.2_lambda.trial_sample.ALL.ages_change.est.yr.R</t>
+  </si>
+  <si>
+    <t>Does lambda become more important if we change the year of estimation?</t>
+  </si>
+  <si>
+    <t>Obj2.2.2_lambda.trial_sample.ALL.ages_change.est.yr</t>
+  </si>
+  <si>
+    <t>Obj2.2.2_lambda.trial_sample.all.juvenile.ages_change.est.yr.R</t>
+  </si>
+  <si>
+    <t>Obj2.2.2_lambda.trial_sample.all.juvenile.ages_change.est.yr</t>
+  </si>
+  <si>
+    <t>Obj2.2.2_lambda.trial_target.YOY_change.est.yr.R</t>
+  </si>
+  <si>
+    <t>Obj2.2.2_lambda.trial_target.YOY_change.est.yr</t>
+  </si>
+  <si>
+    <t>Obj2.2.2_lambda.trial_sample.ALL.ages_stablePopSimLambda_change.est.yr.R</t>
+  </si>
+  <si>
+    <t>Obj2.2.2_lambda.trial_sample.ALL.ages_stablePopSimLambda_change.est.yr</t>
+  </si>
+  <si>
+    <t>Obj2.2.2_lambda.trial_sample.all.juvenile.ages_stablePopSimLambda_change.est.yr.R</t>
+  </si>
+  <si>
+    <t>Obj2.2.2_lambda.trial_sample.all.juvenile.ages_stablePopSimLambda_change.est.yr</t>
+  </si>
+  <si>
+    <t>Obj2.2.2_lambda.trial_target.YOY_stablePopSimLambda_change.est.yr.R</t>
+  </si>
+  <si>
+    <t>Obj2.2.2_lambda.trial_target.YOY_stablePopSimLambda_change.est.yr</t>
   </si>
 </sst>
 </file>
@@ -760,7 +1013,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -770,6 +1023,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1125,26 +1379,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="62.5703125" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="16.5703125" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="43.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="72.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.5546875" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="16.5546875" customWidth="1"/>
+    <col min="6" max="6" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="43.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="72.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>36</v>
       </c>
@@ -1176,7 +1430,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -1208,7 +1462,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -1240,7 +1494,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>78</v>
       </c>
@@ -1272,7 +1526,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>79</v>
       </c>
@@ -1304,7 +1558,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -1333,10 +1587,10 @@
         <v>26</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>41</v>
       </c>
@@ -1356,7 +1610,7 @@
         <v>68</v>
       </c>
       <c r="G7" t="s">
-        <v>18</v>
+        <v>83</v>
       </c>
       <c r="H7" t="s">
         <v>19</v>
@@ -1365,44 +1619,47 @@
         <v>26</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>69</v>
+        <v>42</v>
       </c>
       <c r="B8" t="s">
-        <v>70</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s">
         <v>17</v>
       </c>
       <c r="D8">
-        <v>2</v>
-      </c>
-      <c r="E8" s="4">
-        <v>0.05</v>
-      </c>
-      <c r="F8">
         <v>1</v>
       </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8" t="s">
+        <v>68</v>
+      </c>
       <c r="G8" t="s">
-        <v>15</v>
+        <v>84</v>
       </c>
       <c r="H8" t="s">
         <v>19</v>
       </c>
       <c r="I8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C9" t="s">
         <v>17</v>
@@ -1417,21 +1674,21 @@
         <v>1</v>
       </c>
       <c r="G9" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H9" t="s">
         <v>19</v>
       </c>
       <c r="I9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B10" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C10" t="s">
         <v>17</v>
@@ -1446,21 +1703,21 @@
         <v>1</v>
       </c>
       <c r="G10" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="H10" t="s">
         <v>19</v>
       </c>
       <c r="I10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B11" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C11" t="s">
         <v>17</v>
@@ -1475,21 +1732,21 @@
         <v>1</v>
       </c>
       <c r="G11" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H11" t="s">
         <v>19</v>
       </c>
       <c r="I11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C12" t="s">
         <v>17</v>
@@ -1498,27 +1755,27 @@
         <v>2</v>
       </c>
       <c r="E12" s="4">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="F12">
         <v>1</v>
       </c>
       <c r="G12" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="H12" t="s">
         <v>19</v>
       </c>
       <c r="I12" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B13" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C13" t="s">
         <v>17</v>
@@ -1533,41 +1790,70 @@
         <v>1</v>
       </c>
       <c r="G13" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H13" t="s">
         <v>19</v>
       </c>
       <c r="I13" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B14" t="s">
+        <v>75</v>
+      </c>
+      <c r="C14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14" s="4">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14" t="s">
+        <v>18</v>
+      </c>
+      <c r="H14" t="s">
+        <v>19</v>
+      </c>
+      <c r="I14" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>45</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>10</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B29" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>12</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B30" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1584,20 +1870,20 @@
       <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.5703125" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="43.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="72.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.5546875" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="43.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="72.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>36</v>
       </c>
@@ -1626,7 +1912,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -1655,7 +1941,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -1684,7 +1970,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -1713,7 +1999,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>40</v>
       </c>
@@ -1739,7 +2025,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>41</v>
       </c>
@@ -1768,7 +2054,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>42</v>
       </c>
@@ -1797,7 +2083,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>43</v>
       </c>
@@ -1823,7 +2109,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>44</v>
       </c>
@@ -1849,7 +2135,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>45</v>
       </c>
@@ -1857,12 +2143,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>10</v>
       </c>
@@ -1870,7 +2156,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>12</v>
       </c>
@@ -1884,6 +2170,1583 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{919B2633-F7CB-4C36-8605-E7950C491D12}">
+  <dimension ref="A1:W22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G1" t="s">
+        <v>94</v>
+      </c>
+      <c r="H1" t="s">
+        <v>95</v>
+      </c>
+      <c r="I1" t="s">
+        <v>96</v>
+      </c>
+      <c r="J1" t="s">
+        <v>97</v>
+      </c>
+      <c r="K1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L1" t="s">
+        <v>99</v>
+      </c>
+      <c r="M1" t="s">
+        <v>100</v>
+      </c>
+      <c r="N1" t="s">
+        <v>101</v>
+      </c>
+      <c r="O1" t="s">
+        <v>102</v>
+      </c>
+      <c r="P1" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>104</v>
+      </c>
+      <c r="R1" t="s">
+        <v>105</v>
+      </c>
+      <c r="S1" t="s">
+        <v>106</v>
+      </c>
+      <c r="T1" t="s">
+        <v>107</v>
+      </c>
+      <c r="U1" t="s">
+        <v>108</v>
+      </c>
+      <c r="V1" t="s">
+        <v>109</v>
+      </c>
+      <c r="W1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
+        <v>114</v>
+      </c>
+      <c r="G2" s="5">
+        <v>44754</v>
+      </c>
+      <c r="H2" t="s">
+        <v>115</v>
+      </c>
+      <c r="I2" t="s">
+        <v>116</v>
+      </c>
+      <c r="J2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L2" t="s">
+        <v>115</v>
+      </c>
+      <c r="M2" t="s">
+        <v>116</v>
+      </c>
+      <c r="N2" t="s">
+        <v>117</v>
+      </c>
+      <c r="O2" t="s">
+        <v>118</v>
+      </c>
+      <c r="P2" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q2">
+        <v>20</v>
+      </c>
+      <c r="R2">
+        <v>40000</v>
+      </c>
+      <c r="S2">
+        <v>50000</v>
+      </c>
+      <c r="T2">
+        <v>0.82499999999999996</v>
+      </c>
+      <c r="U2" t="s">
+        <v>15</v>
+      </c>
+      <c r="V2" t="s">
+        <v>15</v>
+      </c>
+      <c r="W2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>122</v>
+      </c>
+      <c r="G3" s="5">
+        <v>44754</v>
+      </c>
+      <c r="H3" t="s">
+        <v>116</v>
+      </c>
+      <c r="I3" t="s">
+        <v>116</v>
+      </c>
+      <c r="J3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L3" t="s">
+        <v>115</v>
+      </c>
+      <c r="M3" t="s">
+        <v>116</v>
+      </c>
+      <c r="N3" t="s">
+        <v>117</v>
+      </c>
+      <c r="O3" t="s">
+        <v>118</v>
+      </c>
+      <c r="P3" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q3">
+        <v>20</v>
+      </c>
+      <c r="R3">
+        <v>40000</v>
+      </c>
+      <c r="S3">
+        <v>50000</v>
+      </c>
+      <c r="T3">
+        <v>0.82499999999999996</v>
+      </c>
+      <c r="U3" t="s">
+        <v>15</v>
+      </c>
+      <c r="V3" t="s">
+        <v>15</v>
+      </c>
+      <c r="W3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C4" t="s">
+        <v>113</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
+        <v>124</v>
+      </c>
+      <c r="G4" s="5">
+        <v>44755</v>
+      </c>
+      <c r="H4" t="s">
+        <v>116</v>
+      </c>
+      <c r="I4" t="s">
+        <v>116</v>
+      </c>
+      <c r="J4" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L4" t="s">
+        <v>116</v>
+      </c>
+      <c r="M4" t="s">
+        <v>116</v>
+      </c>
+      <c r="N4" t="s">
+        <v>117</v>
+      </c>
+      <c r="O4" t="s">
+        <v>118</v>
+      </c>
+      <c r="P4" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q4">
+        <v>20</v>
+      </c>
+      <c r="R4">
+        <v>40000</v>
+      </c>
+      <c r="S4">
+        <v>50000</v>
+      </c>
+      <c r="T4">
+        <v>0.82499999999999996</v>
+      </c>
+      <c r="U4" t="s">
+        <v>15</v>
+      </c>
+      <c r="V4" t="s">
+        <v>15</v>
+      </c>
+      <c r="W4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C5" t="s">
+        <v>126</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" t="s">
+        <v>127</v>
+      </c>
+      <c r="G5" s="5">
+        <v>44755</v>
+      </c>
+      <c r="H5" t="s">
+        <v>115</v>
+      </c>
+      <c r="I5" t="s">
+        <v>116</v>
+      </c>
+      <c r="J5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L5" t="s">
+        <v>115</v>
+      </c>
+      <c r="M5" t="s">
+        <v>116</v>
+      </c>
+      <c r="N5" t="s">
+        <v>117</v>
+      </c>
+      <c r="O5" t="s">
+        <v>118</v>
+      </c>
+      <c r="P5" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q5">
+        <v>20</v>
+      </c>
+      <c r="R5">
+        <v>40000</v>
+      </c>
+      <c r="S5">
+        <v>50000</v>
+      </c>
+      <c r="T5" t="s">
+        <v>15</v>
+      </c>
+      <c r="U5" t="s">
+        <v>15</v>
+      </c>
+      <c r="V5" t="s">
+        <v>15</v>
+      </c>
+      <c r="W5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>128</v>
+      </c>
+      <c r="B6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C6" t="s">
+        <v>126</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" t="s">
+        <v>129</v>
+      </c>
+      <c r="G6" s="5">
+        <v>44755</v>
+      </c>
+      <c r="H6" t="s">
+        <v>116</v>
+      </c>
+      <c r="I6" t="s">
+        <v>116</v>
+      </c>
+      <c r="J6" t="s">
+        <v>15</v>
+      </c>
+      <c r="K6" t="s">
+        <v>15</v>
+      </c>
+      <c r="L6" t="s">
+        <v>115</v>
+      </c>
+      <c r="M6" t="s">
+        <v>116</v>
+      </c>
+      <c r="N6" t="s">
+        <v>117</v>
+      </c>
+      <c r="O6" t="s">
+        <v>118</v>
+      </c>
+      <c r="P6" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q6">
+        <v>20</v>
+      </c>
+      <c r="R6">
+        <v>40000</v>
+      </c>
+      <c r="S6">
+        <v>50000</v>
+      </c>
+      <c r="T6" t="s">
+        <v>15</v>
+      </c>
+      <c r="U6" t="s">
+        <v>15</v>
+      </c>
+      <c r="V6" t="s">
+        <v>15</v>
+      </c>
+      <c r="W6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>130</v>
+      </c>
+      <c r="B7" t="s">
+        <v>112</v>
+      </c>
+      <c r="C7" t="s">
+        <v>126</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" t="s">
+        <v>131</v>
+      </c>
+      <c r="G7" s="5">
+        <v>44755</v>
+      </c>
+      <c r="H7" t="s">
+        <v>116</v>
+      </c>
+      <c r="I7" t="s">
+        <v>116</v>
+      </c>
+      <c r="J7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K7" t="s">
+        <v>15</v>
+      </c>
+      <c r="L7" t="s">
+        <v>116</v>
+      </c>
+      <c r="M7" t="s">
+        <v>116</v>
+      </c>
+      <c r="N7" t="s">
+        <v>117</v>
+      </c>
+      <c r="O7" t="s">
+        <v>118</v>
+      </c>
+      <c r="P7" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q7">
+        <v>20</v>
+      </c>
+      <c r="R7">
+        <v>40000</v>
+      </c>
+      <c r="S7">
+        <v>50000</v>
+      </c>
+      <c r="T7" t="s">
+        <v>15</v>
+      </c>
+      <c r="U7" t="s">
+        <v>15</v>
+      </c>
+      <c r="V7" t="s">
+        <v>15</v>
+      </c>
+      <c r="W7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>132</v>
+      </c>
+      <c r="B8" t="s">
+        <v>133</v>
+      </c>
+      <c r="C8" t="s">
+        <v>134</v>
+      </c>
+      <c r="D8" t="s">
+        <v>135</v>
+      </c>
+      <c r="E8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" t="s">
+        <v>136</v>
+      </c>
+      <c r="G8" s="5">
+        <v>44755</v>
+      </c>
+      <c r="H8" t="s">
+        <v>115</v>
+      </c>
+      <c r="I8" t="s">
+        <v>116</v>
+      </c>
+      <c r="J8" t="s">
+        <v>15</v>
+      </c>
+      <c r="K8" t="s">
+        <v>15</v>
+      </c>
+      <c r="L8" t="s">
+        <v>115</v>
+      </c>
+      <c r="M8" t="s">
+        <v>116</v>
+      </c>
+      <c r="N8" t="s">
+        <v>117</v>
+      </c>
+      <c r="O8" t="s">
+        <v>118</v>
+      </c>
+      <c r="P8" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q8">
+        <v>20</v>
+      </c>
+      <c r="R8">
+        <v>40000</v>
+      </c>
+      <c r="S8">
+        <v>50000</v>
+      </c>
+      <c r="T8" t="s">
+        <v>15</v>
+      </c>
+      <c r="U8" t="s">
+        <v>15</v>
+      </c>
+      <c r="V8" t="s">
+        <v>15</v>
+      </c>
+      <c r="W8" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>137</v>
+      </c>
+      <c r="B9" t="s">
+        <v>133</v>
+      </c>
+      <c r="C9" t="s">
+        <v>134</v>
+      </c>
+      <c r="D9" t="s">
+        <v>135</v>
+      </c>
+      <c r="E9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" t="s">
+        <v>138</v>
+      </c>
+      <c r="G9" s="5">
+        <v>44755</v>
+      </c>
+      <c r="H9" t="s">
+        <v>116</v>
+      </c>
+      <c r="I9" t="s">
+        <v>116</v>
+      </c>
+      <c r="J9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K9" t="s">
+        <v>15</v>
+      </c>
+      <c r="L9" t="s">
+        <v>115</v>
+      </c>
+      <c r="M9" t="s">
+        <v>116</v>
+      </c>
+      <c r="N9" t="s">
+        <v>117</v>
+      </c>
+      <c r="O9" t="s">
+        <v>118</v>
+      </c>
+      <c r="P9" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q9">
+        <v>20</v>
+      </c>
+      <c r="R9">
+        <v>40000</v>
+      </c>
+      <c r="S9">
+        <v>50000</v>
+      </c>
+      <c r="T9" t="s">
+        <v>15</v>
+      </c>
+      <c r="U9" t="s">
+        <v>15</v>
+      </c>
+      <c r="V9" t="s">
+        <v>15</v>
+      </c>
+      <c r="W9" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>139</v>
+      </c>
+      <c r="B10" t="s">
+        <v>133</v>
+      </c>
+      <c r="C10" t="s">
+        <v>134</v>
+      </c>
+      <c r="D10" t="s">
+        <v>135</v>
+      </c>
+      <c r="E10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" t="s">
+        <v>140</v>
+      </c>
+      <c r="G10" s="5">
+        <v>44755</v>
+      </c>
+      <c r="H10" t="s">
+        <v>116</v>
+      </c>
+      <c r="I10" t="s">
+        <v>116</v>
+      </c>
+      <c r="J10" t="s">
+        <v>15</v>
+      </c>
+      <c r="K10" t="s">
+        <v>15</v>
+      </c>
+      <c r="L10" t="s">
+        <v>116</v>
+      </c>
+      <c r="M10" t="s">
+        <v>116</v>
+      </c>
+      <c r="N10" t="s">
+        <v>117</v>
+      </c>
+      <c r="O10" t="s">
+        <v>118</v>
+      </c>
+      <c r="P10" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q10">
+        <v>20</v>
+      </c>
+      <c r="R10">
+        <v>40000</v>
+      </c>
+      <c r="S10">
+        <v>50000</v>
+      </c>
+      <c r="T10" t="s">
+        <v>15</v>
+      </c>
+      <c r="U10" t="s">
+        <v>15</v>
+      </c>
+      <c r="V10" t="s">
+        <v>15</v>
+      </c>
+      <c r="W10" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>141</v>
+      </c>
+      <c r="B11" t="s">
+        <v>133</v>
+      </c>
+      <c r="C11" t="s">
+        <v>134</v>
+      </c>
+      <c r="D11" t="s">
+        <v>135</v>
+      </c>
+      <c r="E11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" t="s">
+        <v>142</v>
+      </c>
+      <c r="G11" s="5">
+        <v>44755</v>
+      </c>
+      <c r="H11" t="s">
+        <v>116</v>
+      </c>
+      <c r="I11" t="s">
+        <v>116</v>
+      </c>
+      <c r="J11" t="s">
+        <v>15</v>
+      </c>
+      <c r="K11" t="s">
+        <v>15</v>
+      </c>
+      <c r="L11" t="s">
+        <v>116</v>
+      </c>
+      <c r="M11" t="s">
+        <v>116</v>
+      </c>
+      <c r="N11" t="s">
+        <v>117</v>
+      </c>
+      <c r="O11" t="s">
+        <v>143</v>
+      </c>
+      <c r="P11" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q11">
+        <v>20</v>
+      </c>
+      <c r="R11">
+        <v>40000</v>
+      </c>
+      <c r="S11">
+        <v>50000</v>
+      </c>
+      <c r="T11" t="s">
+        <v>15</v>
+      </c>
+      <c r="U11" t="s">
+        <v>15</v>
+      </c>
+      <c r="V11" t="s">
+        <v>15</v>
+      </c>
+      <c r="W11" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>144</v>
+      </c>
+      <c r="B12" t="s">
+        <v>133</v>
+      </c>
+      <c r="C12" t="s">
+        <v>134</v>
+      </c>
+      <c r="D12" t="s">
+        <v>135</v>
+      </c>
+      <c r="E12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" t="s">
+        <v>145</v>
+      </c>
+      <c r="G12" s="5">
+        <v>44755</v>
+      </c>
+      <c r="H12" t="s">
+        <v>115</v>
+      </c>
+      <c r="I12" t="s">
+        <v>116</v>
+      </c>
+      <c r="J12" t="s">
+        <v>15</v>
+      </c>
+      <c r="K12" t="s">
+        <v>15</v>
+      </c>
+      <c r="L12" t="s">
+        <v>115</v>
+      </c>
+      <c r="M12" t="s">
+        <v>116</v>
+      </c>
+      <c r="N12" t="s">
+        <v>117</v>
+      </c>
+      <c r="O12" t="s">
+        <v>143</v>
+      </c>
+      <c r="P12" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q12">
+        <v>20</v>
+      </c>
+      <c r="R12">
+        <v>40000</v>
+      </c>
+      <c r="S12">
+        <v>50000</v>
+      </c>
+      <c r="T12" t="s">
+        <v>15</v>
+      </c>
+      <c r="U12" t="s">
+        <v>15</v>
+      </c>
+      <c r="V12" t="s">
+        <v>15</v>
+      </c>
+      <c r="W12" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>146</v>
+      </c>
+      <c r="B13" t="s">
+        <v>133</v>
+      </c>
+      <c r="C13" t="s">
+        <v>134</v>
+      </c>
+      <c r="D13" t="s">
+        <v>135</v>
+      </c>
+      <c r="E13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" t="s">
+        <v>147</v>
+      </c>
+      <c r="G13" s="5">
+        <v>44755</v>
+      </c>
+      <c r="H13" t="s">
+        <v>115</v>
+      </c>
+      <c r="I13" t="s">
+        <v>116</v>
+      </c>
+      <c r="J13" t="s">
+        <v>15</v>
+      </c>
+      <c r="K13" t="s">
+        <v>15</v>
+      </c>
+      <c r="L13" t="s">
+        <v>115</v>
+      </c>
+      <c r="M13" t="s">
+        <v>116</v>
+      </c>
+      <c r="N13" t="s">
+        <v>117</v>
+      </c>
+      <c r="O13" t="s">
+        <v>143</v>
+      </c>
+      <c r="P13" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q13">
+        <v>20</v>
+      </c>
+      <c r="R13">
+        <v>40000</v>
+      </c>
+      <c r="S13">
+        <v>50000</v>
+      </c>
+      <c r="T13" t="s">
+        <v>15</v>
+      </c>
+      <c r="U13" t="s">
+        <v>15</v>
+      </c>
+      <c r="V13" t="s">
+        <v>15</v>
+      </c>
+      <c r="W13" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>148</v>
+      </c>
+      <c r="B14" t="s">
+        <v>133</v>
+      </c>
+      <c r="C14" t="s">
+        <v>134</v>
+      </c>
+      <c r="D14" t="s">
+        <v>135</v>
+      </c>
+      <c r="E14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" t="s">
+        <v>149</v>
+      </c>
+      <c r="G14" s="5">
+        <v>44755</v>
+      </c>
+      <c r="H14" t="s">
+        <v>116</v>
+      </c>
+      <c r="I14" t="s">
+        <v>116</v>
+      </c>
+      <c r="J14" t="s">
+        <v>15</v>
+      </c>
+      <c r="K14" t="s">
+        <v>15</v>
+      </c>
+      <c r="L14" t="s">
+        <v>115</v>
+      </c>
+      <c r="M14" t="s">
+        <v>116</v>
+      </c>
+      <c r="N14" t="s">
+        <v>117</v>
+      </c>
+      <c r="O14" t="s">
+        <v>143</v>
+      </c>
+      <c r="P14" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q14">
+        <v>20</v>
+      </c>
+      <c r="R14">
+        <v>40000</v>
+      </c>
+      <c r="S14">
+        <v>50000</v>
+      </c>
+      <c r="T14" t="s">
+        <v>15</v>
+      </c>
+      <c r="U14" t="s">
+        <v>15</v>
+      </c>
+      <c r="V14" t="s">
+        <v>15</v>
+      </c>
+      <c r="W14" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>150</v>
+      </c>
+      <c r="B15" t="s">
+        <v>133</v>
+      </c>
+      <c r="C15" t="s">
+        <v>134</v>
+      </c>
+      <c r="D15" t="s">
+        <v>135</v>
+      </c>
+      <c r="E15" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" t="s">
+        <v>151</v>
+      </c>
+      <c r="G15" s="5">
+        <v>44755</v>
+      </c>
+      <c r="H15" t="s">
+        <v>116</v>
+      </c>
+      <c r="I15" t="s">
+        <v>116</v>
+      </c>
+      <c r="J15" t="s">
+        <v>15</v>
+      </c>
+      <c r="K15" t="s">
+        <v>15</v>
+      </c>
+      <c r="L15" t="s">
+        <v>115</v>
+      </c>
+      <c r="M15" t="s">
+        <v>116</v>
+      </c>
+      <c r="N15" t="s">
+        <v>117</v>
+      </c>
+      <c r="O15" t="s">
+        <v>143</v>
+      </c>
+      <c r="P15" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q15">
+        <v>20</v>
+      </c>
+      <c r="R15">
+        <v>40000</v>
+      </c>
+      <c r="S15">
+        <v>50000</v>
+      </c>
+      <c r="T15" t="s">
+        <v>15</v>
+      </c>
+      <c r="U15" t="s">
+        <v>15</v>
+      </c>
+      <c r="V15" t="s">
+        <v>15</v>
+      </c>
+      <c r="W15" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>152</v>
+      </c>
+      <c r="B16" t="s">
+        <v>133</v>
+      </c>
+      <c r="C16" t="s">
+        <v>134</v>
+      </c>
+      <c r="D16" t="s">
+        <v>135</v>
+      </c>
+      <c r="E16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" t="s">
+        <v>153</v>
+      </c>
+      <c r="G16" s="5">
+        <v>44755</v>
+      </c>
+      <c r="H16" t="s">
+        <v>116</v>
+      </c>
+      <c r="I16" t="s">
+        <v>116</v>
+      </c>
+      <c r="J16" t="s">
+        <v>15</v>
+      </c>
+      <c r="K16" t="s">
+        <v>15</v>
+      </c>
+      <c r="L16" t="s">
+        <v>116</v>
+      </c>
+      <c r="M16" t="s">
+        <v>116</v>
+      </c>
+      <c r="N16" t="s">
+        <v>117</v>
+      </c>
+      <c r="O16" t="s">
+        <v>143</v>
+      </c>
+      <c r="P16" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q16">
+        <v>20</v>
+      </c>
+      <c r="R16">
+        <v>40000</v>
+      </c>
+      <c r="S16">
+        <v>50000</v>
+      </c>
+      <c r="T16" t="s">
+        <v>15</v>
+      </c>
+      <c r="U16" t="s">
+        <v>15</v>
+      </c>
+      <c r="V16" t="s">
+        <v>15</v>
+      </c>
+      <c r="W16" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>154</v>
+      </c>
+      <c r="B17" t="s">
+        <v>133</v>
+      </c>
+      <c r="C17" t="s">
+        <v>134</v>
+      </c>
+      <c r="D17" t="s">
+        <v>135</v>
+      </c>
+      <c r="E17" t="s">
+        <v>155</v>
+      </c>
+      <c r="F17" t="s">
+        <v>156</v>
+      </c>
+      <c r="G17" s="5">
+        <v>44756</v>
+      </c>
+      <c r="H17" t="s">
+        <v>116</v>
+      </c>
+      <c r="I17" t="s">
+        <v>116</v>
+      </c>
+      <c r="J17" t="s">
+        <v>15</v>
+      </c>
+      <c r="K17" t="s">
+        <v>15</v>
+      </c>
+      <c r="L17" t="s">
+        <v>116</v>
+      </c>
+      <c r="M17" t="s">
+        <v>116</v>
+      </c>
+      <c r="N17" t="s">
+        <v>117</v>
+      </c>
+      <c r="O17" t="s">
+        <v>143</v>
+      </c>
+      <c r="P17" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q17">
+        <v>20</v>
+      </c>
+      <c r="R17">
+        <v>40000</v>
+      </c>
+      <c r="S17">
+        <v>50000</v>
+      </c>
+      <c r="T17" t="s">
+        <v>15</v>
+      </c>
+      <c r="U17" t="s">
+        <v>15</v>
+      </c>
+      <c r="V17" t="s">
+        <v>15</v>
+      </c>
+      <c r="W17" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B18" t="s">
+        <v>133</v>
+      </c>
+      <c r="C18" t="s">
+        <v>134</v>
+      </c>
+      <c r="D18" t="s">
+        <v>135</v>
+      </c>
+      <c r="E18" t="s">
+        <v>155</v>
+      </c>
+      <c r="F18" t="s">
+        <v>158</v>
+      </c>
+      <c r="G18" s="5">
+        <v>44756</v>
+      </c>
+      <c r="H18" t="s">
+        <v>116</v>
+      </c>
+      <c r="I18" t="s">
+        <v>116</v>
+      </c>
+      <c r="J18" t="s">
+        <v>15</v>
+      </c>
+      <c r="K18" t="s">
+        <v>15</v>
+      </c>
+      <c r="L18" t="s">
+        <v>115</v>
+      </c>
+      <c r="M18" t="s">
+        <v>116</v>
+      </c>
+      <c r="N18" t="s">
+        <v>117</v>
+      </c>
+      <c r="O18" t="s">
+        <v>143</v>
+      </c>
+      <c r="P18" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q18">
+        <v>20</v>
+      </c>
+      <c r="R18">
+        <v>40000</v>
+      </c>
+      <c r="S18">
+        <v>50000</v>
+      </c>
+      <c r="T18" t="s">
+        <v>15</v>
+      </c>
+      <c r="U18" t="s">
+        <v>15</v>
+      </c>
+      <c r="V18" t="s">
+        <v>15</v>
+      </c>
+      <c r="W18" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>159</v>
+      </c>
+      <c r="B19" t="s">
+        <v>133</v>
+      </c>
+      <c r="C19" t="s">
+        <v>134</v>
+      </c>
+      <c r="D19" t="s">
+        <v>135</v>
+      </c>
+      <c r="E19" t="s">
+        <v>155</v>
+      </c>
+      <c r="F19" t="s">
+        <v>160</v>
+      </c>
+      <c r="G19" s="5">
+        <v>44756</v>
+      </c>
+      <c r="H19" t="s">
+        <v>115</v>
+      </c>
+      <c r="I19" t="s">
+        <v>116</v>
+      </c>
+      <c r="J19" t="s">
+        <v>15</v>
+      </c>
+      <c r="K19" t="s">
+        <v>15</v>
+      </c>
+      <c r="L19" t="s">
+        <v>115</v>
+      </c>
+      <c r="M19" t="s">
+        <v>116</v>
+      </c>
+      <c r="N19" t="s">
+        <v>117</v>
+      </c>
+      <c r="O19" t="s">
+        <v>143</v>
+      </c>
+      <c r="P19" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q19">
+        <v>20</v>
+      </c>
+      <c r="R19">
+        <v>40000</v>
+      </c>
+      <c r="S19">
+        <v>50000</v>
+      </c>
+      <c r="T19" t="s">
+        <v>15</v>
+      </c>
+      <c r="U19" t="s">
+        <v>15</v>
+      </c>
+      <c r="V19" t="s">
+        <v>15</v>
+      </c>
+      <c r="W19" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>161</v>
+      </c>
+      <c r="B20" t="s">
+        <v>133</v>
+      </c>
+      <c r="C20" t="s">
+        <v>134</v>
+      </c>
+      <c r="D20" t="s">
+        <v>135</v>
+      </c>
+      <c r="E20" t="s">
+        <v>155</v>
+      </c>
+      <c r="F20" t="s">
+        <v>162</v>
+      </c>
+      <c r="G20" s="5">
+        <v>44757</v>
+      </c>
+      <c r="H20" t="s">
+        <v>116</v>
+      </c>
+      <c r="I20" t="s">
+        <v>116</v>
+      </c>
+      <c r="J20" t="s">
+        <v>15</v>
+      </c>
+      <c r="K20" t="s">
+        <v>15</v>
+      </c>
+      <c r="L20" t="s">
+        <v>116</v>
+      </c>
+      <c r="M20" t="s">
+        <v>116</v>
+      </c>
+      <c r="N20" t="s">
+        <v>117</v>
+      </c>
+      <c r="O20" t="s">
+        <v>143</v>
+      </c>
+      <c r="P20" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q20">
+        <v>20</v>
+      </c>
+      <c r="R20">
+        <v>40000</v>
+      </c>
+      <c r="S20">
+        <v>50000</v>
+      </c>
+      <c r="T20" t="s">
+        <v>15</v>
+      </c>
+      <c r="U20" t="s">
+        <v>15</v>
+      </c>
+      <c r="V20" t="s">
+        <v>15</v>
+      </c>
+      <c r="W20" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>163</v>
+      </c>
+      <c r="B21" t="s">
+        <v>133</v>
+      </c>
+      <c r="C21" t="s">
+        <v>134</v>
+      </c>
+      <c r="D21" t="s">
+        <v>135</v>
+      </c>
+      <c r="E21" t="s">
+        <v>155</v>
+      </c>
+      <c r="F21" t="s">
+        <v>164</v>
+      </c>
+      <c r="G21" s="5">
+        <v>44757</v>
+      </c>
+      <c r="H21" t="s">
+        <v>116</v>
+      </c>
+      <c r="I21" t="s">
+        <v>116</v>
+      </c>
+      <c r="J21" t="s">
+        <v>15</v>
+      </c>
+      <c r="K21" t="s">
+        <v>15</v>
+      </c>
+      <c r="L21" t="s">
+        <v>115</v>
+      </c>
+      <c r="M21" t="s">
+        <v>116</v>
+      </c>
+      <c r="N21" t="s">
+        <v>117</v>
+      </c>
+      <c r="O21" t="s">
+        <v>143</v>
+      </c>
+      <c r="P21" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q21">
+        <v>20</v>
+      </c>
+      <c r="R21">
+        <v>40000</v>
+      </c>
+      <c r="S21">
+        <v>50000</v>
+      </c>
+      <c r="T21" t="s">
+        <v>15</v>
+      </c>
+      <c r="U21" t="s">
+        <v>15</v>
+      </c>
+      <c r="V21" t="s">
+        <v>15</v>
+      </c>
+      <c r="W21" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>165</v>
+      </c>
+      <c r="B22" t="s">
+        <v>133</v>
+      </c>
+      <c r="C22" t="s">
+        <v>134</v>
+      </c>
+      <c r="D22" t="s">
+        <v>135</v>
+      </c>
+      <c r="E22" t="s">
+        <v>155</v>
+      </c>
+      <c r="F22" t="s">
+        <v>166</v>
+      </c>
+      <c r="G22" s="5">
+        <v>44757</v>
+      </c>
+      <c r="H22" t="s">
+        <v>115</v>
+      </c>
+      <c r="I22" t="s">
+        <v>116</v>
+      </c>
+      <c r="J22" t="s">
+        <v>15</v>
+      </c>
+      <c r="K22" t="s">
+        <v>15</v>
+      </c>
+      <c r="L22" t="s">
+        <v>115</v>
+      </c>
+      <c r="M22" t="s">
+        <v>116</v>
+      </c>
+      <c r="N22" t="s">
+        <v>117</v>
+      </c>
+      <c r="O22" t="s">
+        <v>143</v>
+      </c>
+      <c r="P22" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q22">
+        <v>20</v>
+      </c>
+      <c r="R22">
+        <v>40000</v>
+      </c>
+      <c r="S22">
+        <v>50000</v>
+      </c>
+      <c r="T22" t="s">
+        <v>15</v>
+      </c>
+      <c r="U22" t="s">
+        <v>15</v>
+      </c>
+      <c r="V22" t="s">
+        <v>15</v>
+      </c>
+      <c r="W22" t="s">
+        <v>120</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{412D6C35-5CAD-470C-B537-E441B956C3CF}">
   <dimension ref="A1:J3"/>
   <sheetViews>
@@ -1891,21 +3754,21 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.7109375" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.6640625" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.140625" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.44140625" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.109375" customWidth="1"/>
+    <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="34.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1937,7 +3800,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>51</v>
       </c>
@@ -1960,7 +3823,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>52</v>
       </c>

</xml_diff>

<commit_message>
Update data viz script
</commit_message>
<xml_diff>
--- a/Simulation_log_key.xlsx
+++ b/Simulation_log_key.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\Documents\R\working_directory\LemonSharkCKMR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zeus\Documents\R\working_directory\LemonSharkCKMR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83640C46-6A68-4AD2-8FCF-DA17C74B6039}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E66845E-B583-4F24-95BF-EAC85BD375FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5085" yWindow="-11640" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-11640" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Simulation_log_key" sheetId="1" r:id="rId1"/>
@@ -1381,24 +1381,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="62.5546875" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="16.5546875" customWidth="1"/>
-    <col min="6" max="6" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="72.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.5703125" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="16.5703125" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="72.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>36</v>
       </c>
@@ -1430,7 +1430,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -1462,7 +1462,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -1494,7 +1494,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>78</v>
       </c>
@@ -1526,7 +1526,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>79</v>
       </c>
@@ -1558,7 +1558,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -1590,7 +1590,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>41</v>
       </c>
@@ -1622,7 +1622,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>42</v>
       </c>
@@ -1654,7 +1654,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>69</v>
       </c>
@@ -1683,7 +1683,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>72</v>
       </c>
@@ -1712,7 +1712,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>73</v>
       </c>
@@ -1741,7 +1741,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>74</v>
       </c>
@@ -1770,7 +1770,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>80</v>
       </c>
@@ -1799,7 +1799,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>81</v>
       </c>
@@ -1828,7 +1828,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>45</v>
       </c>
@@ -1836,12 +1836,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>10</v>
       </c>
@@ -1849,7 +1849,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>12</v>
       </c>
@@ -1870,20 +1870,20 @@
       <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.5546875" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5546875" customWidth="1"/>
-    <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="72.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.5703125" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="72.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>36</v>
       </c>
@@ -1912,7 +1912,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -1941,7 +1941,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -1970,7 +1970,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -1999,7 +1999,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>40</v>
       </c>
@@ -2025,7 +2025,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>41</v>
       </c>
@@ -2054,7 +2054,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>42</v>
       </c>
@@ -2083,7 +2083,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>43</v>
       </c>
@@ -2109,7 +2109,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>44</v>
       </c>
@@ -2135,7 +2135,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>45</v>
       </c>
@@ -2143,12 +2143,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>10</v>
       </c>
@@ -2156,7 +2156,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>12</v>
       </c>
@@ -2173,13 +2173,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{919B2633-F7CB-4C36-8605-E7950C491D12}">
   <dimension ref="A1:W22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="79.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="98.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="62.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="69" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="77.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="41.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>88</v>
       </c>
@@ -2250,7 +2275,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>111</v>
       </c>
@@ -2321,7 +2346,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>121</v>
       </c>
@@ -2392,7 +2417,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>123</v>
       </c>
@@ -2463,7 +2488,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>125</v>
       </c>
@@ -2534,7 +2559,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>128</v>
       </c>
@@ -2605,7 +2630,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>130</v>
       </c>
@@ -2676,7 +2701,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>132</v>
       </c>
@@ -2747,7 +2772,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>137</v>
       </c>
@@ -2818,7 +2843,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>139</v>
       </c>
@@ -2889,7 +2914,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>141</v>
       </c>
@@ -2960,7 +2985,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>144</v>
       </c>
@@ -3031,7 +3056,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>146</v>
       </c>
@@ -3102,7 +3127,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>148</v>
       </c>
@@ -3173,7 +3198,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>150</v>
       </c>
@@ -3244,7 +3269,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>152</v>
       </c>
@@ -3315,7 +3340,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>154</v>
       </c>
@@ -3386,7 +3411,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>157</v>
       </c>
@@ -3457,7 +3482,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>159</v>
       </c>
@@ -3528,7 +3553,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>161</v>
       </c>
@@ -3599,7 +3624,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>163</v>
       </c>
@@ -3670,7 +3695,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>165</v>
       </c>
@@ -3754,21 +3779,21 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.6640625" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.44140625" customWidth="1"/>
-    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.109375" customWidth="1"/>
-    <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="34.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.140625" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="34.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3800,7 +3825,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>51</v>
       </c>
@@ -3823,7 +3848,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>52</v>
       </c>

</xml_diff>

<commit_message>
Major updates to simulation log and (almost) all scripts
</commit_message>
<xml_diff>
--- a/Simulation_log_key.xlsx
+++ b/Simulation_log_key.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zeus\Documents\R\working_directory\LemonSharkCKMR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\Documents\R\working_directory\LemonSharkCKMR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E66845E-B583-4F24-95BF-EAC85BD375FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14E8A10E-E1EA-4499-A0FD-6AC7CDE88FA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-11640" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5085" yWindow="-11640" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Simulation_log_key" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="194">
   <si>
     <t>Objective</t>
   </si>
@@ -163,9 +163,6 @@
     <t>scenario_4.1</t>
   </si>
   <si>
-    <t>Description</t>
-  </si>
-  <si>
     <t>Scenario 1</t>
   </si>
   <si>
@@ -175,72 +172,9 @@
     <t>Scenario 3</t>
   </si>
   <si>
-    <t>Validate model with informed and diffuse prior for survival</t>
-  </si>
-  <si>
-    <t>obj1</t>
-  </si>
-  <si>
-    <t>obj2.1</t>
-  </si>
-  <si>
-    <t>Compare naïve model vs lambda model w/ population growth and a range of estimation years</t>
-  </si>
-  <si>
-    <t>model validation; informed prior on survival</t>
-  </si>
-  <si>
-    <t>model validation; diffuse prior on survival</t>
-  </si>
-  <si>
-    <t>Scenario 1 relevance</t>
-  </si>
-  <si>
-    <t>Scenario 2 relevance</t>
-  </si>
-  <si>
-    <t>Scenario 3 relevance</t>
-  </si>
-  <si>
-    <t>neutral population growth; no prior on lambda</t>
-  </si>
-  <si>
-    <t>variable population growth; no lambda</t>
-  </si>
-  <si>
-    <t>Scenario 4</t>
-  </si>
-  <si>
-    <t>Scenario 4 relevance</t>
-  </si>
-  <si>
-    <t>scenario2.2.1</t>
-  </si>
-  <si>
-    <t>scenario _2.2.2</t>
-  </si>
-  <si>
-    <t>neutral + variable population growth; lambda prior; estimate year 85</t>
-  </si>
-  <si>
-    <t>neutral + variable population growth; lambda prior; estimate years 80 and 90</t>
-  </si>
-  <si>
-    <t>small variations</t>
-  </si>
-  <si>
-    <t>bigger variations</t>
-  </si>
-  <si>
     <t>scenario_3.1.1</t>
   </si>
   <si>
-    <t>Skipped-breeding (SB) in PopSim; not in model; no lambda in model</t>
-  </si>
-  <si>
-    <t>Skipped-breeding (SB) in PopSim; not in model; lambda in model</t>
-  </si>
-  <si>
     <t>scenario_3.1.2</t>
   </si>
   <si>
@@ -250,12 +184,6 @@
     <t>scenario_3.2.2</t>
   </si>
   <si>
-    <t>SB in PopSim; SB in model; lambda in model</t>
-  </si>
-  <si>
-    <t>SB in PopSim; SB in model; no lambda in model</t>
-  </si>
-  <si>
     <t>Liz's derivation (minus lambda)</t>
   </si>
   <si>
@@ -274,18 +202,12 @@
     <t>Non-conformists</t>
   </si>
   <si>
-    <t>Uniform(0.80, 1.0)</t>
-  </si>
-  <si>
     <t>Uniform(0.80, 1.20)</t>
   </si>
   <si>
     <t>Minimal population growth; estimate abundance in three different years.</t>
   </si>
   <si>
-    <t>More extreme population decline; estimate abundance in three different years; set a lambda prior that reflects knowledge that the population is declining.</t>
-  </si>
-  <si>
     <t>More extreme population decline; estimate abundance in three different years; set a lambda prior that does not assume knowledge about the direction of annual population change.</t>
   </si>
   <si>
@@ -524,6 +446,165 @@
   </si>
   <si>
     <t>Obj2.2.2_lambda.trial_target.YOY_stablePopSimLambda_change.est.yr</t>
+  </si>
+  <si>
+    <t>scenario_4.2</t>
+  </si>
+  <si>
+    <t>scenario_2.3.1</t>
+  </si>
+  <si>
+    <t>scenario_2.3.2</t>
+  </si>
+  <si>
+    <t>scenario_3.3.3</t>
+  </si>
+  <si>
+    <t>Fixed psi</t>
+  </si>
+  <si>
+    <t>scenario_3.3.4</t>
+  </si>
+  <si>
+    <t>Major population decline; no lambda in model</t>
+  </si>
+  <si>
+    <t>Small population change; lambda in model w/ wide prior</t>
+  </si>
+  <si>
+    <t>Small population decline; no lambda in model</t>
+  </si>
+  <si>
+    <t>Major population decline; lambda in model w/ wide prior</t>
+  </si>
+  <si>
+    <t>Small population change; lambda in model w/ tight prior</t>
+  </si>
+  <si>
+    <t>Major population decline; lambda in model w/ tight prior</t>
+  </si>
+  <si>
+    <t>Breeding in model</t>
+  </si>
+  <si>
+    <t>annual</t>
+  </si>
+  <si>
+    <t>biennial</t>
+  </si>
+  <si>
+    <t>small change</t>
+  </si>
+  <si>
+    <t>major decline</t>
+  </si>
+  <si>
+    <t>Biennial breeding; biennial model; no lambda in model; no non-conformists</t>
+  </si>
+  <si>
+    <t>Biennial breeding; biennial model; lambda in model w/ wide prior; no non-conformists</t>
+  </si>
+  <si>
+    <t>Biennial breeding; biennial model; lambda in model w/ wide prior; no non-conformists; psi fixed</t>
+  </si>
+  <si>
+    <t>Biennial breeding; biennial model; lambda in model w/ tight prior; no non-conformists</t>
+  </si>
+  <si>
+    <t>Aging error; biennial breeding; biennial model; lambda in model w/ wide prior; no non-conformists</t>
+  </si>
+  <si>
+    <t>Aging error; biennial breeding; biennial model; lambda in model w/ tight prior; no non-conformists</t>
+  </si>
+  <si>
+    <t>Model validation</t>
+  </si>
+  <si>
+    <t>Scenario 1 justification</t>
+  </si>
+  <si>
+    <t>Scenario 2 justification</t>
+  </si>
+  <si>
+    <t>Scenario 3 justification</t>
+  </si>
+  <si>
+    <t>No lambda</t>
+  </si>
+  <si>
+    <t>Major scenario 1 variable</t>
+  </si>
+  <si>
+    <t>Naïve model</t>
+  </si>
+  <si>
+    <t>Major scenario 2 variable</t>
+  </si>
+  <si>
+    <t>includes lambda with tight prior</t>
+  </si>
+  <si>
+    <t>Major scenario 3 variable</t>
+  </si>
+  <si>
+    <t>Wide prior on lambda</t>
+  </si>
+  <si>
+    <t>Introduce major population decline</t>
+  </si>
+  <si>
+    <t>Introduce small population change</t>
+  </si>
+  <si>
+    <t>include lambda with wide prior</t>
+  </si>
+  <si>
+    <t>Does including a prior on lambda improve parameter estimates?</t>
+  </si>
+  <si>
+    <t>Does the width of the lambda prior matter?</t>
+  </si>
+  <si>
+    <t>Can the model identify significant population declines?</t>
+  </si>
+  <si>
+    <t>Tight prior on lambda</t>
+  </si>
+  <si>
+    <t>What happens if the population declines and the prior on lambda is improperly specified?</t>
+  </si>
+  <si>
+    <t>Introduce biennial breeding; NO non-conformists</t>
+  </si>
+  <si>
+    <t>Annual breeding in model</t>
+  </si>
+  <si>
+    <t>Naïve model; lambda w/ wide prior</t>
+  </si>
+  <si>
+    <t>scenario_</t>
+  </si>
+  <si>
+    <t>scenario_3.1.3</t>
+  </si>
+  <si>
+    <t>Biennial breeding; annual model; no lambda in model; no non-conformists</t>
+  </si>
+  <si>
+    <t>Biennial breeding; annual model; lambda in model w/ wide prior; no non-conformists</t>
+  </si>
+  <si>
+    <t>Biennial breeding; annual model; lambda in model w/ tight prior; no non-conformists</t>
+  </si>
+  <si>
+    <t>scenario_3.2.3</t>
+  </si>
+  <si>
+    <t>scenario_4.3</t>
+  </si>
+  <si>
+    <t>Aging error; biennial breeding; biennial model; no lambda in model; no non-conformists</t>
   </si>
 </sst>
 </file>
@@ -1013,7 +1094,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1024,6 +1105,8 @@
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1379,26 +1462,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J30"/>
+  <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="62.5703125" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="16.5703125" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="43.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="72.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="86.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" customWidth="1"/>
+    <col min="4" max="4" width="27.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5546875" customWidth="1"/>
+    <col min="6" max="6" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="43.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="72.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>36</v>
       </c>
@@ -1406,13 +1491,13 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D1" t="s">
-        <v>14</v>
+        <v>153</v>
       </c>
       <c r="E1" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
@@ -1427,21 +1512,24 @@
         <v>24</v>
       </c>
       <c r="J1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>37</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2">
+      <c r="C2">
         <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>154</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -1458,22 +1546,25 @@
       <c r="I2" t="s">
         <v>25</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>38</v>
       </c>
       <c r="B3" t="s">
         <v>31</v>
       </c>
-      <c r="C3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3">
+      <c r="C3">
         <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>154</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -1490,28 +1581,31 @@
       <c r="I3" t="s">
         <v>25</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>78</v>
+        <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4">
+        <v>149</v>
+      </c>
+      <c r="C4">
         <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>154</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>67</v>
+        <v>156</v>
       </c>
       <c r="G4" t="s">
         <v>15</v>
@@ -1522,28 +1616,31 @@
       <c r="I4" t="s">
         <v>25</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="J4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>79</v>
+        <v>55</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5">
+        <v>147</v>
+      </c>
+      <c r="C5">
         <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>154</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5" t="s">
-        <v>68</v>
+        <v>157</v>
       </c>
       <c r="G5" t="s">
         <v>15</v>
@@ -1554,31 +1651,34 @@
       <c r="I5" t="s">
         <v>25</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="J5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K5" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>40</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6">
+        <v>148</v>
+      </c>
+      <c r="C6">
         <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>154</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>67</v>
+        <v>156</v>
       </c>
       <c r="G6" t="s">
-        <v>18</v>
+        <v>59</v>
       </c>
       <c r="H6" t="s">
         <v>19</v>
@@ -1586,31 +1686,34 @@
       <c r="I6" t="s">
         <v>26</v>
       </c>
-      <c r="J6" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="J6" t="s">
+        <v>17</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>41</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7">
+        <v>150</v>
+      </c>
+      <c r="C7">
         <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>154</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
       <c r="F7" t="s">
-        <v>68</v>
+        <v>157</v>
       </c>
       <c r="G7" t="s">
-        <v>83</v>
+        <v>59</v>
       </c>
       <c r="H7" t="s">
         <v>19</v>
@@ -1618,242 +1721,510 @@
       <c r="I7" t="s">
         <v>26</v>
       </c>
-      <c r="J7" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="J7" t="s">
+        <v>17</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>142</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8">
+        <v>151</v>
+      </c>
+      <c r="C8">
         <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>154</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
       <c r="F8" t="s">
-        <v>68</v>
+        <v>156</v>
       </c>
       <c r="G8" t="s">
-        <v>84</v>
-      </c>
-      <c r="H8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J8" t="s">
+        <v>17</v>
+      </c>
+      <c r="K8" s="1"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>143</v>
+      </c>
+      <c r="B9" t="s">
+        <v>152</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>154</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9" t="s">
+        <v>157</v>
+      </c>
+      <c r="G9" t="s">
+        <v>18</v>
+      </c>
+      <c r="J9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K9" s="1"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="C10" s="6">
+        <v>2</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="E10" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="F10" s="6">
+        <v>1</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I10" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="K10" s="6"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="C11" s="6">
+        <v>2</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="E11" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="F11" s="6">
+        <v>1</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="I11" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="J8" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>69</v>
-      </c>
-      <c r="B9" t="s">
-        <v>70</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="J11" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D9">
+      <c r="K11" s="6"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="C12" s="6">
         <v>2</v>
       </c>
-      <c r="E9" s="4">
+      <c r="D12" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="E12" s="7">
         <v>0.05</v>
       </c>
-      <c r="F9">
+      <c r="F12" s="6">
         <v>1</v>
       </c>
-      <c r="G9" t="s">
-        <v>15</v>
-      </c>
-      <c r="H9" t="s">
+      <c r="G12" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="H12" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="I9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>72</v>
-      </c>
-      <c r="B10" t="s">
-        <v>71</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="I12" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="J12" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D10">
+      <c r="K12" s="6"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="C13" s="6">
         <v>2</v>
       </c>
-      <c r="E10" s="4">
+      <c r="D13" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="E13" s="7">
         <v>0.05</v>
       </c>
-      <c r="F10">
+      <c r="F13" s="6">
         <v>1</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G13" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="K13" s="6"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="C14" s="6">
+        <v>2</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="E14" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="F14" s="6">
+        <v>1</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="K14" s="6"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="C15" s="6">
+        <v>2</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="E15" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="F15" s="6">
+        <v>1</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="J15" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="K15" s="6"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" t="s">
+        <v>158</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16" t="s">
+        <v>155</v>
+      </c>
+      <c r="E16" s="4">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16" t="s">
+        <v>15</v>
+      </c>
+      <c r="H16" t="s">
+        <v>19</v>
+      </c>
+      <c r="I16" t="s">
+        <v>53</v>
+      </c>
+      <c r="J16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" t="s">
+        <v>159</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17" t="s">
+        <v>155</v>
+      </c>
+      <c r="E17" s="4">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17" t="s">
+        <v>59</v>
+      </c>
+      <c r="H17" t="s">
+        <v>19</v>
+      </c>
+      <c r="I17" t="s">
+        <v>27</v>
+      </c>
+      <c r="J17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>144</v>
+      </c>
+      <c r="B18" t="s">
+        <v>160</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18" t="s">
+        <v>155</v>
+      </c>
+      <c r="E18" s="4">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18" t="s">
+        <v>59</v>
+      </c>
+      <c r="H18" t="s">
+        <v>19</v>
+      </c>
+      <c r="I18" t="s">
+        <v>27</v>
+      </c>
+      <c r="J18" t="s">
+        <v>17</v>
+      </c>
+      <c r="K18" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>146</v>
+      </c>
+      <c r="B19" t="s">
+        <v>161</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19" t="s">
+        <v>155</v>
+      </c>
+      <c r="E19" s="4">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19" t="s">
         <v>18</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H19" t="s">
         <v>19</v>
       </c>
-      <c r="I10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>73</v>
-      </c>
-      <c r="B11" t="s">
-        <v>76</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="I19" t="s">
+        <v>27</v>
+      </c>
+      <c r="J19" t="s">
         <v>17</v>
       </c>
-      <c r="D11">
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" t="s">
+        <v>162</v>
+      </c>
+      <c r="C20">
         <v>2</v>
       </c>
-      <c r="E11" s="4">
-        <v>0.05</v>
-      </c>
-      <c r="F11">
+      <c r="D20" t="s">
+        <v>155</v>
+      </c>
+      <c r="E20" s="4">
+        <v>0</v>
+      </c>
+      <c r="F20">
         <v>1</v>
       </c>
-      <c r="G11" t="s">
-        <v>15</v>
-      </c>
-      <c r="H11" t="s">
+      <c r="G20" t="s">
+        <v>59</v>
+      </c>
+      <c r="H20" t="s">
         <v>19</v>
       </c>
-      <c r="I11" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>74</v>
-      </c>
-      <c r="B12" t="s">
-        <v>75</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="I20" t="s">
+        <v>27</v>
+      </c>
+      <c r="J20" t="s">
         <v>17</v>
       </c>
-      <c r="D12">
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>141</v>
+      </c>
+      <c r="B21" t="s">
+        <v>163</v>
+      </c>
+      <c r="C21">
         <v>2</v>
       </c>
-      <c r="E12" s="4">
-        <v>0.05</v>
-      </c>
-      <c r="F12">
+      <c r="D21" t="s">
+        <v>155</v>
+      </c>
+      <c r="E21" s="4">
+        <v>0</v>
+      </c>
+      <c r="F21">
         <v>1</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G21" t="s">
         <v>18</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H21" t="s">
         <v>19</v>
       </c>
-      <c r="I12" t="s">
+      <c r="I21" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>80</v>
-      </c>
-      <c r="B13" t="s">
-        <v>76</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="J21" t="s">
         <v>17</v>
       </c>
-      <c r="D13">
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>192</v>
+      </c>
+      <c r="B22" t="s">
+        <v>193</v>
+      </c>
+      <c r="C22">
         <v>2</v>
       </c>
-      <c r="E13" s="4">
+      <c r="D22" t="s">
+        <v>155</v>
+      </c>
+      <c r="E22" s="4">
         <v>0</v>
       </c>
-      <c r="F13">
+      <c r="F22">
         <v>1</v>
       </c>
-      <c r="G13" t="s">
-        <v>15</v>
-      </c>
-      <c r="H13" t="s">
+      <c r="G22" t="s">
+        <v>15</v>
+      </c>
+      <c r="H22" t="s">
         <v>19</v>
       </c>
-      <c r="I13" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B14" t="s">
-        <v>75</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="I22" t="s">
+        <v>27</v>
+      </c>
+      <c r="J22" t="s">
         <v>17</v>
       </c>
-      <c r="D14">
-        <v>2</v>
-      </c>
-      <c r="E14" s="4">
-        <v>0</v>
-      </c>
-      <c r="F14">
-        <v>1</v>
-      </c>
-      <c r="G14" t="s">
-        <v>18</v>
-      </c>
-      <c r="H14" t="s">
-        <v>19</v>
-      </c>
-      <c r="I14" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>45</v>
-      </c>
-      <c r="B15" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
         <v>10</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B34" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
         <v>12</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B35" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1870,20 +2241,20 @@
       <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.5703125" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="43.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="72.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.5546875" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="43.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="72.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>36</v>
       </c>
@@ -1912,7 +2283,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -1941,7 +2312,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -1970,7 +2341,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -1999,7 +2370,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>40</v>
       </c>
@@ -2025,7 +2396,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>41</v>
       </c>
@@ -2054,7 +2425,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>42</v>
       </c>
@@ -2083,7 +2454,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>43</v>
       </c>
@@ -2109,7 +2480,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>44</v>
       </c>
@@ -2135,7 +2506,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>45</v>
       </c>
@@ -2143,12 +2514,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>10</v>
       </c>
@@ -2156,7 +2527,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>12</v>
       </c>
@@ -2177,131 +2548,131 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="79.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="98.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="62.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="79.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="98.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="62.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="69" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="77.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="77.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="8" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.88671875" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="17" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="41.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="41.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1" t="s">
+        <v>71</v>
+      </c>
+      <c r="K1" t="s">
+        <v>72</v>
+      </c>
+      <c r="L1" t="s">
+        <v>73</v>
+      </c>
+      <c r="M1" t="s">
+        <v>74</v>
+      </c>
+      <c r="N1" t="s">
+        <v>75</v>
+      </c>
+      <c r="O1" t="s">
+        <v>76</v>
+      </c>
+      <c r="P1" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>78</v>
+      </c>
+      <c r="R1" t="s">
+        <v>79</v>
+      </c>
+      <c r="S1" t="s">
+        <v>80</v>
+      </c>
+      <c r="T1" t="s">
+        <v>81</v>
+      </c>
+      <c r="U1" t="s">
+        <v>82</v>
+      </c>
+      <c r="V1" t="s">
+        <v>83</v>
+      </c>
+      <c r="W1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
         <v>88</v>
-      </c>
-      <c r="B1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C1" t="s">
-        <v>90</v>
-      </c>
-      <c r="D1" t="s">
-        <v>91</v>
-      </c>
-      <c r="E1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F1" t="s">
-        <v>93</v>
-      </c>
-      <c r="G1" t="s">
-        <v>94</v>
-      </c>
-      <c r="H1" t="s">
-        <v>95</v>
-      </c>
-      <c r="I1" t="s">
-        <v>96</v>
-      </c>
-      <c r="J1" t="s">
-        <v>97</v>
-      </c>
-      <c r="K1" t="s">
-        <v>98</v>
-      </c>
-      <c r="L1" t="s">
-        <v>99</v>
-      </c>
-      <c r="M1" t="s">
-        <v>100</v>
-      </c>
-      <c r="N1" t="s">
-        <v>101</v>
-      </c>
-      <c r="O1" t="s">
-        <v>102</v>
-      </c>
-      <c r="P1" t="s">
-        <v>103</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>104</v>
-      </c>
-      <c r="R1" t="s">
-        <v>105</v>
-      </c>
-      <c r="S1" t="s">
-        <v>106</v>
-      </c>
-      <c r="T1" t="s">
-        <v>107</v>
-      </c>
-      <c r="U1" t="s">
-        <v>108</v>
-      </c>
-      <c r="V1" t="s">
-        <v>109</v>
-      </c>
-      <c r="W1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>111</v>
-      </c>
-      <c r="B2" t="s">
-        <v>112</v>
-      </c>
-      <c r="C2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" t="s">
-        <v>114</v>
       </c>
       <c r="G2" s="5">
         <v>44754</v>
       </c>
       <c r="H2" t="s">
-        <v>115</v>
+        <v>89</v>
       </c>
       <c r="I2" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="J2" t="s">
         <v>15</v>
@@ -2310,19 +2681,19 @@
         <v>15</v>
       </c>
       <c r="L2" t="s">
-        <v>115</v>
+        <v>89</v>
       </c>
       <c r="M2" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="N2" t="s">
-        <v>117</v>
+        <v>91</v>
       </c>
       <c r="O2" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="P2" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="Q2">
         <v>20</v>
@@ -2343,18 +2714,18 @@
         <v>15</v>
       </c>
       <c r="W2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>121</v>
+        <v>95</v>
       </c>
       <c r="B3" t="s">
-        <v>112</v>
+        <v>86</v>
       </c>
       <c r="C3" t="s">
-        <v>113</v>
+        <v>87</v>
       </c>
       <c r="D3" t="s">
         <v>15</v>
@@ -2363,16 +2734,16 @@
         <v>15</v>
       </c>
       <c r="F3" t="s">
-        <v>122</v>
+        <v>96</v>
       </c>
       <c r="G3" s="5">
         <v>44754</v>
       </c>
       <c r="H3" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="I3" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="J3" t="s">
         <v>15</v>
@@ -2381,19 +2752,19 @@
         <v>15</v>
       </c>
       <c r="L3" t="s">
-        <v>115</v>
+        <v>89</v>
       </c>
       <c r="M3" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="N3" t="s">
-        <v>117</v>
+        <v>91</v>
       </c>
       <c r="O3" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="P3" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="Q3">
         <v>20</v>
@@ -2414,18 +2785,18 @@
         <v>15</v>
       </c>
       <c r="W3" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>123</v>
+        <v>97</v>
       </c>
       <c r="B4" t="s">
-        <v>112</v>
+        <v>86</v>
       </c>
       <c r="C4" t="s">
-        <v>113</v>
+        <v>87</v>
       </c>
       <c r="D4" t="s">
         <v>15</v>
@@ -2434,16 +2805,16 @@
         <v>15</v>
       </c>
       <c r="F4" t="s">
-        <v>124</v>
+        <v>98</v>
       </c>
       <c r="G4" s="5">
         <v>44755</v>
       </c>
       <c r="H4" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="I4" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="J4" t="s">
         <v>15</v>
@@ -2452,19 +2823,19 @@
         <v>15</v>
       </c>
       <c r="L4" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="M4" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="N4" t="s">
-        <v>117</v>
+        <v>91</v>
       </c>
       <c r="O4" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="P4" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="Q4">
         <v>20</v>
@@ -2485,18 +2856,18 @@
         <v>15</v>
       </c>
       <c r="W4" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>125</v>
+        <v>99</v>
       </c>
       <c r="B5" t="s">
-        <v>112</v>
+        <v>86</v>
       </c>
       <c r="C5" t="s">
-        <v>126</v>
+        <v>100</v>
       </c>
       <c r="D5" t="s">
         <v>15</v>
@@ -2505,16 +2876,16 @@
         <v>15</v>
       </c>
       <c r="F5" t="s">
-        <v>127</v>
+        <v>101</v>
       </c>
       <c r="G5" s="5">
         <v>44755</v>
       </c>
       <c r="H5" t="s">
-        <v>115</v>
+        <v>89</v>
       </c>
       <c r="I5" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="J5" t="s">
         <v>15</v>
@@ -2523,19 +2894,19 @@
         <v>15</v>
       </c>
       <c r="L5" t="s">
-        <v>115</v>
+        <v>89</v>
       </c>
       <c r="M5" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="N5" t="s">
-        <v>117</v>
+        <v>91</v>
       </c>
       <c r="O5" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="P5" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="Q5">
         <v>20</v>
@@ -2556,18 +2927,18 @@
         <v>15</v>
       </c>
       <c r="W5" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="B6" t="s">
-        <v>112</v>
+        <v>86</v>
       </c>
       <c r="C6" t="s">
-        <v>126</v>
+        <v>100</v>
       </c>
       <c r="D6" t="s">
         <v>15</v>
@@ -2576,16 +2947,16 @@
         <v>15</v>
       </c>
       <c r="F6" t="s">
-        <v>129</v>
+        <v>103</v>
       </c>
       <c r="G6" s="5">
         <v>44755</v>
       </c>
       <c r="H6" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="I6" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="J6" t="s">
         <v>15</v>
@@ -2594,19 +2965,19 @@
         <v>15</v>
       </c>
       <c r="L6" t="s">
-        <v>115</v>
+        <v>89</v>
       </c>
       <c r="M6" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="N6" t="s">
-        <v>117</v>
+        <v>91</v>
       </c>
       <c r="O6" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="P6" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="Q6">
         <v>20</v>
@@ -2627,18 +2998,18 @@
         <v>15</v>
       </c>
       <c r="W6" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>130</v>
+        <v>104</v>
       </c>
       <c r="B7" t="s">
-        <v>112</v>
+        <v>86</v>
       </c>
       <c r="C7" t="s">
-        <v>126</v>
+        <v>100</v>
       </c>
       <c r="D7" t="s">
         <v>15</v>
@@ -2647,16 +3018,16 @@
         <v>15</v>
       </c>
       <c r="F7" t="s">
-        <v>131</v>
+        <v>105</v>
       </c>
       <c r="G7" s="5">
         <v>44755</v>
       </c>
       <c r="H7" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="I7" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="J7" t="s">
         <v>15</v>
@@ -2665,19 +3036,19 @@
         <v>15</v>
       </c>
       <c r="L7" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="M7" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="N7" t="s">
-        <v>117</v>
+        <v>91</v>
       </c>
       <c r="O7" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="P7" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="Q7">
         <v>20</v>
@@ -2698,36 +3069,36 @@
         <v>15</v>
       </c>
       <c r="W7" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>132</v>
+        <v>106</v>
       </c>
       <c r="B8" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="C8" t="s">
-        <v>134</v>
+        <v>108</v>
       </c>
       <c r="D8" t="s">
-        <v>135</v>
+        <v>109</v>
       </c>
       <c r="E8" t="s">
         <v>15</v>
       </c>
       <c r="F8" t="s">
-        <v>136</v>
+        <v>110</v>
       </c>
       <c r="G8" s="5">
         <v>44755</v>
       </c>
       <c r="H8" t="s">
-        <v>115</v>
+        <v>89</v>
       </c>
       <c r="I8" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="J8" t="s">
         <v>15</v>
@@ -2736,19 +3107,19 @@
         <v>15</v>
       </c>
       <c r="L8" t="s">
-        <v>115</v>
+        <v>89</v>
       </c>
       <c r="M8" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="N8" t="s">
-        <v>117</v>
+        <v>91</v>
       </c>
       <c r="O8" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="P8" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="Q8">
         <v>20</v>
@@ -2769,36 +3140,36 @@
         <v>15</v>
       </c>
       <c r="W8" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>137</v>
+        <v>111</v>
       </c>
       <c r="B9" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="C9" t="s">
-        <v>134</v>
+        <v>108</v>
       </c>
       <c r="D9" t="s">
-        <v>135</v>
+        <v>109</v>
       </c>
       <c r="E9" t="s">
         <v>15</v>
       </c>
       <c r="F9" t="s">
-        <v>138</v>
+        <v>112</v>
       </c>
       <c r="G9" s="5">
         <v>44755</v>
       </c>
       <c r="H9" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="I9" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="J9" t="s">
         <v>15</v>
@@ -2807,19 +3178,19 @@
         <v>15</v>
       </c>
       <c r="L9" t="s">
-        <v>115</v>
+        <v>89</v>
       </c>
       <c r="M9" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="N9" t="s">
-        <v>117</v>
+        <v>91</v>
       </c>
       <c r="O9" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="P9" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="Q9">
         <v>20</v>
@@ -2840,36 +3211,36 @@
         <v>15</v>
       </c>
       <c r="W9" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>139</v>
+        <v>113</v>
       </c>
       <c r="B10" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="C10" t="s">
-        <v>134</v>
+        <v>108</v>
       </c>
       <c r="D10" t="s">
-        <v>135</v>
+        <v>109</v>
       </c>
       <c r="E10" t="s">
         <v>15</v>
       </c>
       <c r="F10" t="s">
-        <v>140</v>
+        <v>114</v>
       </c>
       <c r="G10" s="5">
         <v>44755</v>
       </c>
       <c r="H10" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="I10" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="J10" t="s">
         <v>15</v>
@@ -2878,19 +3249,19 @@
         <v>15</v>
       </c>
       <c r="L10" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="M10" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="N10" t="s">
-        <v>117</v>
+        <v>91</v>
       </c>
       <c r="O10" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="P10" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="Q10">
         <v>20</v>
@@ -2911,36 +3282,36 @@
         <v>15</v>
       </c>
       <c r="W10" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>141</v>
+        <v>115</v>
       </c>
       <c r="B11" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="C11" t="s">
-        <v>134</v>
+        <v>108</v>
       </c>
       <c r="D11" t="s">
-        <v>135</v>
+        <v>109</v>
       </c>
       <c r="E11" t="s">
         <v>15</v>
       </c>
       <c r="F11" t="s">
-        <v>142</v>
+        <v>116</v>
       </c>
       <c r="G11" s="5">
         <v>44755</v>
       </c>
       <c r="H11" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="I11" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="J11" t="s">
         <v>15</v>
@@ -2949,19 +3320,19 @@
         <v>15</v>
       </c>
       <c r="L11" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="M11" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="N11" t="s">
+        <v>91</v>
+      </c>
+      <c r="O11" t="s">
         <v>117</v>
       </c>
-      <c r="O11" t="s">
-        <v>143</v>
-      </c>
       <c r="P11" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="Q11">
         <v>20</v>
@@ -2982,36 +3353,36 @@
         <v>15</v>
       </c>
       <c r="W11" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>144</v>
+        <v>118</v>
       </c>
       <c r="B12" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="C12" t="s">
-        <v>134</v>
+        <v>108</v>
       </c>
       <c r="D12" t="s">
-        <v>135</v>
+        <v>109</v>
       </c>
       <c r="E12" t="s">
         <v>15</v>
       </c>
       <c r="F12" t="s">
-        <v>145</v>
+        <v>119</v>
       </c>
       <c r="G12" s="5">
         <v>44755</v>
       </c>
       <c r="H12" t="s">
-        <v>115</v>
+        <v>89</v>
       </c>
       <c r="I12" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="J12" t="s">
         <v>15</v>
@@ -3020,19 +3391,19 @@
         <v>15</v>
       </c>
       <c r="L12" t="s">
-        <v>115</v>
+        <v>89</v>
       </c>
       <c r="M12" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="N12" t="s">
+        <v>91</v>
+      </c>
+      <c r="O12" t="s">
         <v>117</v>
       </c>
-      <c r="O12" t="s">
-        <v>143</v>
-      </c>
       <c r="P12" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="Q12">
         <v>20</v>
@@ -3053,36 +3424,36 @@
         <v>15</v>
       </c>
       <c r="W12" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>146</v>
-      </c>
       <c r="B13" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="C13" t="s">
-        <v>134</v>
+        <v>108</v>
       </c>
       <c r="D13" t="s">
-        <v>135</v>
+        <v>109</v>
       </c>
       <c r="E13" t="s">
         <v>15</v>
       </c>
       <c r="F13" t="s">
-        <v>147</v>
+        <v>121</v>
       </c>
       <c r="G13" s="5">
         <v>44755</v>
       </c>
       <c r="H13" t="s">
-        <v>115</v>
+        <v>89</v>
       </c>
       <c r="I13" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="J13" t="s">
         <v>15</v>
@@ -3091,19 +3462,19 @@
         <v>15</v>
       </c>
       <c r="L13" t="s">
-        <v>115</v>
+        <v>89</v>
       </c>
       <c r="M13" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="N13" t="s">
+        <v>91</v>
+      </c>
+      <c r="O13" t="s">
         <v>117</v>
       </c>
-      <c r="O13" t="s">
-        <v>143</v>
-      </c>
       <c r="P13" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="Q13">
         <v>20</v>
@@ -3124,36 +3495,36 @@
         <v>15</v>
       </c>
       <c r="W13" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>148</v>
+        <v>122</v>
       </c>
       <c r="B14" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="C14" t="s">
-        <v>134</v>
+        <v>108</v>
       </c>
       <c r="D14" t="s">
-        <v>135</v>
+        <v>109</v>
       </c>
       <c r="E14" t="s">
         <v>15</v>
       </c>
       <c r="F14" t="s">
-        <v>149</v>
+        <v>123</v>
       </c>
       <c r="G14" s="5">
         <v>44755</v>
       </c>
       <c r="H14" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="I14" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="J14" t="s">
         <v>15</v>
@@ -3162,19 +3533,19 @@
         <v>15</v>
       </c>
       <c r="L14" t="s">
-        <v>115</v>
+        <v>89</v>
       </c>
       <c r="M14" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="N14" t="s">
+        <v>91</v>
+      </c>
+      <c r="O14" t="s">
         <v>117</v>
       </c>
-      <c r="O14" t="s">
-        <v>143</v>
-      </c>
       <c r="P14" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="Q14">
         <v>20</v>
@@ -3195,36 +3566,36 @@
         <v>15</v>
       </c>
       <c r="W14" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>150</v>
+        <v>124</v>
       </c>
       <c r="B15" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="C15" t="s">
-        <v>134</v>
+        <v>108</v>
       </c>
       <c r="D15" t="s">
-        <v>135</v>
+        <v>109</v>
       </c>
       <c r="E15" t="s">
         <v>15</v>
       </c>
       <c r="F15" t="s">
-        <v>151</v>
+        <v>125</v>
       </c>
       <c r="G15" s="5">
         <v>44755</v>
       </c>
       <c r="H15" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="I15" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="J15" t="s">
         <v>15</v>
@@ -3233,19 +3604,19 @@
         <v>15</v>
       </c>
       <c r="L15" t="s">
-        <v>115</v>
+        <v>89</v>
       </c>
       <c r="M15" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="N15" t="s">
+        <v>91</v>
+      </c>
+      <c r="O15" t="s">
         <v>117</v>
       </c>
-      <c r="O15" t="s">
-        <v>143</v>
-      </c>
       <c r="P15" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="Q15">
         <v>20</v>
@@ -3266,36 +3637,36 @@
         <v>15</v>
       </c>
       <c r="W15" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>152</v>
+        <v>126</v>
       </c>
       <c r="B16" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="C16" t="s">
-        <v>134</v>
+        <v>108</v>
       </c>
       <c r="D16" t="s">
-        <v>135</v>
+        <v>109</v>
       </c>
       <c r="E16" t="s">
         <v>15</v>
       </c>
       <c r="F16" t="s">
-        <v>153</v>
+        <v>127</v>
       </c>
       <c r="G16" s="5">
         <v>44755</v>
       </c>
       <c r="H16" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="I16" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="J16" t="s">
         <v>15</v>
@@ -3304,19 +3675,19 @@
         <v>15</v>
       </c>
       <c r="L16" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="M16" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="N16" t="s">
+        <v>91</v>
+      </c>
+      <c r="O16" t="s">
         <v>117</v>
       </c>
-      <c r="O16" t="s">
-        <v>143</v>
-      </c>
       <c r="P16" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="Q16">
         <v>20</v>
@@ -3337,36 +3708,36 @@
         <v>15</v>
       </c>
       <c r="W16" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>154</v>
+        <v>128</v>
       </c>
       <c r="B17" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="C17" t="s">
-        <v>134</v>
+        <v>108</v>
       </c>
       <c r="D17" t="s">
-        <v>135</v>
+        <v>109</v>
       </c>
       <c r="E17" t="s">
-        <v>155</v>
+        <v>129</v>
       </c>
       <c r="F17" t="s">
-        <v>156</v>
+        <v>130</v>
       </c>
       <c r="G17" s="5">
         <v>44756</v>
       </c>
       <c r="H17" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="I17" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="J17" t="s">
         <v>15</v>
@@ -3375,19 +3746,19 @@
         <v>15</v>
       </c>
       <c r="L17" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="M17" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="N17" t="s">
+        <v>91</v>
+      </c>
+      <c r="O17" t="s">
         <v>117</v>
       </c>
-      <c r="O17" t="s">
-        <v>143</v>
-      </c>
       <c r="P17" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="Q17">
         <v>20</v>
@@ -3408,36 +3779,36 @@
         <v>15</v>
       </c>
       <c r="W17" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>157</v>
+        <v>131</v>
       </c>
       <c r="B18" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="C18" t="s">
-        <v>134</v>
+        <v>108</v>
       </c>
       <c r="D18" t="s">
-        <v>135</v>
+        <v>109</v>
       </c>
       <c r="E18" t="s">
-        <v>155</v>
+        <v>129</v>
       </c>
       <c r="F18" t="s">
-        <v>158</v>
+        <v>132</v>
       </c>
       <c r="G18" s="5">
         <v>44756</v>
       </c>
       <c r="H18" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="I18" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="J18" t="s">
         <v>15</v>
@@ -3446,19 +3817,19 @@
         <v>15</v>
       </c>
       <c r="L18" t="s">
-        <v>115</v>
+        <v>89</v>
       </c>
       <c r="M18" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="N18" t="s">
+        <v>91</v>
+      </c>
+      <c r="O18" t="s">
         <v>117</v>
       </c>
-      <c r="O18" t="s">
-        <v>143</v>
-      </c>
       <c r="P18" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="Q18">
         <v>20</v>
@@ -3479,36 +3850,36 @@
         <v>15</v>
       </c>
       <c r="W18" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>159</v>
+        <v>133</v>
       </c>
       <c r="B19" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="C19" t="s">
+        <v>108</v>
+      </c>
+      <c r="D19" t="s">
+        <v>109</v>
+      </c>
+      <c r="E19" t="s">
+        <v>129</v>
+      </c>
+      <c r="F19" t="s">
         <v>134</v>
-      </c>
-      <c r="D19" t="s">
-        <v>135</v>
-      </c>
-      <c r="E19" t="s">
-        <v>155</v>
-      </c>
-      <c r="F19" t="s">
-        <v>160</v>
       </c>
       <c r="G19" s="5">
         <v>44756</v>
       </c>
       <c r="H19" t="s">
-        <v>115</v>
+        <v>89</v>
       </c>
       <c r="I19" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="J19" t="s">
         <v>15</v>
@@ -3517,19 +3888,19 @@
         <v>15</v>
       </c>
       <c r="L19" t="s">
-        <v>115</v>
+        <v>89</v>
       </c>
       <c r="M19" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="N19" t="s">
+        <v>91</v>
+      </c>
+      <c r="O19" t="s">
         <v>117</v>
       </c>
-      <c r="O19" t="s">
-        <v>143</v>
-      </c>
       <c r="P19" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="Q19">
         <v>20</v>
@@ -3550,36 +3921,36 @@
         <v>15</v>
       </c>
       <c r="W19" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>161</v>
+        <v>135</v>
       </c>
       <c r="B20" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="C20" t="s">
-        <v>134</v>
+        <v>108</v>
       </c>
       <c r="D20" t="s">
-        <v>135</v>
+        <v>109</v>
       </c>
       <c r="E20" t="s">
-        <v>155</v>
+        <v>129</v>
       </c>
       <c r="F20" t="s">
-        <v>162</v>
+        <v>136</v>
       </c>
       <c r="G20" s="5">
         <v>44757</v>
       </c>
       <c r="H20" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="I20" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="J20" t="s">
         <v>15</v>
@@ -3588,19 +3959,19 @@
         <v>15</v>
       </c>
       <c r="L20" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="M20" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="N20" t="s">
+        <v>91</v>
+      </c>
+      <c r="O20" t="s">
         <v>117</v>
       </c>
-      <c r="O20" t="s">
-        <v>143</v>
-      </c>
       <c r="P20" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="Q20">
         <v>20</v>
@@ -3621,36 +3992,36 @@
         <v>15</v>
       </c>
       <c r="W20" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>163</v>
+        <v>137</v>
       </c>
       <c r="B21" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="C21" t="s">
-        <v>134</v>
+        <v>108</v>
       </c>
       <c r="D21" t="s">
-        <v>135</v>
+        <v>109</v>
       </c>
       <c r="E21" t="s">
-        <v>155</v>
+        <v>129</v>
       </c>
       <c r="F21" t="s">
-        <v>164</v>
+        <v>138</v>
       </c>
       <c r="G21" s="5">
         <v>44757</v>
       </c>
       <c r="H21" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="I21" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="J21" t="s">
         <v>15</v>
@@ -3659,19 +4030,19 @@
         <v>15</v>
       </c>
       <c r="L21" t="s">
-        <v>115</v>
+        <v>89</v>
       </c>
       <c r="M21" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="N21" t="s">
+        <v>91</v>
+      </c>
+      <c r="O21" t="s">
         <v>117</v>
       </c>
-      <c r="O21" t="s">
-        <v>143</v>
-      </c>
       <c r="P21" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="Q21">
         <v>20</v>
@@ -3692,36 +4063,36 @@
         <v>15</v>
       </c>
       <c r="W21" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>165</v>
+        <v>139</v>
       </c>
       <c r="B22" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="C22" t="s">
-        <v>134</v>
+        <v>108</v>
       </c>
       <c r="D22" t="s">
-        <v>135</v>
+        <v>109</v>
       </c>
       <c r="E22" t="s">
-        <v>155</v>
+        <v>129</v>
       </c>
       <c r="F22" t="s">
-        <v>166</v>
+        <v>140</v>
       </c>
       <c r="G22" s="5">
         <v>44757</v>
       </c>
       <c r="H22" t="s">
-        <v>115</v>
+        <v>89</v>
       </c>
       <c r="I22" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="J22" t="s">
         <v>15</v>
@@ -3730,19 +4101,19 @@
         <v>15</v>
       </c>
       <c r="L22" t="s">
-        <v>115</v>
+        <v>89</v>
       </c>
       <c r="M22" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="N22" t="s">
+        <v>91</v>
+      </c>
+      <c r="O22" t="s">
         <v>117</v>
       </c>
-      <c r="O22" t="s">
-        <v>143</v>
-      </c>
       <c r="P22" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="Q22">
         <v>20</v>
@@ -3763,7 +4134,7 @@
         <v>15</v>
       </c>
       <c r="W22" t="s">
-        <v>120</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -3773,27 +4144,29 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{412D6C35-5CAD-470C-B537-E441B956C3CF}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:O109"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.7109375" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.140625" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="52.6640625" customWidth="1"/>
+    <col min="2" max="2" width="47.6640625" customWidth="1"/>
+    <col min="3" max="3" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="47.6640625" customWidth="1"/>
+    <col min="5" max="5" width="26.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="26.77734375" customWidth="1"/>
+    <col min="8" max="8" width="26.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.77734375" customWidth="1"/>
+    <col min="10" max="12" width="26.77734375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="26.109375" customWidth="1"/>
+    <col min="14" max="14" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="34.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3801,84 +4174,1381 @@
         <v>46</v>
       </c>
       <c r="C1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D1" t="s">
+        <v>165</v>
+      </c>
+      <c r="E1" t="s">
         <v>47</v>
       </c>
-      <c r="D1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>171</v>
+      </c>
+      <c r="G1" t="s">
+        <v>166</v>
+      </c>
+      <c r="H1" t="s">
         <v>48</v>
       </c>
-      <c r="F1" t="s">
-        <v>57</v>
-      </c>
-      <c r="G1" t="s">
-        <v>49</v>
-      </c>
-      <c r="H1" t="s">
-        <v>58</v>
-      </c>
       <c r="I1" t="s">
-        <v>61</v>
+        <v>173</v>
       </c>
       <c r="J1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="C3" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="M3" s="1"/>
+      <c r="O3" s="1"/>
+    </row>
+    <row r="4" spans="1:15" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="G2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F3" t="s">
-        <v>60</v>
-      </c>
-      <c r="G3" t="s">
-        <v>63</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="I3" t="s">
-        <v>64</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>66</v>
-      </c>
+      <c r="C4" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+      <c r="J39" s="1"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+      <c r="J40" s="1"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A41" s="1"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A42" s="1"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
+      <c r="I42" s="1"/>
+      <c r="J42" s="1"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A43" s="1"/>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+      <c r="H43" s="1"/>
+      <c r="I43" s="1"/>
+      <c r="J43" s="1"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A44" s="1"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+      <c r="H44" s="1"/>
+      <c r="I44" s="1"/>
+      <c r="J44" s="1"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A45" s="1"/>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+      <c r="H45" s="1"/>
+      <c r="I45" s="1"/>
+      <c r="J45" s="1"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A46" s="1"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
+      <c r="H46" s="1"/>
+      <c r="I46" s="1"/>
+      <c r="J46" s="1"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
+      <c r="H47" s="1"/>
+      <c r="I47" s="1"/>
+      <c r="J47" s="1"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A48" s="1"/>
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
+      <c r="H48" s="1"/>
+      <c r="I48" s="1"/>
+      <c r="J48" s="1"/>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A49" s="1"/>
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1"/>
+      <c r="H49" s="1"/>
+      <c r="I49" s="1"/>
+      <c r="J49" s="1"/>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A50" s="1"/>
+      <c r="B50" s="1"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+      <c r="F50" s="1"/>
+      <c r="G50" s="1"/>
+      <c r="H50" s="1"/>
+      <c r="I50" s="1"/>
+      <c r="J50" s="1"/>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A51" s="1"/>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+      <c r="F51" s="1"/>
+      <c r="G51" s="1"/>
+      <c r="H51" s="1"/>
+      <c r="I51" s="1"/>
+      <c r="J51" s="1"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A52" s="1"/>
+      <c r="B52" s="1"/>
+      <c r="C52" s="1"/>
+      <c r="D52" s="1"/>
+      <c r="E52" s="1"/>
+      <c r="F52" s="1"/>
+      <c r="G52" s="1"/>
+      <c r="H52" s="1"/>
+      <c r="I52" s="1"/>
+      <c r="J52" s="1"/>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A53" s="1"/>
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+      <c r="F53" s="1"/>
+      <c r="G53" s="1"/>
+      <c r="H53" s="1"/>
+      <c r="I53" s="1"/>
+      <c r="J53" s="1"/>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A54" s="1"/>
+      <c r="B54" s="1"/>
+      <c r="C54" s="1"/>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+      <c r="F54" s="1"/>
+      <c r="G54" s="1"/>
+      <c r="H54" s="1"/>
+      <c r="I54" s="1"/>
+      <c r="J54" s="1"/>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A55" s="1"/>
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+      <c r="F55" s="1"/>
+      <c r="G55" s="1"/>
+      <c r="H55" s="1"/>
+      <c r="I55" s="1"/>
+      <c r="J55" s="1"/>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A56" s="1"/>
+      <c r="B56" s="1"/>
+      <c r="C56" s="1"/>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
+      <c r="F56" s="1"/>
+      <c r="G56" s="1"/>
+      <c r="H56" s="1"/>
+      <c r="I56" s="1"/>
+      <c r="J56" s="1"/>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A57" s="1"/>
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
+      <c r="E57" s="1"/>
+      <c r="F57" s="1"/>
+      <c r="G57" s="1"/>
+      <c r="H57" s="1"/>
+      <c r="I57" s="1"/>
+      <c r="J57" s="1"/>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A58" s="1"/>
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
+      <c r="D58" s="1"/>
+      <c r="E58" s="1"/>
+      <c r="F58" s="1"/>
+      <c r="G58" s="1"/>
+      <c r="H58" s="1"/>
+      <c r="I58" s="1"/>
+      <c r="J58" s="1"/>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A59" s="1"/>
+      <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
+      <c r="D59" s="1"/>
+      <c r="E59" s="1"/>
+      <c r="F59" s="1"/>
+      <c r="G59" s="1"/>
+      <c r="H59" s="1"/>
+      <c r="I59" s="1"/>
+      <c r="J59" s="1"/>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A60" s="1"/>
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
+      <c r="F60" s="1"/>
+      <c r="G60" s="1"/>
+      <c r="H60" s="1"/>
+      <c r="I60" s="1"/>
+      <c r="J60" s="1"/>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A61" s="1"/>
+      <c r="B61" s="1"/>
+      <c r="C61" s="1"/>
+      <c r="D61" s="1"/>
+      <c r="E61" s="1"/>
+      <c r="F61" s="1"/>
+      <c r="G61" s="1"/>
+      <c r="H61" s="1"/>
+      <c r="I61" s="1"/>
+      <c r="J61" s="1"/>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A62" s="1"/>
+      <c r="B62" s="1"/>
+      <c r="C62" s="1"/>
+      <c r="D62" s="1"/>
+      <c r="E62" s="1"/>
+      <c r="F62" s="1"/>
+      <c r="G62" s="1"/>
+      <c r="H62" s="1"/>
+      <c r="I62" s="1"/>
+      <c r="J62" s="1"/>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A63" s="1"/>
+      <c r="B63" s="1"/>
+      <c r="C63" s="1"/>
+      <c r="D63" s="1"/>
+      <c r="E63" s="1"/>
+      <c r="F63" s="1"/>
+      <c r="G63" s="1"/>
+      <c r="H63" s="1"/>
+      <c r="I63" s="1"/>
+      <c r="J63" s="1"/>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A64" s="1"/>
+      <c r="B64" s="1"/>
+      <c r="C64" s="1"/>
+      <c r="D64" s="1"/>
+      <c r="E64" s="1"/>
+      <c r="F64" s="1"/>
+      <c r="G64" s="1"/>
+      <c r="H64" s="1"/>
+      <c r="I64" s="1"/>
+      <c r="J64" s="1"/>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A65" s="1"/>
+      <c r="B65" s="1"/>
+      <c r="C65" s="1"/>
+      <c r="D65" s="1"/>
+      <c r="E65" s="1"/>
+      <c r="F65" s="1"/>
+      <c r="G65" s="1"/>
+      <c r="H65" s="1"/>
+      <c r="I65" s="1"/>
+      <c r="J65" s="1"/>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A66" s="1"/>
+      <c r="B66" s="1"/>
+      <c r="C66" s="1"/>
+      <c r="D66" s="1"/>
+      <c r="E66" s="1"/>
+      <c r="F66" s="1"/>
+      <c r="G66" s="1"/>
+      <c r="H66" s="1"/>
+      <c r="I66" s="1"/>
+      <c r="J66" s="1"/>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A67" s="1"/>
+      <c r="B67" s="1"/>
+      <c r="C67" s="1"/>
+      <c r="D67" s="1"/>
+      <c r="E67" s="1"/>
+      <c r="F67" s="1"/>
+      <c r="G67" s="1"/>
+      <c r="H67" s="1"/>
+      <c r="I67" s="1"/>
+      <c r="J67" s="1"/>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A68" s="1"/>
+      <c r="B68" s="1"/>
+      <c r="C68" s="1"/>
+      <c r="D68" s="1"/>
+      <c r="E68" s="1"/>
+      <c r="F68" s="1"/>
+      <c r="G68" s="1"/>
+      <c r="H68" s="1"/>
+      <c r="I68" s="1"/>
+      <c r="J68" s="1"/>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A69" s="1"/>
+      <c r="B69" s="1"/>
+      <c r="C69" s="1"/>
+      <c r="D69" s="1"/>
+      <c r="E69" s="1"/>
+      <c r="F69" s="1"/>
+      <c r="G69" s="1"/>
+      <c r="H69" s="1"/>
+      <c r="I69" s="1"/>
+      <c r="J69" s="1"/>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A70" s="1"/>
+      <c r="B70" s="1"/>
+      <c r="C70" s="1"/>
+      <c r="D70" s="1"/>
+      <c r="E70" s="1"/>
+      <c r="F70" s="1"/>
+      <c r="G70" s="1"/>
+      <c r="H70" s="1"/>
+      <c r="I70" s="1"/>
+      <c r="J70" s="1"/>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A71" s="1"/>
+      <c r="B71" s="1"/>
+      <c r="C71" s="1"/>
+      <c r="D71" s="1"/>
+      <c r="E71" s="1"/>
+      <c r="F71" s="1"/>
+      <c r="G71" s="1"/>
+      <c r="H71" s="1"/>
+      <c r="I71" s="1"/>
+      <c r="J71" s="1"/>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A72" s="1"/>
+      <c r="B72" s="1"/>
+      <c r="C72" s="1"/>
+      <c r="D72" s="1"/>
+      <c r="E72" s="1"/>
+      <c r="F72" s="1"/>
+      <c r="G72" s="1"/>
+      <c r="H72" s="1"/>
+      <c r="I72" s="1"/>
+      <c r="J72" s="1"/>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A73" s="1"/>
+      <c r="B73" s="1"/>
+      <c r="C73" s="1"/>
+      <c r="D73" s="1"/>
+      <c r="E73" s="1"/>
+      <c r="F73" s="1"/>
+      <c r="G73" s="1"/>
+      <c r="H73" s="1"/>
+      <c r="I73" s="1"/>
+      <c r="J73" s="1"/>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A74" s="1"/>
+      <c r="B74" s="1"/>
+      <c r="C74" s="1"/>
+      <c r="D74" s="1"/>
+      <c r="E74" s="1"/>
+      <c r="F74" s="1"/>
+      <c r="G74" s="1"/>
+      <c r="H74" s="1"/>
+      <c r="I74" s="1"/>
+      <c r="J74" s="1"/>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A75" s="1"/>
+      <c r="B75" s="1"/>
+      <c r="C75" s="1"/>
+      <c r="D75" s="1"/>
+      <c r="E75" s="1"/>
+      <c r="F75" s="1"/>
+      <c r="G75" s="1"/>
+      <c r="H75" s="1"/>
+      <c r="I75" s="1"/>
+      <c r="J75" s="1"/>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A76" s="1"/>
+      <c r="B76" s="1"/>
+      <c r="C76" s="1"/>
+      <c r="D76" s="1"/>
+      <c r="E76" s="1"/>
+      <c r="F76" s="1"/>
+      <c r="G76" s="1"/>
+      <c r="H76" s="1"/>
+      <c r="I76" s="1"/>
+      <c r="J76" s="1"/>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A77" s="1"/>
+      <c r="B77" s="1"/>
+      <c r="C77" s="1"/>
+      <c r="D77" s="1"/>
+      <c r="E77" s="1"/>
+      <c r="F77" s="1"/>
+      <c r="G77" s="1"/>
+      <c r="H77" s="1"/>
+      <c r="I77" s="1"/>
+      <c r="J77" s="1"/>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A78" s="1"/>
+      <c r="B78" s="1"/>
+      <c r="C78" s="1"/>
+      <c r="D78" s="1"/>
+      <c r="E78" s="1"/>
+      <c r="F78" s="1"/>
+      <c r="G78" s="1"/>
+      <c r="H78" s="1"/>
+      <c r="I78" s="1"/>
+      <c r="J78" s="1"/>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A79" s="1"/>
+      <c r="B79" s="1"/>
+      <c r="C79" s="1"/>
+      <c r="D79" s="1"/>
+      <c r="E79" s="1"/>
+      <c r="F79" s="1"/>
+      <c r="G79" s="1"/>
+      <c r="H79" s="1"/>
+      <c r="I79" s="1"/>
+      <c r="J79" s="1"/>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A80" s="1"/>
+      <c r="B80" s="1"/>
+      <c r="C80" s="1"/>
+      <c r="D80" s="1"/>
+      <c r="E80" s="1"/>
+      <c r="F80" s="1"/>
+      <c r="G80" s="1"/>
+      <c r="H80" s="1"/>
+      <c r="I80" s="1"/>
+      <c r="J80" s="1"/>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A81" s="1"/>
+      <c r="B81" s="1"/>
+      <c r="C81" s="1"/>
+      <c r="D81" s="1"/>
+      <c r="E81" s="1"/>
+      <c r="F81" s="1"/>
+      <c r="G81" s="1"/>
+      <c r="H81" s="1"/>
+      <c r="I81" s="1"/>
+      <c r="J81" s="1"/>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A82" s="1"/>
+      <c r="B82" s="1"/>
+      <c r="C82" s="1"/>
+      <c r="D82" s="1"/>
+      <c r="E82" s="1"/>
+      <c r="F82" s="1"/>
+      <c r="G82" s="1"/>
+      <c r="H82" s="1"/>
+      <c r="I82" s="1"/>
+      <c r="J82" s="1"/>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A83" s="1"/>
+      <c r="B83" s="1"/>
+      <c r="C83" s="1"/>
+      <c r="D83" s="1"/>
+      <c r="E83" s="1"/>
+      <c r="F83" s="1"/>
+      <c r="G83" s="1"/>
+      <c r="H83" s="1"/>
+      <c r="I83" s="1"/>
+      <c r="J83" s="1"/>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A84" s="1"/>
+      <c r="B84" s="1"/>
+      <c r="C84" s="1"/>
+      <c r="D84" s="1"/>
+      <c r="E84" s="1"/>
+      <c r="F84" s="1"/>
+      <c r="G84" s="1"/>
+      <c r="H84" s="1"/>
+      <c r="I84" s="1"/>
+      <c r="J84" s="1"/>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A85" s="1"/>
+      <c r="B85" s="1"/>
+      <c r="C85" s="1"/>
+      <c r="D85" s="1"/>
+      <c r="E85" s="1"/>
+      <c r="F85" s="1"/>
+      <c r="G85" s="1"/>
+      <c r="H85" s="1"/>
+      <c r="I85" s="1"/>
+      <c r="J85" s="1"/>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A86" s="1"/>
+      <c r="B86" s="1"/>
+      <c r="C86" s="1"/>
+      <c r="D86" s="1"/>
+      <c r="E86" s="1"/>
+      <c r="F86" s="1"/>
+      <c r="G86" s="1"/>
+      <c r="H86" s="1"/>
+      <c r="I86" s="1"/>
+      <c r="J86" s="1"/>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A87" s="1"/>
+      <c r="B87" s="1"/>
+      <c r="C87" s="1"/>
+      <c r="D87" s="1"/>
+      <c r="E87" s="1"/>
+      <c r="F87" s="1"/>
+      <c r="G87" s="1"/>
+      <c r="H87" s="1"/>
+      <c r="I87" s="1"/>
+      <c r="J87" s="1"/>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A88" s="1"/>
+      <c r="B88" s="1"/>
+      <c r="C88" s="1"/>
+      <c r="D88" s="1"/>
+      <c r="E88" s="1"/>
+      <c r="F88" s="1"/>
+      <c r="G88" s="1"/>
+      <c r="H88" s="1"/>
+      <c r="I88" s="1"/>
+      <c r="J88" s="1"/>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A89" s="1"/>
+      <c r="B89" s="1"/>
+      <c r="C89" s="1"/>
+      <c r="D89" s="1"/>
+      <c r="E89" s="1"/>
+      <c r="F89" s="1"/>
+      <c r="G89" s="1"/>
+      <c r="H89" s="1"/>
+      <c r="I89" s="1"/>
+      <c r="J89" s="1"/>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A90" s="1"/>
+      <c r="B90" s="1"/>
+      <c r="C90" s="1"/>
+      <c r="D90" s="1"/>
+      <c r="E90" s="1"/>
+      <c r="F90" s="1"/>
+      <c r="G90" s="1"/>
+      <c r="H90" s="1"/>
+      <c r="I90" s="1"/>
+      <c r="J90" s="1"/>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A91" s="1"/>
+      <c r="B91" s="1"/>
+      <c r="C91" s="1"/>
+      <c r="D91" s="1"/>
+      <c r="E91" s="1"/>
+      <c r="F91" s="1"/>
+      <c r="G91" s="1"/>
+      <c r="H91" s="1"/>
+      <c r="I91" s="1"/>
+      <c r="J91" s="1"/>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A92" s="1"/>
+      <c r="B92" s="1"/>
+      <c r="C92" s="1"/>
+      <c r="D92" s="1"/>
+      <c r="E92" s="1"/>
+      <c r="F92" s="1"/>
+      <c r="G92" s="1"/>
+      <c r="H92" s="1"/>
+      <c r="I92" s="1"/>
+      <c r="J92" s="1"/>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A93" s="1"/>
+      <c r="B93" s="1"/>
+      <c r="C93" s="1"/>
+      <c r="D93" s="1"/>
+      <c r="E93" s="1"/>
+      <c r="F93" s="1"/>
+      <c r="G93" s="1"/>
+      <c r="H93" s="1"/>
+      <c r="I93" s="1"/>
+      <c r="J93" s="1"/>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A94" s="1"/>
+      <c r="B94" s="1"/>
+      <c r="C94" s="1"/>
+      <c r="D94" s="1"/>
+      <c r="E94" s="1"/>
+      <c r="F94" s="1"/>
+      <c r="G94" s="1"/>
+      <c r="H94" s="1"/>
+      <c r="I94" s="1"/>
+      <c r="J94" s="1"/>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A95" s="1"/>
+      <c r="B95" s="1"/>
+      <c r="C95" s="1"/>
+      <c r="D95" s="1"/>
+      <c r="E95" s="1"/>
+      <c r="F95" s="1"/>
+      <c r="G95" s="1"/>
+      <c r="H95" s="1"/>
+      <c r="I95" s="1"/>
+      <c r="J95" s="1"/>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A96" s="1"/>
+      <c r="B96" s="1"/>
+      <c r="C96" s="1"/>
+      <c r="D96" s="1"/>
+      <c r="E96" s="1"/>
+      <c r="F96" s="1"/>
+      <c r="G96" s="1"/>
+      <c r="H96" s="1"/>
+      <c r="I96" s="1"/>
+      <c r="J96" s="1"/>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A97" s="1"/>
+      <c r="B97" s="1"/>
+      <c r="C97" s="1"/>
+      <c r="D97" s="1"/>
+      <c r="E97" s="1"/>
+      <c r="F97" s="1"/>
+      <c r="G97" s="1"/>
+      <c r="H97" s="1"/>
+      <c r="I97" s="1"/>
+      <c r="J97" s="1"/>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A98" s="1"/>
+      <c r="B98" s="1"/>
+      <c r="C98" s="1"/>
+      <c r="D98" s="1"/>
+      <c r="E98" s="1"/>
+      <c r="F98" s="1"/>
+      <c r="G98" s="1"/>
+      <c r="H98" s="1"/>
+      <c r="I98" s="1"/>
+      <c r="J98" s="1"/>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A99" s="1"/>
+      <c r="B99" s="1"/>
+      <c r="C99" s="1"/>
+      <c r="D99" s="1"/>
+      <c r="E99" s="1"/>
+      <c r="F99" s="1"/>
+      <c r="G99" s="1"/>
+      <c r="H99" s="1"/>
+      <c r="I99" s="1"/>
+      <c r="J99" s="1"/>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A100" s="1"/>
+      <c r="B100" s="1"/>
+      <c r="C100" s="1"/>
+      <c r="D100" s="1"/>
+      <c r="E100" s="1"/>
+      <c r="F100" s="1"/>
+      <c r="G100" s="1"/>
+      <c r="H100" s="1"/>
+      <c r="I100" s="1"/>
+      <c r="J100" s="1"/>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A101" s="1"/>
+      <c r="B101" s="1"/>
+      <c r="C101" s="1"/>
+      <c r="D101" s="1"/>
+      <c r="E101" s="1"/>
+      <c r="F101" s="1"/>
+      <c r="G101" s="1"/>
+      <c r="H101" s="1"/>
+      <c r="I101" s="1"/>
+      <c r="J101" s="1"/>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A102" s="1"/>
+      <c r="B102" s="1"/>
+      <c r="C102" s="1"/>
+      <c r="D102" s="1"/>
+      <c r="E102" s="1"/>
+      <c r="F102" s="1"/>
+      <c r="G102" s="1"/>
+      <c r="H102" s="1"/>
+      <c r="I102" s="1"/>
+      <c r="J102" s="1"/>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A103" s="1"/>
+      <c r="B103" s="1"/>
+      <c r="C103" s="1"/>
+      <c r="D103" s="1"/>
+      <c r="E103" s="1"/>
+      <c r="F103" s="1"/>
+      <c r="G103" s="1"/>
+      <c r="H103" s="1"/>
+      <c r="I103" s="1"/>
+      <c r="J103" s="1"/>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A104" s="1"/>
+      <c r="B104" s="1"/>
+      <c r="C104" s="1"/>
+      <c r="D104" s="1"/>
+      <c r="E104" s="1"/>
+      <c r="F104" s="1"/>
+      <c r="G104" s="1"/>
+      <c r="H104" s="1"/>
+      <c r="I104" s="1"/>
+      <c r="J104" s="1"/>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A105" s="1"/>
+      <c r="B105" s="1"/>
+      <c r="C105" s="1"/>
+      <c r="D105" s="1"/>
+      <c r="E105" s="1"/>
+      <c r="F105" s="1"/>
+      <c r="G105" s="1"/>
+      <c r="H105" s="1"/>
+      <c r="I105" s="1"/>
+      <c r="J105" s="1"/>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A106" s="1"/>
+      <c r="B106" s="1"/>
+      <c r="C106" s="1"/>
+      <c r="D106" s="1"/>
+      <c r="E106" s="1"/>
+      <c r="F106" s="1"/>
+      <c r="G106" s="1"/>
+      <c r="H106" s="1"/>
+      <c r="I106" s="1"/>
+      <c r="J106" s="1"/>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A107" s="1"/>
+      <c r="B107" s="1"/>
+      <c r="C107" s="1"/>
+      <c r="D107" s="1"/>
+      <c r="E107" s="1"/>
+      <c r="F107" s="1"/>
+      <c r="G107" s="1"/>
+      <c r="H107" s="1"/>
+      <c r="I107" s="1"/>
+      <c r="J107" s="1"/>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A108" s="1"/>
+      <c r="B108" s="1"/>
+      <c r="C108" s="1"/>
+      <c r="D108" s="1"/>
+      <c r="E108" s="1"/>
+      <c r="F108" s="1"/>
+      <c r="G108" s="1"/>
+      <c r="H108" s="1"/>
+      <c r="I108" s="1"/>
+      <c r="J108" s="1"/>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A109" s="1"/>
+      <c r="B109" s="1"/>
+      <c r="C109" s="1"/>
+      <c r="D109" s="1"/>
+      <c r="E109" s="1"/>
+      <c r="F109" s="1"/>
+      <c r="G109" s="1"/>
+      <c r="H109" s="1"/>
+      <c r="I109" s="1"/>
+      <c r="J109" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update data viz and simulation log
</commit_message>
<xml_diff>
--- a/Simulation_log_key.xlsx
+++ b/Simulation_log_key.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\Documents\R\working_directory\LemonSharkCKMR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{785B9CF8-B2C2-4195-8E29-1D5CC038C228}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DD3C6DE-3F20-4189-AD23-2FCAC37E2448}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5085" yWindow="-11640" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Simulation_log_key" sheetId="1" r:id="rId1"/>
@@ -26,6 +26,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={7C8B021F-519D-4857-BD5A-15B80B44043B}</author>
+    <author>John</author>
   </authors>
   <commentList>
     <comment ref="A1" authorId="0" shapeId="0" xr:uid="{7C8B021F-519D-4857-BD5A-15B80B44043B}">
@@ -37,12 +38,36 @@
 Green highlight means I have all of the results downloaded to Drive but I have not downloaded the comparison dataframes or model output for trials on August 24th and later.</t>
       </text>
     </comment>
+    <comment ref="A13" authorId="1" shapeId="0" xr:uid="{8F388C97-A7B0-449C-B48B-BBDC639632C7}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>John:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+These seem to be exactly the same simulations as 3.3? Except the initial value of psi was different? Gonna assume they were the same otherwise; looked through script and didn’t see any difference</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="197">
   <si>
     <t>Objective</t>
   </si>
@@ -497,9 +522,6 @@
     <t>Major population decline; lambda in model w/ wide prior</t>
   </si>
   <si>
-    <t>Small population change; lambda in model w/ tight prior</t>
-  </si>
-  <si>
     <t>Major population decline; lambda in model w/ tight prior</t>
   </si>
   <si>
@@ -629,23 +651,20 @@
     <t>Still need to download</t>
   </si>
   <si>
-    <t>All</t>
-  </si>
-  <si>
-    <t>sample.all.juvenile.ages_lambda.variable; running the second part right now; it didn't run before.</t>
-  </si>
-  <si>
-    <t>All; re-running juvenile sample scenario as array bc the output files were overwriting themselves; adults are still running as of 08/26</t>
-  </si>
-  <si>
-    <t>All; may need to pull first 400 iterations for adults</t>
+    <t>Pulled first 400 iterations for adults; need to run last 100</t>
+  </si>
+  <si>
+    <t>Used previous run for adults. Results should be the same, just won't have DIC scores</t>
+  </si>
+  <si>
+    <t>Small population change; lambda in model w/ tight prior - for stable scenario for all ages and YOY, used results from scenario_1.2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -780,8 +799,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="36">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -979,6 +1011,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -1140,7 +1178,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1153,6 +1191,15 @@
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1525,14 +1572,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="32.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="86.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.5546875" customWidth="1"/>
     <col min="5" max="5" width="27.6640625" bestFit="1" customWidth="1"/>
@@ -1550,7 +1597,7 @@
         <v>36</v>
       </c>
       <c r="B1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1559,7 +1606,7 @@
         <v>14</v>
       </c>
       <c r="E1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F1" t="s">
         <v>58</v>
@@ -1595,7 +1642,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -1631,7 +1678,7 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -1667,13 +1714,13 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H4" t="s">
         <v>15</v>
@@ -1703,13 +1750,13 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H5" t="s">
         <v>15</v>
@@ -1727,13 +1774,11 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>196</v>
-      </c>
+      <c r="B6" s="8"/>
       <c r="C6" t="s">
         <v>148</v>
       </c>
@@ -1741,13 +1786,13 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H6" t="s">
         <v>59</v>
@@ -1777,13 +1822,13 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F7">
         <v>0</v>
       </c>
       <c r="G7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H7" t="s">
         <v>59</v>
@@ -1801,27 +1846,27 @@
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="8" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C8" t="s">
-        <v>151</v>
+      <c r="B8" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>196</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F8">
         <v>0</v>
       </c>
       <c r="G8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H8" t="s">
         <v>18</v>
@@ -1835,23 +1880,21 @@
       <c r="A9" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>195</v>
-      </c>
+      <c r="B9" s="6"/>
       <c r="C9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D9">
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F9">
         <v>0</v>
       </c>
       <c r="G9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H9" t="s">
         <v>18</v>
@@ -1865,17 +1908,15 @@
       <c r="A10" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B10" s="6" t="s">
-        <v>195</v>
-      </c>
+      <c r="B10" s="6"/>
       <c r="C10" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D10">
         <v>2</v>
       </c>
       <c r="E10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F10" s="4">
         <v>0</v>
@@ -1897,20 +1938,20 @@
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="A11" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="B11" t="s">
-        <v>198</v>
+      <c r="B11" s="9" t="s">
+        <v>194</v>
       </c>
       <c r="C11" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D11">
         <v>2</v>
       </c>
       <c r="E11" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F11" s="4">
         <v>0</v>
@@ -1932,20 +1973,20 @@
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>187</v>
-      </c>
-      <c r="B12" t="s">
-        <v>198</v>
+      <c r="A12" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>194</v>
       </c>
       <c r="C12" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D12">
         <v>2</v>
       </c>
       <c r="E12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F12" s="4">
         <v>0</v>
@@ -1954,7 +1995,7 @@
         <v>1</v>
       </c>
       <c r="H12" t="s">
-        <v>59</v>
+        <v>18</v>
       </c>
       <c r="I12" t="s">
         <v>19</v>
@@ -1967,105 +2008,106 @@
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B13" s="6"/>
-      <c r="C13" t="s">
+      <c r="B13" s="2"/>
+      <c r="C13" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D13" s="2">
+        <v>2</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="F13" s="11">
+        <v>0</v>
+      </c>
+      <c r="G13" s="2">
+        <v>1</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L13" s="2"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="D13">
+      <c r="D14" s="2">
         <v>2</v>
       </c>
-      <c r="E13" t="s">
-        <v>155</v>
-      </c>
-      <c r="F13" s="4">
+      <c r="E14" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="F14" s="11">
         <v>0</v>
       </c>
-      <c r="G13">
+      <c r="G14" s="2">
         <v>1</v>
       </c>
-      <c r="H13" t="s">
-        <v>15</v>
-      </c>
-      <c r="I13" t="s">
+      <c r="H14" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="I14" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J13" t="s">
-        <v>53</v>
-      </c>
-      <c r="K13" t="s">
+      <c r="J14" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K14" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>195</v>
-      </c>
-      <c r="C14" t="s">
-        <v>159</v>
-      </c>
-      <c r="D14">
+      <c r="L14" s="2"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="D15" s="2">
         <v>2</v>
       </c>
-      <c r="E14" t="s">
-        <v>155</v>
-      </c>
-      <c r="F14" s="4">
+      <c r="E15" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="F15" s="11">
         <v>0</v>
       </c>
-      <c r="G14">
+      <c r="G15" s="2">
         <v>1</v>
       </c>
-      <c r="H14" t="s">
-        <v>59</v>
-      </c>
-      <c r="I14" t="s">
+      <c r="H15" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I15" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J14" t="s">
+      <c r="J15" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="K14" t="s">
+      <c r="K15" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="6" t="s">
-        <v>191</v>
-      </c>
-      <c r="B15" s="6"/>
-      <c r="C15" t="s">
-        <v>161</v>
-      </c>
-      <c r="D15">
-        <v>2</v>
-      </c>
-      <c r="E15" t="s">
-        <v>155</v>
-      </c>
-      <c r="F15" s="4">
-        <v>0</v>
-      </c>
-      <c r="G15">
-        <v>1</v>
-      </c>
-      <c r="H15" t="s">
-        <v>59</v>
-      </c>
-      <c r="I15" t="s">
-        <v>19</v>
-      </c>
-      <c r="J15" t="s">
-        <v>27</v>
-      </c>
-      <c r="K15" t="s">
-        <v>17</v>
-      </c>
+      <c r="L15" s="2"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
@@ -2073,13 +2115,13 @@
       </c>
       <c r="B16" s="6"/>
       <c r="C16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D16">
         <v>2</v>
       </c>
       <c r="E16" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F16" s="4">
         <v>0</v>
@@ -2106,13 +2148,13 @@
       </c>
       <c r="B17" s="6"/>
       <c r="C17" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D17">
         <v>2</v>
       </c>
       <c r="E17" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F17" s="4">
         <v>0</v>
@@ -2137,15 +2179,15 @@
       <c r="A18" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="B18" s="6"/>
+      <c r="B18" s="12"/>
       <c r="C18" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D18">
         <v>2</v>
       </c>
       <c r="E18" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F18" s="4">
         <v>0</v>
@@ -2173,17 +2215,15 @@
       <c r="A19" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="B19" s="6" t="s">
-        <v>195</v>
-      </c>
+      <c r="B19" s="6"/>
       <c r="C19" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D19">
         <v>2</v>
       </c>
       <c r="E19" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F19" s="4">
         <v>0</v>
@@ -2210,13 +2250,13 @@
       </c>
       <c r="B20" s="7"/>
       <c r="C20" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D20">
         <v>2</v>
       </c>
       <c r="E20" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F20" s="4">
         <v>0</v>
@@ -2243,13 +2283,13 @@
       </c>
       <c r="B21" s="7"/>
       <c r="C21" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D21">
         <v>2</v>
       </c>
       <c r="E21" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F21" s="4">
         <v>0</v>
@@ -2272,17 +2312,17 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B22" s="7"/>
       <c r="C22" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D22">
         <v>2</v>
       </c>
       <c r="E22" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F22" s="4">
         <v>0</v>
@@ -4244,7 +4284,7 @@
   <dimension ref="A1:O109"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4271,33 +4311,33 @@
         <v>46</v>
       </c>
       <c r="C1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E1" t="s">
         <v>47</v>
       </c>
       <c r="F1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H1" t="s">
         <v>48</v>
       </c>
       <c r="I1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>37</v>
@@ -4313,85 +4353,85 @@
     </row>
     <row r="3" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>142</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>40</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M3" s="1"/>
       <c r="O3" s="1"/>
     </row>
     <row r="4" spans="1:15" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>41</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>143</v>
       </c>
       <c r="I4" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>181</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>185</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>186</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>

</xml_diff>

<commit_message>
Update simulation log; start scripts for comparing skipped-breeding equations
</commit_message>
<xml_diff>
--- a/Simulation_log_key.xlsx
+++ b/Simulation_log_key.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zeus\Documents\R\working_directory\LemonSharkCKMR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B24A48E2-61D0-49D3-9C87-F17D7E519FEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE40CEC8-D02B-426C-AB70-D7E5647B5ED4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11565" yWindow="1785" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Simulation_log_key" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="201">
   <si>
     <t>Objective</t>
   </si>
@@ -633,13 +633,25 @@
   </si>
   <si>
     <t>All</t>
+  </si>
+  <si>
+    <t>scenario_3.4.1</t>
+  </si>
+  <si>
+    <t>scenario_3.4.2</t>
+  </si>
+  <si>
+    <t>Biennial breeding; Liz's biennial model; psi = 0.75, lambda in model w/ tight prior</t>
+  </si>
+  <si>
+    <t>Biennial breeding; Ben's biennial model; psi = 0.75, lambda in model w/ tight prior</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -773,12 +785,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="36">
@@ -1140,7 +1146,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1153,6 +1159,7 @@
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1523,10 +1530,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L35"/>
+  <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21:K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2205,12 +2212,11 @@
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="B20" s="7"/>
+      <c r="A20" s="8" t="s">
+        <v>197</v>
+      </c>
       <c r="C20" t="s">
-        <v>162</v>
+        <v>199</v>
       </c>
       <c r="D20">
         <v>2</v>
@@ -2225,7 +2231,7 @@
         <v>1</v>
       </c>
       <c r="H20" t="s">
-        <v>59</v>
+        <v>18</v>
       </c>
       <c r="I20" t="s">
         <v>19</v>
@@ -2238,12 +2244,11 @@
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="B21" s="7"/>
+      <c r="A21" s="8" t="s">
+        <v>198</v>
+      </c>
       <c r="C21" t="s">
-        <v>163</v>
+        <v>200</v>
       </c>
       <c r="D21">
         <v>2</v>
@@ -2272,11 +2277,11 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>192</v>
+        <v>45</v>
       </c>
       <c r="B22" s="7"/>
       <c r="C22" t="s">
-        <v>193</v>
+        <v>162</v>
       </c>
       <c r="D22">
         <v>2</v>
@@ -2291,7 +2296,7 @@
         <v>1</v>
       </c>
       <c r="H22" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
       <c r="I22" t="s">
         <v>19</v>
@@ -2303,24 +2308,90 @@
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>10</v>
-      </c>
-      <c r="C34" t="s">
-        <v>11</v>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="B23" s="7"/>
+      <c r="C23" t="s">
+        <v>163</v>
+      </c>
+      <c r="D23">
+        <v>2</v>
+      </c>
+      <c r="E23" t="s">
+        <v>155</v>
+      </c>
+      <c r="F23" s="4">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23" t="s">
+        <v>18</v>
+      </c>
+      <c r="I23" t="s">
+        <v>19</v>
+      </c>
+      <c r="J23" t="s">
+        <v>27</v>
+      </c>
+      <c r="K23" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="B24" s="7"/>
+      <c r="C24" t="s">
+        <v>193</v>
+      </c>
+      <c r="D24">
+        <v>2</v>
+      </c>
+      <c r="E24" t="s">
+        <v>155</v>
+      </c>
+      <c r="F24" s="4">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24" t="s">
+        <v>15</v>
+      </c>
+      <c r="I24" t="s">
+        <v>19</v>
+      </c>
+      <c r="J24" t="s">
+        <v>27</v>
+      </c>
+      <c r="K24" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>10</v>
+      </c>
+      <c r="C36" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>12</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C37" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update objective 4 viz and simulation log
</commit_message>
<xml_diff>
--- a/Simulation_log_key.xlsx
+++ b/Simulation_log_key.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\Documents\R\working_directory\LemonSharkCKMR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DD3C6DE-3F20-4189-AD23-2FCAC37E2448}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CE8F7E1-683D-43F9-91A9-861B42F4F6C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5085" yWindow="-11640" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Simulation_log_key" sheetId="1" r:id="rId1"/>
-    <sheet name="Simulation_log_old_7.24.22" sheetId="3" r:id="rId2"/>
-    <sheet name="model_settings_old" sheetId="4" r:id="rId3"/>
-    <sheet name="Objective_key" sheetId="2" r:id="rId4"/>
+    <sheet name="Objective_key" sheetId="2" r:id="rId2"/>
+    <sheet name="Simulation_log_old_7.24.22" sheetId="3" r:id="rId3"/>
+    <sheet name="model_settings_old" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -1572,8 +1572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2371,6 +2371,1419 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{412D6C35-5CAD-470C-B537-E441B956C3CF}">
+  <dimension ref="A1:O109"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="52.6640625" customWidth="1"/>
+    <col min="2" max="2" width="47.6640625" customWidth="1"/>
+    <col min="3" max="3" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="47.6640625" customWidth="1"/>
+    <col min="5" max="5" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="26.6640625" customWidth="1"/>
+    <col min="8" max="8" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.6640625" customWidth="1"/>
+    <col min="10" max="12" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="26.109375" customWidth="1"/>
+    <col min="14" max="14" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="34.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D1" t="s">
+        <v>164</v>
+      </c>
+      <c r="E1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" t="s">
+        <v>170</v>
+      </c>
+      <c r="G1" t="s">
+        <v>165</v>
+      </c>
+      <c r="H1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="M3" s="1"/>
+      <c r="O3" s="1"/>
+    </row>
+    <row r="4" spans="1:15" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+      <c r="J39" s="1"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+      <c r="J40" s="1"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A41" s="1"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A42" s="1"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
+      <c r="I42" s="1"/>
+      <c r="J42" s="1"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A43" s="1"/>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+      <c r="H43" s="1"/>
+      <c r="I43" s="1"/>
+      <c r="J43" s="1"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A44" s="1"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+      <c r="H44" s="1"/>
+      <c r="I44" s="1"/>
+      <c r="J44" s="1"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A45" s="1"/>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+      <c r="H45" s="1"/>
+      <c r="I45" s="1"/>
+      <c r="J45" s="1"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A46" s="1"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
+      <c r="H46" s="1"/>
+      <c r="I46" s="1"/>
+      <c r="J46" s="1"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
+      <c r="H47" s="1"/>
+      <c r="I47" s="1"/>
+      <c r="J47" s="1"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A48" s="1"/>
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
+      <c r="H48" s="1"/>
+      <c r="I48" s="1"/>
+      <c r="J48" s="1"/>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A49" s="1"/>
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1"/>
+      <c r="H49" s="1"/>
+      <c r="I49" s="1"/>
+      <c r="J49" s="1"/>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A50" s="1"/>
+      <c r="B50" s="1"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+      <c r="F50" s="1"/>
+      <c r="G50" s="1"/>
+      <c r="H50" s="1"/>
+      <c r="I50" s="1"/>
+      <c r="J50" s="1"/>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A51" s="1"/>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+      <c r="F51" s="1"/>
+      <c r="G51" s="1"/>
+      <c r="H51" s="1"/>
+      <c r="I51" s="1"/>
+      <c r="J51" s="1"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A52" s="1"/>
+      <c r="B52" s="1"/>
+      <c r="C52" s="1"/>
+      <c r="D52" s="1"/>
+      <c r="E52" s="1"/>
+      <c r="F52" s="1"/>
+      <c r="G52" s="1"/>
+      <c r="H52" s="1"/>
+      <c r="I52" s="1"/>
+      <c r="J52" s="1"/>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A53" s="1"/>
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+      <c r="F53" s="1"/>
+      <c r="G53" s="1"/>
+      <c r="H53" s="1"/>
+      <c r="I53" s="1"/>
+      <c r="J53" s="1"/>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A54" s="1"/>
+      <c r="B54" s="1"/>
+      <c r="C54" s="1"/>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+      <c r="F54" s="1"/>
+      <c r="G54" s="1"/>
+      <c r="H54" s="1"/>
+      <c r="I54" s="1"/>
+      <c r="J54" s="1"/>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A55" s="1"/>
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+      <c r="F55" s="1"/>
+      <c r="G55" s="1"/>
+      <c r="H55" s="1"/>
+      <c r="I55" s="1"/>
+      <c r="J55" s="1"/>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A56" s="1"/>
+      <c r="B56" s="1"/>
+      <c r="C56" s="1"/>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
+      <c r="F56" s="1"/>
+      <c r="G56" s="1"/>
+      <c r="H56" s="1"/>
+      <c r="I56" s="1"/>
+      <c r="J56" s="1"/>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A57" s="1"/>
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
+      <c r="E57" s="1"/>
+      <c r="F57" s="1"/>
+      <c r="G57" s="1"/>
+      <c r="H57" s="1"/>
+      <c r="I57" s="1"/>
+      <c r="J57" s="1"/>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A58" s="1"/>
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
+      <c r="D58" s="1"/>
+      <c r="E58" s="1"/>
+      <c r="F58" s="1"/>
+      <c r="G58" s="1"/>
+      <c r="H58" s="1"/>
+      <c r="I58" s="1"/>
+      <c r="J58" s="1"/>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A59" s="1"/>
+      <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
+      <c r="D59" s="1"/>
+      <c r="E59" s="1"/>
+      <c r="F59" s="1"/>
+      <c r="G59" s="1"/>
+      <c r="H59" s="1"/>
+      <c r="I59" s="1"/>
+      <c r="J59" s="1"/>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A60" s="1"/>
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
+      <c r="F60" s="1"/>
+      <c r="G60" s="1"/>
+      <c r="H60" s="1"/>
+      <c r="I60" s="1"/>
+      <c r="J60" s="1"/>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A61" s="1"/>
+      <c r="B61" s="1"/>
+      <c r="C61" s="1"/>
+      <c r="D61" s="1"/>
+      <c r="E61" s="1"/>
+      <c r="F61" s="1"/>
+      <c r="G61" s="1"/>
+      <c r="H61" s="1"/>
+      <c r="I61" s="1"/>
+      <c r="J61" s="1"/>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A62" s="1"/>
+      <c r="B62" s="1"/>
+      <c r="C62" s="1"/>
+      <c r="D62" s="1"/>
+      <c r="E62" s="1"/>
+      <c r="F62" s="1"/>
+      <c r="G62" s="1"/>
+      <c r="H62" s="1"/>
+      <c r="I62" s="1"/>
+      <c r="J62" s="1"/>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A63" s="1"/>
+      <c r="B63" s="1"/>
+      <c r="C63" s="1"/>
+      <c r="D63" s="1"/>
+      <c r="E63" s="1"/>
+      <c r="F63" s="1"/>
+      <c r="G63" s="1"/>
+      <c r="H63" s="1"/>
+      <c r="I63" s="1"/>
+      <c r="J63" s="1"/>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A64" s="1"/>
+      <c r="B64" s="1"/>
+      <c r="C64" s="1"/>
+      <c r="D64" s="1"/>
+      <c r="E64" s="1"/>
+      <c r="F64" s="1"/>
+      <c r="G64" s="1"/>
+      <c r="H64" s="1"/>
+      <c r="I64" s="1"/>
+      <c r="J64" s="1"/>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A65" s="1"/>
+      <c r="B65" s="1"/>
+      <c r="C65" s="1"/>
+      <c r="D65" s="1"/>
+      <c r="E65" s="1"/>
+      <c r="F65" s="1"/>
+      <c r="G65" s="1"/>
+      <c r="H65" s="1"/>
+      <c r="I65" s="1"/>
+      <c r="J65" s="1"/>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A66" s="1"/>
+      <c r="B66" s="1"/>
+      <c r="C66" s="1"/>
+      <c r="D66" s="1"/>
+      <c r="E66" s="1"/>
+      <c r="F66" s="1"/>
+      <c r="G66" s="1"/>
+      <c r="H66" s="1"/>
+      <c r="I66" s="1"/>
+      <c r="J66" s="1"/>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A67" s="1"/>
+      <c r="B67" s="1"/>
+      <c r="C67" s="1"/>
+      <c r="D67" s="1"/>
+      <c r="E67" s="1"/>
+      <c r="F67" s="1"/>
+      <c r="G67" s="1"/>
+      <c r="H67" s="1"/>
+      <c r="I67" s="1"/>
+      <c r="J67" s="1"/>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A68" s="1"/>
+      <c r="B68" s="1"/>
+      <c r="C68" s="1"/>
+      <c r="D68" s="1"/>
+      <c r="E68" s="1"/>
+      <c r="F68" s="1"/>
+      <c r="G68" s="1"/>
+      <c r="H68" s="1"/>
+      <c r="I68" s="1"/>
+      <c r="J68" s="1"/>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A69" s="1"/>
+      <c r="B69" s="1"/>
+      <c r="C69" s="1"/>
+      <c r="D69" s="1"/>
+      <c r="E69" s="1"/>
+      <c r="F69" s="1"/>
+      <c r="G69" s="1"/>
+      <c r="H69" s="1"/>
+      <c r="I69" s="1"/>
+      <c r="J69" s="1"/>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A70" s="1"/>
+      <c r="B70" s="1"/>
+      <c r="C70" s="1"/>
+      <c r="D70" s="1"/>
+      <c r="E70" s="1"/>
+      <c r="F70" s="1"/>
+      <c r="G70" s="1"/>
+      <c r="H70" s="1"/>
+      <c r="I70" s="1"/>
+      <c r="J70" s="1"/>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A71" s="1"/>
+      <c r="B71" s="1"/>
+      <c r="C71" s="1"/>
+      <c r="D71" s="1"/>
+      <c r="E71" s="1"/>
+      <c r="F71" s="1"/>
+      <c r="G71" s="1"/>
+      <c r="H71" s="1"/>
+      <c r="I71" s="1"/>
+      <c r="J71" s="1"/>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A72" s="1"/>
+      <c r="B72" s="1"/>
+      <c r="C72" s="1"/>
+      <c r="D72" s="1"/>
+      <c r="E72" s="1"/>
+      <c r="F72" s="1"/>
+      <c r="G72" s="1"/>
+      <c r="H72" s="1"/>
+      <c r="I72" s="1"/>
+      <c r="J72" s="1"/>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A73" s="1"/>
+      <c r="B73" s="1"/>
+      <c r="C73" s="1"/>
+      <c r="D73" s="1"/>
+      <c r="E73" s="1"/>
+      <c r="F73" s="1"/>
+      <c r="G73" s="1"/>
+      <c r="H73" s="1"/>
+      <c r="I73" s="1"/>
+      <c r="J73" s="1"/>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A74" s="1"/>
+      <c r="B74" s="1"/>
+      <c r="C74" s="1"/>
+      <c r="D74" s="1"/>
+      <c r="E74" s="1"/>
+      <c r="F74" s="1"/>
+      <c r="G74" s="1"/>
+      <c r="H74" s="1"/>
+      <c r="I74" s="1"/>
+      <c r="J74" s="1"/>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A75" s="1"/>
+      <c r="B75" s="1"/>
+      <c r="C75" s="1"/>
+      <c r="D75" s="1"/>
+      <c r="E75" s="1"/>
+      <c r="F75" s="1"/>
+      <c r="G75" s="1"/>
+      <c r="H75" s="1"/>
+      <c r="I75" s="1"/>
+      <c r="J75" s="1"/>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A76" s="1"/>
+      <c r="B76" s="1"/>
+      <c r="C76" s="1"/>
+      <c r="D76" s="1"/>
+      <c r="E76" s="1"/>
+      <c r="F76" s="1"/>
+      <c r="G76" s="1"/>
+      <c r="H76" s="1"/>
+      <c r="I76" s="1"/>
+      <c r="J76" s="1"/>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A77" s="1"/>
+      <c r="B77" s="1"/>
+      <c r="C77" s="1"/>
+      <c r="D77" s="1"/>
+      <c r="E77" s="1"/>
+      <c r="F77" s="1"/>
+      <c r="G77" s="1"/>
+      <c r="H77" s="1"/>
+      <c r="I77" s="1"/>
+      <c r="J77" s="1"/>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A78" s="1"/>
+      <c r="B78" s="1"/>
+      <c r="C78" s="1"/>
+      <c r="D78" s="1"/>
+      <c r="E78" s="1"/>
+      <c r="F78" s="1"/>
+      <c r="G78" s="1"/>
+      <c r="H78" s="1"/>
+      <c r="I78" s="1"/>
+      <c r="J78" s="1"/>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A79" s="1"/>
+      <c r="B79" s="1"/>
+      <c r="C79" s="1"/>
+      <c r="D79" s="1"/>
+      <c r="E79" s="1"/>
+      <c r="F79" s="1"/>
+      <c r="G79" s="1"/>
+      <c r="H79" s="1"/>
+      <c r="I79" s="1"/>
+      <c r="J79" s="1"/>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A80" s="1"/>
+      <c r="B80" s="1"/>
+      <c r="C80" s="1"/>
+      <c r="D80" s="1"/>
+      <c r="E80" s="1"/>
+      <c r="F80" s="1"/>
+      <c r="G80" s="1"/>
+      <c r="H80" s="1"/>
+      <c r="I80" s="1"/>
+      <c r="J80" s="1"/>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A81" s="1"/>
+      <c r="B81" s="1"/>
+      <c r="C81" s="1"/>
+      <c r="D81" s="1"/>
+      <c r="E81" s="1"/>
+      <c r="F81" s="1"/>
+      <c r="G81" s="1"/>
+      <c r="H81" s="1"/>
+      <c r="I81" s="1"/>
+      <c r="J81" s="1"/>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A82" s="1"/>
+      <c r="B82" s="1"/>
+      <c r="C82" s="1"/>
+      <c r="D82" s="1"/>
+      <c r="E82" s="1"/>
+      <c r="F82" s="1"/>
+      <c r="G82" s="1"/>
+      <c r="H82" s="1"/>
+      <c r="I82" s="1"/>
+      <c r="J82" s="1"/>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A83" s="1"/>
+      <c r="B83" s="1"/>
+      <c r="C83" s="1"/>
+      <c r="D83" s="1"/>
+      <c r="E83" s="1"/>
+      <c r="F83" s="1"/>
+      <c r="G83" s="1"/>
+      <c r="H83" s="1"/>
+      <c r="I83" s="1"/>
+      <c r="J83" s="1"/>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A84" s="1"/>
+      <c r="B84" s="1"/>
+      <c r="C84" s="1"/>
+      <c r="D84" s="1"/>
+      <c r="E84" s="1"/>
+      <c r="F84" s="1"/>
+      <c r="G84" s="1"/>
+      <c r="H84" s="1"/>
+      <c r="I84" s="1"/>
+      <c r="J84" s="1"/>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A85" s="1"/>
+      <c r="B85" s="1"/>
+      <c r="C85" s="1"/>
+      <c r="D85" s="1"/>
+      <c r="E85" s="1"/>
+      <c r="F85" s="1"/>
+      <c r="G85" s="1"/>
+      <c r="H85" s="1"/>
+      <c r="I85" s="1"/>
+      <c r="J85" s="1"/>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A86" s="1"/>
+      <c r="B86" s="1"/>
+      <c r="C86" s="1"/>
+      <c r="D86" s="1"/>
+      <c r="E86" s="1"/>
+      <c r="F86" s="1"/>
+      <c r="G86" s="1"/>
+      <c r="H86" s="1"/>
+      <c r="I86" s="1"/>
+      <c r="J86" s="1"/>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A87" s="1"/>
+      <c r="B87" s="1"/>
+      <c r="C87" s="1"/>
+      <c r="D87" s="1"/>
+      <c r="E87" s="1"/>
+      <c r="F87" s="1"/>
+      <c r="G87" s="1"/>
+      <c r="H87" s="1"/>
+      <c r="I87" s="1"/>
+      <c r="J87" s="1"/>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A88" s="1"/>
+      <c r="B88" s="1"/>
+      <c r="C88" s="1"/>
+      <c r="D88" s="1"/>
+      <c r="E88" s="1"/>
+      <c r="F88" s="1"/>
+      <c r="G88" s="1"/>
+      <c r="H88" s="1"/>
+      <c r="I88" s="1"/>
+      <c r="J88" s="1"/>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A89" s="1"/>
+      <c r="B89" s="1"/>
+      <c r="C89" s="1"/>
+      <c r="D89" s="1"/>
+      <c r="E89" s="1"/>
+      <c r="F89" s="1"/>
+      <c r="G89" s="1"/>
+      <c r="H89" s="1"/>
+      <c r="I89" s="1"/>
+      <c r="J89" s="1"/>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A90" s="1"/>
+      <c r="B90" s="1"/>
+      <c r="C90" s="1"/>
+      <c r="D90" s="1"/>
+      <c r="E90" s="1"/>
+      <c r="F90" s="1"/>
+      <c r="G90" s="1"/>
+      <c r="H90" s="1"/>
+      <c r="I90" s="1"/>
+      <c r="J90" s="1"/>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A91" s="1"/>
+      <c r="B91" s="1"/>
+      <c r="C91" s="1"/>
+      <c r="D91" s="1"/>
+      <c r="E91" s="1"/>
+      <c r="F91" s="1"/>
+      <c r="G91" s="1"/>
+      <c r="H91" s="1"/>
+      <c r="I91" s="1"/>
+      <c r="J91" s="1"/>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A92" s="1"/>
+      <c r="B92" s="1"/>
+      <c r="C92" s="1"/>
+      <c r="D92" s="1"/>
+      <c r="E92" s="1"/>
+      <c r="F92" s="1"/>
+      <c r="G92" s="1"/>
+      <c r="H92" s="1"/>
+      <c r="I92" s="1"/>
+      <c r="J92" s="1"/>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A93" s="1"/>
+      <c r="B93" s="1"/>
+      <c r="C93" s="1"/>
+      <c r="D93" s="1"/>
+      <c r="E93" s="1"/>
+      <c r="F93" s="1"/>
+      <c r="G93" s="1"/>
+      <c r="H93" s="1"/>
+      <c r="I93" s="1"/>
+      <c r="J93" s="1"/>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A94" s="1"/>
+      <c r="B94" s="1"/>
+      <c r="C94" s="1"/>
+      <c r="D94" s="1"/>
+      <c r="E94" s="1"/>
+      <c r="F94" s="1"/>
+      <c r="G94" s="1"/>
+      <c r="H94" s="1"/>
+      <c r="I94" s="1"/>
+      <c r="J94" s="1"/>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A95" s="1"/>
+      <c r="B95" s="1"/>
+      <c r="C95" s="1"/>
+      <c r="D95" s="1"/>
+      <c r="E95" s="1"/>
+      <c r="F95" s="1"/>
+      <c r="G95" s="1"/>
+      <c r="H95" s="1"/>
+      <c r="I95" s="1"/>
+      <c r="J95" s="1"/>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A96" s="1"/>
+      <c r="B96" s="1"/>
+      <c r="C96" s="1"/>
+      <c r="D96" s="1"/>
+      <c r="E96" s="1"/>
+      <c r="F96" s="1"/>
+      <c r="G96" s="1"/>
+      <c r="H96" s="1"/>
+      <c r="I96" s="1"/>
+      <c r="J96" s="1"/>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A97" s="1"/>
+      <c r="B97" s="1"/>
+      <c r="C97" s="1"/>
+      <c r="D97" s="1"/>
+      <c r="E97" s="1"/>
+      <c r="F97" s="1"/>
+      <c r="G97" s="1"/>
+      <c r="H97" s="1"/>
+      <c r="I97" s="1"/>
+      <c r="J97" s="1"/>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A98" s="1"/>
+      <c r="B98" s="1"/>
+      <c r="C98" s="1"/>
+      <c r="D98" s="1"/>
+      <c r="E98" s="1"/>
+      <c r="F98" s="1"/>
+      <c r="G98" s="1"/>
+      <c r="H98" s="1"/>
+      <c r="I98" s="1"/>
+      <c r="J98" s="1"/>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A99" s="1"/>
+      <c r="B99" s="1"/>
+      <c r="C99" s="1"/>
+      <c r="D99" s="1"/>
+      <c r="E99" s="1"/>
+      <c r="F99" s="1"/>
+      <c r="G99" s="1"/>
+      <c r="H99" s="1"/>
+      <c r="I99" s="1"/>
+      <c r="J99" s="1"/>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A100" s="1"/>
+      <c r="B100" s="1"/>
+      <c r="C100" s="1"/>
+      <c r="D100" s="1"/>
+      <c r="E100" s="1"/>
+      <c r="F100" s="1"/>
+      <c r="G100" s="1"/>
+      <c r="H100" s="1"/>
+      <c r="I100" s="1"/>
+      <c r="J100" s="1"/>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A101" s="1"/>
+      <c r="B101" s="1"/>
+      <c r="C101" s="1"/>
+      <c r="D101" s="1"/>
+      <c r="E101" s="1"/>
+      <c r="F101" s="1"/>
+      <c r="G101" s="1"/>
+      <c r="H101" s="1"/>
+      <c r="I101" s="1"/>
+      <c r="J101" s="1"/>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A102" s="1"/>
+      <c r="B102" s="1"/>
+      <c r="C102" s="1"/>
+      <c r="D102" s="1"/>
+      <c r="E102" s="1"/>
+      <c r="F102" s="1"/>
+      <c r="G102" s="1"/>
+      <c r="H102" s="1"/>
+      <c r="I102" s="1"/>
+      <c r="J102" s="1"/>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A103" s="1"/>
+      <c r="B103" s="1"/>
+      <c r="C103" s="1"/>
+      <c r="D103" s="1"/>
+      <c r="E103" s="1"/>
+      <c r="F103" s="1"/>
+      <c r="G103" s="1"/>
+      <c r="H103" s="1"/>
+      <c r="I103" s="1"/>
+      <c r="J103" s="1"/>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A104" s="1"/>
+      <c r="B104" s="1"/>
+      <c r="C104" s="1"/>
+      <c r="D104" s="1"/>
+      <c r="E104" s="1"/>
+      <c r="F104" s="1"/>
+      <c r="G104" s="1"/>
+      <c r="H104" s="1"/>
+      <c r="I104" s="1"/>
+      <c r="J104" s="1"/>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A105" s="1"/>
+      <c r="B105" s="1"/>
+      <c r="C105" s="1"/>
+      <c r="D105" s="1"/>
+      <c r="E105" s="1"/>
+      <c r="F105" s="1"/>
+      <c r="G105" s="1"/>
+      <c r="H105" s="1"/>
+      <c r="I105" s="1"/>
+      <c r="J105" s="1"/>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A106" s="1"/>
+      <c r="B106" s="1"/>
+      <c r="C106" s="1"/>
+      <c r="D106" s="1"/>
+      <c r="E106" s="1"/>
+      <c r="F106" s="1"/>
+      <c r="G106" s="1"/>
+      <c r="H106" s="1"/>
+      <c r="I106" s="1"/>
+      <c r="J106" s="1"/>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A107" s="1"/>
+      <c r="B107" s="1"/>
+      <c r="C107" s="1"/>
+      <c r="D107" s="1"/>
+      <c r="E107" s="1"/>
+      <c r="F107" s="1"/>
+      <c r="G107" s="1"/>
+      <c r="H107" s="1"/>
+      <c r="I107" s="1"/>
+      <c r="J107" s="1"/>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A108" s="1"/>
+      <c r="B108" s="1"/>
+      <c r="C108" s="1"/>
+      <c r="D108" s="1"/>
+      <c r="E108" s="1"/>
+      <c r="F108" s="1"/>
+      <c r="G108" s="1"/>
+      <c r="H108" s="1"/>
+      <c r="I108" s="1"/>
+      <c r="J108" s="1"/>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A109" s="1"/>
+      <c r="B109" s="1"/>
+      <c r="C109" s="1"/>
+      <c r="D109" s="1"/>
+      <c r="E109" s="1"/>
+      <c r="F109" s="1"/>
+      <c r="G109" s="1"/>
+      <c r="H109" s="1"/>
+      <c r="I109" s="1"/>
+      <c r="J109" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB1D795D-554E-4B31-8732-D7CC78219987}">
   <dimension ref="A1:I25"/>
   <sheetViews>
@@ -2677,7 +4090,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{919B2633-F7CB-4C36-8605-E7950C491D12}">
   <dimension ref="A1:W22"/>
   <sheetViews>
@@ -4277,1417 +5690,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{412D6C35-5CAD-470C-B537-E441B956C3CF}">
-  <dimension ref="A1:O109"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="52.6640625" customWidth="1"/>
-    <col min="2" max="2" width="47.6640625" customWidth="1"/>
-    <col min="3" max="3" width="21.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="47.6640625" customWidth="1"/>
-    <col min="5" max="5" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="26.6640625" customWidth="1"/>
-    <col min="8" max="8" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.6640625" customWidth="1"/>
-    <col min="10" max="12" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="26.109375" customWidth="1"/>
-    <col min="14" max="14" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="34.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C1" t="s">
-        <v>168</v>
-      </c>
-      <c r="D1" t="s">
-        <v>164</v>
-      </c>
-      <c r="E1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F1" t="s">
-        <v>170</v>
-      </c>
-      <c r="G1" t="s">
-        <v>165</v>
-      </c>
-      <c r="H1" t="s">
-        <v>48</v>
-      </c>
-      <c r="I1" t="s">
-        <v>172</v>
-      </c>
-      <c r="J1" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-    </row>
-    <row r="3" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="M3" s="1"/>
-      <c r="O3" s="1"/>
-    </row>
-    <row r="4" spans="1:15" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
-      <c r="J31" s="1"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
-      <c r="J32" s="1"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
-      <c r="I33" s="1"/>
-      <c r="J33" s="1"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
-      <c r="H35" s="1"/>
-      <c r="I35" s="1"/>
-      <c r="J35" s="1"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
-      <c r="I36" s="1"/>
-      <c r="J36" s="1"/>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
-      <c r="I37" s="1"/>
-      <c r="J37" s="1"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
-      <c r="H38" s="1"/>
-      <c r="I38" s="1"/>
-      <c r="J38" s="1"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
-      <c r="I39" s="1"/>
-      <c r="J39" s="1"/>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A40" s="1"/>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
-      <c r="H40" s="1"/>
-      <c r="I40" s="1"/>
-      <c r="J40" s="1"/>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
-      <c r="H41" s="1"/>
-      <c r="I41" s="1"/>
-      <c r="J41" s="1"/>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A42" s="1"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-      <c r="F42" s="1"/>
-      <c r="G42" s="1"/>
-      <c r="H42" s="1"/>
-      <c r="I42" s="1"/>
-      <c r="J42" s="1"/>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
-      <c r="F43" s="1"/>
-      <c r="G43" s="1"/>
-      <c r="H43" s="1"/>
-      <c r="I43" s="1"/>
-      <c r="J43" s="1"/>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A44" s="1"/>
-      <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
-      <c r="G44" s="1"/>
-      <c r="H44" s="1"/>
-      <c r="I44" s="1"/>
-      <c r="J44" s="1"/>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A45" s="1"/>
-      <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
-      <c r="D45" s="1"/>
-      <c r="E45" s="1"/>
-      <c r="F45" s="1"/>
-      <c r="G45" s="1"/>
-      <c r="H45" s="1"/>
-      <c r="I45" s="1"/>
-      <c r="J45" s="1"/>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A46" s="1"/>
-      <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
-      <c r="F46" s="1"/>
-      <c r="G46" s="1"/>
-      <c r="H46" s="1"/>
-      <c r="I46" s="1"/>
-      <c r="J46" s="1"/>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A47" s="1"/>
-      <c r="B47" s="1"/>
-      <c r="C47" s="1"/>
-      <c r="D47" s="1"/>
-      <c r="E47" s="1"/>
-      <c r="F47" s="1"/>
-      <c r="G47" s="1"/>
-      <c r="H47" s="1"/>
-      <c r="I47" s="1"/>
-      <c r="J47" s="1"/>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A48" s="1"/>
-      <c r="B48" s="1"/>
-      <c r="C48" s="1"/>
-      <c r="D48" s="1"/>
-      <c r="E48" s="1"/>
-      <c r="F48" s="1"/>
-      <c r="G48" s="1"/>
-      <c r="H48" s="1"/>
-      <c r="I48" s="1"/>
-      <c r="J48" s="1"/>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A49" s="1"/>
-      <c r="B49" s="1"/>
-      <c r="C49" s="1"/>
-      <c r="D49" s="1"/>
-      <c r="E49" s="1"/>
-      <c r="F49" s="1"/>
-      <c r="G49" s="1"/>
-      <c r="H49" s="1"/>
-      <c r="I49" s="1"/>
-      <c r="J49" s="1"/>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A50" s="1"/>
-      <c r="B50" s="1"/>
-      <c r="C50" s="1"/>
-      <c r="D50" s="1"/>
-      <c r="E50" s="1"/>
-      <c r="F50" s="1"/>
-      <c r="G50" s="1"/>
-      <c r="H50" s="1"/>
-      <c r="I50" s="1"/>
-      <c r="J50" s="1"/>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A51" s="1"/>
-      <c r="B51" s="1"/>
-      <c r="C51" s="1"/>
-      <c r="D51" s="1"/>
-      <c r="E51" s="1"/>
-      <c r="F51" s="1"/>
-      <c r="G51" s="1"/>
-      <c r="H51" s="1"/>
-      <c r="I51" s="1"/>
-      <c r="J51" s="1"/>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A52" s="1"/>
-      <c r="B52" s="1"/>
-      <c r="C52" s="1"/>
-      <c r="D52" s="1"/>
-      <c r="E52" s="1"/>
-      <c r="F52" s="1"/>
-      <c r="G52" s="1"/>
-      <c r="H52" s="1"/>
-      <c r="I52" s="1"/>
-      <c r="J52" s="1"/>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A53" s="1"/>
-      <c r="B53" s="1"/>
-      <c r="C53" s="1"/>
-      <c r="D53" s="1"/>
-      <c r="E53" s="1"/>
-      <c r="F53" s="1"/>
-      <c r="G53" s="1"/>
-      <c r="H53" s="1"/>
-      <c r="I53" s="1"/>
-      <c r="J53" s="1"/>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A54" s="1"/>
-      <c r="B54" s="1"/>
-      <c r="C54" s="1"/>
-      <c r="D54" s="1"/>
-      <c r="E54" s="1"/>
-      <c r="F54" s="1"/>
-      <c r="G54" s="1"/>
-      <c r="H54" s="1"/>
-      <c r="I54" s="1"/>
-      <c r="J54" s="1"/>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A55" s="1"/>
-      <c r="B55" s="1"/>
-      <c r="C55" s="1"/>
-      <c r="D55" s="1"/>
-      <c r="E55" s="1"/>
-      <c r="F55" s="1"/>
-      <c r="G55" s="1"/>
-      <c r="H55" s="1"/>
-      <c r="I55" s="1"/>
-      <c r="J55" s="1"/>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A56" s="1"/>
-      <c r="B56" s="1"/>
-      <c r="C56" s="1"/>
-      <c r="D56" s="1"/>
-      <c r="E56" s="1"/>
-      <c r="F56" s="1"/>
-      <c r="G56" s="1"/>
-      <c r="H56" s="1"/>
-      <c r="I56" s="1"/>
-      <c r="J56" s="1"/>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A57" s="1"/>
-      <c r="B57" s="1"/>
-      <c r="C57" s="1"/>
-      <c r="D57" s="1"/>
-      <c r="E57" s="1"/>
-      <c r="F57" s="1"/>
-      <c r="G57" s="1"/>
-      <c r="H57" s="1"/>
-      <c r="I57" s="1"/>
-      <c r="J57" s="1"/>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A58" s="1"/>
-      <c r="B58" s="1"/>
-      <c r="C58" s="1"/>
-      <c r="D58" s="1"/>
-      <c r="E58" s="1"/>
-      <c r="F58" s="1"/>
-      <c r="G58" s="1"/>
-      <c r="H58" s="1"/>
-      <c r="I58" s="1"/>
-      <c r="J58" s="1"/>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A59" s="1"/>
-      <c r="B59" s="1"/>
-      <c r="C59" s="1"/>
-      <c r="D59" s="1"/>
-      <c r="E59" s="1"/>
-      <c r="F59" s="1"/>
-      <c r="G59" s="1"/>
-      <c r="H59" s="1"/>
-      <c r="I59" s="1"/>
-      <c r="J59" s="1"/>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A60" s="1"/>
-      <c r="B60" s="1"/>
-      <c r="C60" s="1"/>
-      <c r="D60" s="1"/>
-      <c r="E60" s="1"/>
-      <c r="F60" s="1"/>
-      <c r="G60" s="1"/>
-      <c r="H60" s="1"/>
-      <c r="I60" s="1"/>
-      <c r="J60" s="1"/>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A61" s="1"/>
-      <c r="B61" s="1"/>
-      <c r="C61" s="1"/>
-      <c r="D61" s="1"/>
-      <c r="E61" s="1"/>
-      <c r="F61" s="1"/>
-      <c r="G61" s="1"/>
-      <c r="H61" s="1"/>
-      <c r="I61" s="1"/>
-      <c r="J61" s="1"/>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A62" s="1"/>
-      <c r="B62" s="1"/>
-      <c r="C62" s="1"/>
-      <c r="D62" s="1"/>
-      <c r="E62" s="1"/>
-      <c r="F62" s="1"/>
-      <c r="G62" s="1"/>
-      <c r="H62" s="1"/>
-      <c r="I62" s="1"/>
-      <c r="J62" s="1"/>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A63" s="1"/>
-      <c r="B63" s="1"/>
-      <c r="C63" s="1"/>
-      <c r="D63" s="1"/>
-      <c r="E63" s="1"/>
-      <c r="F63" s="1"/>
-      <c r="G63" s="1"/>
-      <c r="H63" s="1"/>
-      <c r="I63" s="1"/>
-      <c r="J63" s="1"/>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A64" s="1"/>
-      <c r="B64" s="1"/>
-      <c r="C64" s="1"/>
-      <c r="D64" s="1"/>
-      <c r="E64" s="1"/>
-      <c r="F64" s="1"/>
-      <c r="G64" s="1"/>
-      <c r="H64" s="1"/>
-      <c r="I64" s="1"/>
-      <c r="J64" s="1"/>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A65" s="1"/>
-      <c r="B65" s="1"/>
-      <c r="C65" s="1"/>
-      <c r="D65" s="1"/>
-      <c r="E65" s="1"/>
-      <c r="F65" s="1"/>
-      <c r="G65" s="1"/>
-      <c r="H65" s="1"/>
-      <c r="I65" s="1"/>
-      <c r="J65" s="1"/>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A66" s="1"/>
-      <c r="B66" s="1"/>
-      <c r="C66" s="1"/>
-      <c r="D66" s="1"/>
-      <c r="E66" s="1"/>
-      <c r="F66" s="1"/>
-      <c r="G66" s="1"/>
-      <c r="H66" s="1"/>
-      <c r="I66" s="1"/>
-      <c r="J66" s="1"/>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A67" s="1"/>
-      <c r="B67" s="1"/>
-      <c r="C67" s="1"/>
-      <c r="D67" s="1"/>
-      <c r="E67" s="1"/>
-      <c r="F67" s="1"/>
-      <c r="G67" s="1"/>
-      <c r="H67" s="1"/>
-      <c r="I67" s="1"/>
-      <c r="J67" s="1"/>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A68" s="1"/>
-      <c r="B68" s="1"/>
-      <c r="C68" s="1"/>
-      <c r="D68" s="1"/>
-      <c r="E68" s="1"/>
-      <c r="F68" s="1"/>
-      <c r="G68" s="1"/>
-      <c r="H68" s="1"/>
-      <c r="I68" s="1"/>
-      <c r="J68" s="1"/>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A69" s="1"/>
-      <c r="B69" s="1"/>
-      <c r="C69" s="1"/>
-      <c r="D69" s="1"/>
-      <c r="E69" s="1"/>
-      <c r="F69" s="1"/>
-      <c r="G69" s="1"/>
-      <c r="H69" s="1"/>
-      <c r="I69" s="1"/>
-      <c r="J69" s="1"/>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A70" s="1"/>
-      <c r="B70" s="1"/>
-      <c r="C70" s="1"/>
-      <c r="D70" s="1"/>
-      <c r="E70" s="1"/>
-      <c r="F70" s="1"/>
-      <c r="G70" s="1"/>
-      <c r="H70" s="1"/>
-      <c r="I70" s="1"/>
-      <c r="J70" s="1"/>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A71" s="1"/>
-      <c r="B71" s="1"/>
-      <c r="C71" s="1"/>
-      <c r="D71" s="1"/>
-      <c r="E71" s="1"/>
-      <c r="F71" s="1"/>
-      <c r="G71" s="1"/>
-      <c r="H71" s="1"/>
-      <c r="I71" s="1"/>
-      <c r="J71" s="1"/>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A72" s="1"/>
-      <c r="B72" s="1"/>
-      <c r="C72" s="1"/>
-      <c r="D72" s="1"/>
-      <c r="E72" s="1"/>
-      <c r="F72" s="1"/>
-      <c r="G72" s="1"/>
-      <c r="H72" s="1"/>
-      <c r="I72" s="1"/>
-      <c r="J72" s="1"/>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A73" s="1"/>
-      <c r="B73" s="1"/>
-      <c r="C73" s="1"/>
-      <c r="D73" s="1"/>
-      <c r="E73" s="1"/>
-      <c r="F73" s="1"/>
-      <c r="G73" s="1"/>
-      <c r="H73" s="1"/>
-      <c r="I73" s="1"/>
-      <c r="J73" s="1"/>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A74" s="1"/>
-      <c r="B74" s="1"/>
-      <c r="C74" s="1"/>
-      <c r="D74" s="1"/>
-      <c r="E74" s="1"/>
-      <c r="F74" s="1"/>
-      <c r="G74" s="1"/>
-      <c r="H74" s="1"/>
-      <c r="I74" s="1"/>
-      <c r="J74" s="1"/>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A75" s="1"/>
-      <c r="B75" s="1"/>
-      <c r="C75" s="1"/>
-      <c r="D75" s="1"/>
-      <c r="E75" s="1"/>
-      <c r="F75" s="1"/>
-      <c r="G75" s="1"/>
-      <c r="H75" s="1"/>
-      <c r="I75" s="1"/>
-      <c r="J75" s="1"/>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A76" s="1"/>
-      <c r="B76" s="1"/>
-      <c r="C76" s="1"/>
-      <c r="D76" s="1"/>
-      <c r="E76" s="1"/>
-      <c r="F76" s="1"/>
-      <c r="G76" s="1"/>
-      <c r="H76" s="1"/>
-      <c r="I76" s="1"/>
-      <c r="J76" s="1"/>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A77" s="1"/>
-      <c r="B77" s="1"/>
-      <c r="C77" s="1"/>
-      <c r="D77" s="1"/>
-      <c r="E77" s="1"/>
-      <c r="F77" s="1"/>
-      <c r="G77" s="1"/>
-      <c r="H77" s="1"/>
-      <c r="I77" s="1"/>
-      <c r="J77" s="1"/>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A78" s="1"/>
-      <c r="B78" s="1"/>
-      <c r="C78" s="1"/>
-      <c r="D78" s="1"/>
-      <c r="E78" s="1"/>
-      <c r="F78" s="1"/>
-      <c r="G78" s="1"/>
-      <c r="H78" s="1"/>
-      <c r="I78" s="1"/>
-      <c r="J78" s="1"/>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A79" s="1"/>
-      <c r="B79" s="1"/>
-      <c r="C79" s="1"/>
-      <c r="D79" s="1"/>
-      <c r="E79" s="1"/>
-      <c r="F79" s="1"/>
-      <c r="G79" s="1"/>
-      <c r="H79" s="1"/>
-      <c r="I79" s="1"/>
-      <c r="J79" s="1"/>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A80" s="1"/>
-      <c r="B80" s="1"/>
-      <c r="C80" s="1"/>
-      <c r="D80" s="1"/>
-      <c r="E80" s="1"/>
-      <c r="F80" s="1"/>
-      <c r="G80" s="1"/>
-      <c r="H80" s="1"/>
-      <c r="I80" s="1"/>
-      <c r="J80" s="1"/>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A81" s="1"/>
-      <c r="B81" s="1"/>
-      <c r="C81" s="1"/>
-      <c r="D81" s="1"/>
-      <c r="E81" s="1"/>
-      <c r="F81" s="1"/>
-      <c r="G81" s="1"/>
-      <c r="H81" s="1"/>
-      <c r="I81" s="1"/>
-      <c r="J81" s="1"/>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A82" s="1"/>
-      <c r="B82" s="1"/>
-      <c r="C82" s="1"/>
-      <c r="D82" s="1"/>
-      <c r="E82" s="1"/>
-      <c r="F82" s="1"/>
-      <c r="G82" s="1"/>
-      <c r="H82" s="1"/>
-      <c r="I82" s="1"/>
-      <c r="J82" s="1"/>
-    </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A83" s="1"/>
-      <c r="B83" s="1"/>
-      <c r="C83" s="1"/>
-      <c r="D83" s="1"/>
-      <c r="E83" s="1"/>
-      <c r="F83" s="1"/>
-      <c r="G83" s="1"/>
-      <c r="H83" s="1"/>
-      <c r="I83" s="1"/>
-      <c r="J83" s="1"/>
-    </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A84" s="1"/>
-      <c r="B84" s="1"/>
-      <c r="C84" s="1"/>
-      <c r="D84" s="1"/>
-      <c r="E84" s="1"/>
-      <c r="F84" s="1"/>
-      <c r="G84" s="1"/>
-      <c r="H84" s="1"/>
-      <c r="I84" s="1"/>
-      <c r="J84" s="1"/>
-    </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A85" s="1"/>
-      <c r="B85" s="1"/>
-      <c r="C85" s="1"/>
-      <c r="D85" s="1"/>
-      <c r="E85" s="1"/>
-      <c r="F85" s="1"/>
-      <c r="G85" s="1"/>
-      <c r="H85" s="1"/>
-      <c r="I85" s="1"/>
-      <c r="J85" s="1"/>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A86" s="1"/>
-      <c r="B86" s="1"/>
-      <c r="C86" s="1"/>
-      <c r="D86" s="1"/>
-      <c r="E86" s="1"/>
-      <c r="F86" s="1"/>
-      <c r="G86" s="1"/>
-      <c r="H86" s="1"/>
-      <c r="I86" s="1"/>
-      <c r="J86" s="1"/>
-    </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A87" s="1"/>
-      <c r="B87" s="1"/>
-      <c r="C87" s="1"/>
-      <c r="D87" s="1"/>
-      <c r="E87" s="1"/>
-      <c r="F87" s="1"/>
-      <c r="G87" s="1"/>
-      <c r="H87" s="1"/>
-      <c r="I87" s="1"/>
-      <c r="J87" s="1"/>
-    </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A88" s="1"/>
-      <c r="B88" s="1"/>
-      <c r="C88" s="1"/>
-      <c r="D88" s="1"/>
-      <c r="E88" s="1"/>
-      <c r="F88" s="1"/>
-      <c r="G88" s="1"/>
-      <c r="H88" s="1"/>
-      <c r="I88" s="1"/>
-      <c r="J88" s="1"/>
-    </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A89" s="1"/>
-      <c r="B89" s="1"/>
-      <c r="C89" s="1"/>
-      <c r="D89" s="1"/>
-      <c r="E89" s="1"/>
-      <c r="F89" s="1"/>
-      <c r="G89" s="1"/>
-      <c r="H89" s="1"/>
-      <c r="I89" s="1"/>
-      <c r="J89" s="1"/>
-    </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A90" s="1"/>
-      <c r="B90" s="1"/>
-      <c r="C90" s="1"/>
-      <c r="D90" s="1"/>
-      <c r="E90" s="1"/>
-      <c r="F90" s="1"/>
-      <c r="G90" s="1"/>
-      <c r="H90" s="1"/>
-      <c r="I90" s="1"/>
-      <c r="J90" s="1"/>
-    </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A91" s="1"/>
-      <c r="B91" s="1"/>
-      <c r="C91" s="1"/>
-      <c r="D91" s="1"/>
-      <c r="E91" s="1"/>
-      <c r="F91" s="1"/>
-      <c r="G91" s="1"/>
-      <c r="H91" s="1"/>
-      <c r="I91" s="1"/>
-      <c r="J91" s="1"/>
-    </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A92" s="1"/>
-      <c r="B92" s="1"/>
-      <c r="C92" s="1"/>
-      <c r="D92" s="1"/>
-      <c r="E92" s="1"/>
-      <c r="F92" s="1"/>
-      <c r="G92" s="1"/>
-      <c r="H92" s="1"/>
-      <c r="I92" s="1"/>
-      <c r="J92" s="1"/>
-    </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A93" s="1"/>
-      <c r="B93" s="1"/>
-      <c r="C93" s="1"/>
-      <c r="D93" s="1"/>
-      <c r="E93" s="1"/>
-      <c r="F93" s="1"/>
-      <c r="G93" s="1"/>
-      <c r="H93" s="1"/>
-      <c r="I93" s="1"/>
-      <c r="J93" s="1"/>
-    </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A94" s="1"/>
-      <c r="B94" s="1"/>
-      <c r="C94" s="1"/>
-      <c r="D94" s="1"/>
-      <c r="E94" s="1"/>
-      <c r="F94" s="1"/>
-      <c r="G94" s="1"/>
-      <c r="H94" s="1"/>
-      <c r="I94" s="1"/>
-      <c r="J94" s="1"/>
-    </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A95" s="1"/>
-      <c r="B95" s="1"/>
-      <c r="C95" s="1"/>
-      <c r="D95" s="1"/>
-      <c r="E95" s="1"/>
-      <c r="F95" s="1"/>
-      <c r="G95" s="1"/>
-      <c r="H95" s="1"/>
-      <c r="I95" s="1"/>
-      <c r="J95" s="1"/>
-    </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A96" s="1"/>
-      <c r="B96" s="1"/>
-      <c r="C96" s="1"/>
-      <c r="D96" s="1"/>
-      <c r="E96" s="1"/>
-      <c r="F96" s="1"/>
-      <c r="G96" s="1"/>
-      <c r="H96" s="1"/>
-      <c r="I96" s="1"/>
-      <c r="J96" s="1"/>
-    </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A97" s="1"/>
-      <c r="B97" s="1"/>
-      <c r="C97" s="1"/>
-      <c r="D97" s="1"/>
-      <c r="E97" s="1"/>
-      <c r="F97" s="1"/>
-      <c r="G97" s="1"/>
-      <c r="H97" s="1"/>
-      <c r="I97" s="1"/>
-      <c r="J97" s="1"/>
-    </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A98" s="1"/>
-      <c r="B98" s="1"/>
-      <c r="C98" s="1"/>
-      <c r="D98" s="1"/>
-      <c r="E98" s="1"/>
-      <c r="F98" s="1"/>
-      <c r="G98" s="1"/>
-      <c r="H98" s="1"/>
-      <c r="I98" s="1"/>
-      <c r="J98" s="1"/>
-    </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A99" s="1"/>
-      <c r="B99" s="1"/>
-      <c r="C99" s="1"/>
-      <c r="D99" s="1"/>
-      <c r="E99" s="1"/>
-      <c r="F99" s="1"/>
-      <c r="G99" s="1"/>
-      <c r="H99" s="1"/>
-      <c r="I99" s="1"/>
-      <c r="J99" s="1"/>
-    </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A100" s="1"/>
-      <c r="B100" s="1"/>
-      <c r="C100" s="1"/>
-      <c r="D100" s="1"/>
-      <c r="E100" s="1"/>
-      <c r="F100" s="1"/>
-      <c r="G100" s="1"/>
-      <c r="H100" s="1"/>
-      <c r="I100" s="1"/>
-      <c r="J100" s="1"/>
-    </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A101" s="1"/>
-      <c r="B101" s="1"/>
-      <c r="C101" s="1"/>
-      <c r="D101" s="1"/>
-      <c r="E101" s="1"/>
-      <c r="F101" s="1"/>
-      <c r="G101" s="1"/>
-      <c r="H101" s="1"/>
-      <c r="I101" s="1"/>
-      <c r="J101" s="1"/>
-    </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A102" s="1"/>
-      <c r="B102" s="1"/>
-      <c r="C102" s="1"/>
-      <c r="D102" s="1"/>
-      <c r="E102" s="1"/>
-      <c r="F102" s="1"/>
-      <c r="G102" s="1"/>
-      <c r="H102" s="1"/>
-      <c r="I102" s="1"/>
-      <c r="J102" s="1"/>
-    </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A103" s="1"/>
-      <c r="B103" s="1"/>
-      <c r="C103" s="1"/>
-      <c r="D103" s="1"/>
-      <c r="E103" s="1"/>
-      <c r="F103" s="1"/>
-      <c r="G103" s="1"/>
-      <c r="H103" s="1"/>
-      <c r="I103" s="1"/>
-      <c r="J103" s="1"/>
-    </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A104" s="1"/>
-      <c r="B104" s="1"/>
-      <c r="C104" s="1"/>
-      <c r="D104" s="1"/>
-      <c r="E104" s="1"/>
-      <c r="F104" s="1"/>
-      <c r="G104" s="1"/>
-      <c r="H104" s="1"/>
-      <c r="I104" s="1"/>
-      <c r="J104" s="1"/>
-    </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A105" s="1"/>
-      <c r="B105" s="1"/>
-      <c r="C105" s="1"/>
-      <c r="D105" s="1"/>
-      <c r="E105" s="1"/>
-      <c r="F105" s="1"/>
-      <c r="G105" s="1"/>
-      <c r="H105" s="1"/>
-      <c r="I105" s="1"/>
-      <c r="J105" s="1"/>
-    </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A106" s="1"/>
-      <c r="B106" s="1"/>
-      <c r="C106" s="1"/>
-      <c r="D106" s="1"/>
-      <c r="E106" s="1"/>
-      <c r="F106" s="1"/>
-      <c r="G106" s="1"/>
-      <c r="H106" s="1"/>
-      <c r="I106" s="1"/>
-      <c r="J106" s="1"/>
-    </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A107" s="1"/>
-      <c r="B107" s="1"/>
-      <c r="C107" s="1"/>
-      <c r="D107" s="1"/>
-      <c r="E107" s="1"/>
-      <c r="F107" s="1"/>
-      <c r="G107" s="1"/>
-      <c r="H107" s="1"/>
-      <c r="I107" s="1"/>
-      <c r="J107" s="1"/>
-    </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A108" s="1"/>
-      <c r="B108" s="1"/>
-      <c r="C108" s="1"/>
-      <c r="D108" s="1"/>
-      <c r="E108" s="1"/>
-      <c r="F108" s="1"/>
-      <c r="G108" s="1"/>
-      <c r="H108" s="1"/>
-      <c r="I108" s="1"/>
-      <c r="J108" s="1"/>
-    </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A109" s="1"/>
-      <c r="B109" s="1"/>
-      <c r="C109" s="1"/>
-      <c r="D109" s="1"/>
-      <c r="E109" s="1"/>
-      <c r="F109" s="1"/>
-      <c r="G109" s="1"/>
-      <c r="H109" s="1"/>
-      <c r="I109" s="1"/>
-      <c r="J109" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Update data viz (lots of improvements) and age misassignment scripts
</commit_message>
<xml_diff>
--- a/Simulation_log_key.xlsx
+++ b/Simulation_log_key.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\Documents\R\working_directory\LemonSharkCKMR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CE8F7E1-683D-43F9-91A9-861B42F4F6C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E935F37-81B2-47DC-A970-01C5AA8D7762}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5085" yWindow="-11640" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="204">
   <si>
     <t>Objective</t>
   </si>
@@ -492,9 +492,6 @@
     <t>Obj2.2.2_lambda.trial_target.YOY_stablePopSimLambda_change.est.yr</t>
   </si>
   <si>
-    <t>scenario_4.2</t>
-  </si>
-  <si>
     <t>scenario_2.3.1</t>
   </si>
   <si>
@@ -552,12 +549,6 @@
     <t>Biennial breeding; biennial model; lambda in model w/ tight prior; no non-conformists</t>
   </si>
   <si>
-    <t>Aging error; biennial breeding; biennial model; lambda in model w/ wide prior; no non-conformists</t>
-  </si>
-  <si>
-    <t>Aging error; biennial breeding; biennial model; lambda in model w/ tight prior; no non-conformists</t>
-  </si>
-  <si>
     <t>Model validation</t>
   </si>
   <si>
@@ -642,12 +633,6 @@
     <t>scenario_3.2.3</t>
   </si>
   <si>
-    <t>scenario_4.3</t>
-  </si>
-  <si>
-    <t>Aging error; biennial breeding; biennial model; no lambda in model; no non-conformists</t>
-  </si>
-  <si>
     <t>Still need to download</t>
   </si>
   <si>
@@ -658,6 +643,48 @@
   </si>
   <si>
     <t>Small population change; lambda in model w/ tight prior - for stable scenario for all ages and YOY, used results from scenario_1.2</t>
+  </si>
+  <si>
+    <t>scenario_4.1.1</t>
+  </si>
+  <si>
+    <t>scenario_4.1.2</t>
+  </si>
+  <si>
+    <t>scenario_4.1.3</t>
+  </si>
+  <si>
+    <t>Aging error; biennial breeding; biennial model; lambda in model w/ wide prior; no non-conformists;
+aging error 5% CV</t>
+  </si>
+  <si>
+    <t>Aging error; biennial breeding; biennial model; lambda in model w/ tight prior; no non-conformists;
+aging error 5% CV</t>
+  </si>
+  <si>
+    <t>Aging error; biennial breeding; biennial model; no lambda in model; no non-conformists;
+aging error 5% CV</t>
+  </si>
+  <si>
+    <t>Aging error; biennial breeding; biennial model; lambda in model w/ wide prior; no non-conformists;
+aging error 10% CV</t>
+  </si>
+  <si>
+    <t>Aging error; biennial breeding; biennial model; lambda in model w/ tight prior; no non-conformists;
+aging error 10% CV</t>
+  </si>
+  <si>
+    <t>Aging error; biennial breeding; biennial model; no lambda in model; no non-conformists;
+aging error 10% CV</t>
+  </si>
+  <si>
+    <t>scenario_4.2.1</t>
+  </si>
+  <si>
+    <t>scenario_4.2.2</t>
+  </si>
+  <si>
+    <t>scenario_4.2.3</t>
   </si>
 </sst>
 </file>
@@ -1572,8 +1599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1597,7 +1624,7 @@
         <v>36</v>
       </c>
       <c r="B1" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1606,7 +1633,7 @@
         <v>14</v>
       </c>
       <c r="E1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F1" t="s">
         <v>58</v>
@@ -1642,7 +1669,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -1678,7 +1705,7 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -1708,19 +1735,19 @@
       </c>
       <c r="B4" s="6"/>
       <c r="C4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H4" t="s">
         <v>15</v>
@@ -1744,19 +1771,19 @@
       </c>
       <c r="B5" s="6"/>
       <c r="C5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H5" t="s">
         <v>15</v>
@@ -1780,19 +1807,19 @@
       </c>
       <c r="B6" s="8"/>
       <c r="C6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H6" t="s">
         <v>59</v>
@@ -1816,19 +1843,19 @@
       </c>
       <c r="B7" s="6"/>
       <c r="C7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F7">
         <v>0</v>
       </c>
       <c r="G7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H7" t="s">
         <v>59</v>
@@ -1848,25 +1875,25 @@
     </row>
     <row r="8" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F8">
         <v>0</v>
       </c>
       <c r="G8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H8" t="s">
         <v>18</v>
@@ -1878,23 +1905,23 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D9">
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F9">
         <v>0</v>
       </c>
       <c r="G9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H9" t="s">
         <v>18</v>
@@ -1910,13 +1937,13 @@
       </c>
       <c r="B10" s="6"/>
       <c r="C10" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D10">
         <v>2</v>
       </c>
       <c r="E10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F10" s="4">
         <v>0</v>
@@ -1942,16 +1969,16 @@
         <v>50</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="C11" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D11">
         <v>2</v>
       </c>
       <c r="E11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F11" s="4">
         <v>0</v>
@@ -1974,19 +2001,19 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="C12" t="s">
         <v>186</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>194</v>
-      </c>
-      <c r="C12" t="s">
-        <v>189</v>
       </c>
       <c r="D12">
         <v>2</v>
       </c>
       <c r="E12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F12" s="4">
         <v>0</v>
@@ -2013,13 +2040,13 @@
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D13" s="2">
         <v>2</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F13" s="11">
         <v>0</v>
@@ -2047,13 +2074,13 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D14" s="2">
         <v>2</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F14" s="11">
         <v>0</v>
@@ -2077,17 +2104,17 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D15" s="2">
         <v>2</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F15" s="11">
         <v>0</v>
@@ -2115,13 +2142,13 @@
       </c>
       <c r="B16" s="6"/>
       <c r="C16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D16">
         <v>2</v>
       </c>
       <c r="E16" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F16" s="4">
         <v>0</v>
@@ -2148,13 +2175,13 @@
       </c>
       <c r="B17" s="6"/>
       <c r="C17" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D17">
         <v>2</v>
       </c>
       <c r="E17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F17" s="4">
         <v>0</v>
@@ -2177,17 +2204,17 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D18">
         <v>2</v>
       </c>
       <c r="E18" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F18" s="4">
         <v>0</v>
@@ -2208,22 +2235,22 @@
         <v>17</v>
       </c>
       <c r="L18" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B19" s="6"/>
       <c r="C19" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D19">
         <v>2</v>
       </c>
       <c r="E19" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F19" s="4">
         <v>0</v>
@@ -2244,19 +2271,19 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
-        <v>45</v>
+        <v>192</v>
       </c>
       <c r="B20" s="7"/>
-      <c r="C20" t="s">
-        <v>161</v>
+      <c r="C20" s="1" t="s">
+        <v>195</v>
       </c>
       <c r="D20">
         <v>2</v>
       </c>
       <c r="E20" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F20" s="4">
         <v>0</v>
@@ -2277,19 +2304,19 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
-        <v>141</v>
+        <v>193</v>
       </c>
       <c r="B21" s="7"/>
-      <c r="C21" t="s">
-        <v>162</v>
+      <c r="C21" s="1" t="s">
+        <v>196</v>
       </c>
       <c r="D21">
         <v>2</v>
       </c>
       <c r="E21" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F21" s="4">
         <v>0</v>
@@ -2310,19 +2337,19 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="B22" s="7"/>
-      <c r="C22" t="s">
-        <v>192</v>
+      <c r="C22" s="1" t="s">
+        <v>197</v>
       </c>
       <c r="D22">
         <v>2</v>
       </c>
       <c r="E22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F22" s="4">
         <v>0</v>
@@ -2340,6 +2367,105 @@
         <v>27</v>
       </c>
       <c r="K22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="B23" s="7"/>
+      <c r="C23" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D23">
+        <v>2</v>
+      </c>
+      <c r="E23" t="s">
+        <v>153</v>
+      </c>
+      <c r="F23" s="4">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23" t="s">
+        <v>59</v>
+      </c>
+      <c r="I23" t="s">
+        <v>19</v>
+      </c>
+      <c r="J23" t="s">
+        <v>27</v>
+      </c>
+      <c r="K23" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="B24" s="7"/>
+      <c r="C24" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="D24">
+        <v>2</v>
+      </c>
+      <c r="E24" t="s">
+        <v>153</v>
+      </c>
+      <c r="F24" s="4">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24" t="s">
+        <v>18</v>
+      </c>
+      <c r="I24" t="s">
+        <v>19</v>
+      </c>
+      <c r="J24" t="s">
+        <v>27</v>
+      </c>
+      <c r="K24" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A25" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="B25" s="7"/>
+      <c r="C25" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="D25">
+        <v>2</v>
+      </c>
+      <c r="E25" t="s">
+        <v>153</v>
+      </c>
+      <c r="F25" s="4">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+      <c r="H25" t="s">
+        <v>15</v>
+      </c>
+      <c r="I25" t="s">
+        <v>19</v>
+      </c>
+      <c r="J25" t="s">
+        <v>27</v>
+      </c>
+      <c r="K25" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2402,33 +2528,33 @@
         <v>46</v>
       </c>
       <c r="C1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E1" t="s">
         <v>47</v>
       </c>
       <c r="F1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="G1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="H1" t="s">
         <v>48</v>
       </c>
       <c r="I1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="J1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>37</v>
@@ -2444,85 +2570,85 @@
     </row>
     <row r="3" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>40</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="M3" s="1"/>
       <c r="O3" s="1"/>
     </row>
     <row r="4" spans="1:15" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>41</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>179</v>
-      </c>
       <c r="H4" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>182</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>185</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>

</xml_diff>

<commit_message>
Major updates to lemon shark model and data viz: split viz into 1) collating and exporting results, then 2) analysis and viz
</commit_message>
<xml_diff>
--- a/Simulation_log_key.xlsx
+++ b/Simulation_log_key.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\Documents\R\working_directory\LemonSharkCKMR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zeus\Documents\R\working_directory\LemonSharkCKMR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E935F37-81B2-47DC-A970-01C5AA8D7762}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4CF8340-DE81-4178-8AC3-6E04FC435323}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5085" yWindow="-11640" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Simulation_log_key" sheetId="1" r:id="rId1"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="805" uniqueCount="212">
   <si>
     <t>Objective</t>
   </si>
@@ -241,9 +241,6 @@
   </si>
   <si>
     <t>scenario_3.3.2</t>
-  </si>
-  <si>
-    <t>Non-conformists</t>
   </si>
   <si>
     <t>Uniform(0.80, 1.20)</t>
@@ -685,13 +682,40 @@
   </si>
   <si>
     <t>scenario_4.2.3</t>
+  </si>
+  <si>
+    <t>Ben's derivation (minus lambda)</t>
+  </si>
+  <si>
+    <t>Ben's derivation</t>
+  </si>
+  <si>
+    <t>scenario_3.4.1</t>
+  </si>
+  <si>
+    <t>scenario_3.4.2</t>
+  </si>
+  <si>
+    <t>scenario_3.4.3</t>
+  </si>
+  <si>
+    <t>scenario_3.5.1</t>
+  </si>
+  <si>
+    <t>scenario_3.5.2</t>
+  </si>
+  <si>
+    <t>scenario_3.5.3</t>
+  </si>
+  <si>
+    <t>Conformists</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -838,6 +862,17 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="37">
@@ -1205,7 +1240,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1227,6 +1262,8 @@
     </xf>
     <xf numFmtId="9" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1597,34 +1634,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L35"/>
+  <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="86.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5546875" customWidth="1"/>
-    <col min="5" max="5" width="27.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.5546875" customWidth="1"/>
-    <col min="7" max="7" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="72.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="56.7109375" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="28.7109375" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="72.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>36</v>
       </c>
       <c r="B1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1633,10 +1670,10 @@
         <v>14</v>
       </c>
       <c r="E1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F1" t="s">
-        <v>58</v>
+        <v>211</v>
       </c>
       <c r="G1" t="s">
         <v>3</v>
@@ -1657,7 +1694,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>37</v>
       </c>
@@ -1669,7 +1706,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -1693,7 +1730,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>38</v>
       </c>
@@ -1705,7 +1742,7 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -1729,25 +1766,25 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>54</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H4" t="s">
         <v>15</v>
@@ -1765,25 +1802,25 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>55</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H5" t="s">
         <v>15</v>
@@ -1801,28 +1838,28 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>40</v>
       </c>
       <c r="B6" s="8"/>
       <c r="C6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I6" t="s">
         <v>19</v>
@@ -1834,31 +1871,31 @@
         <v>17</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>41</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F7">
         <v>0</v>
       </c>
       <c r="G7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I7" t="s">
         <v>19</v>
@@ -1870,30 +1907,30 @@
         <v>17</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B8" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>190</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>191</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F8">
         <v>0</v>
       </c>
       <c r="G8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H8" t="s">
         <v>18</v>
@@ -1903,25 +1940,25 @@
       </c>
       <c r="L8" s="1"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D9">
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F9">
         <v>0</v>
       </c>
       <c r="G9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H9" t="s">
         <v>18</v>
@@ -1931,22 +1968,22 @@
       </c>
       <c r="L9" s="1"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>49</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D10">
         <v>2</v>
       </c>
       <c r="E10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F10" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10">
         <v>1</v>
@@ -1964,30 +2001,30 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>50</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C11" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D11">
         <v>2</v>
       </c>
       <c r="E11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F11" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11">
         <v>1</v>
       </c>
       <c r="H11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I11" t="s">
         <v>19</v>
@@ -1999,24 +2036,24 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C12" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D12">
         <v>2</v>
       </c>
       <c r="E12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F12" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12">
         <v>1</v>
@@ -2034,19 +2071,19 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D13" s="2">
         <v>2</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F13" s="11">
         <v>0</v>
@@ -2068,19 +2105,19 @@
       </c>
       <c r="L13" s="2"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>52</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D14" s="2">
         <v>2</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F14" s="11">
         <v>0</v>
@@ -2089,7 +2126,7 @@
         <v>1</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I14" s="2" t="s">
         <v>19</v>
@@ -2102,19 +2139,19 @@
       </c>
       <c r="L14" s="2"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D15" s="2">
         <v>2</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F15" s="11">
         <v>0</v>
@@ -2136,19 +2173,19 @@
       </c>
       <c r="L15" s="2"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>56</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D16">
         <v>2</v>
       </c>
       <c r="E16" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F16" s="4">
         <v>0</v>
@@ -2169,19 +2206,19 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>57</v>
       </c>
       <c r="B17" s="6"/>
       <c r="C17" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D17">
         <v>2</v>
       </c>
       <c r="E17" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F17" s="4">
         <v>0</v>
@@ -2190,7 +2227,7 @@
         <v>1</v>
       </c>
       <c r="H17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I17" t="s">
         <v>19</v>
@@ -2202,19 +2239,19 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D18">
         <v>2</v>
       </c>
       <c r="E18" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F18" s="4">
         <v>0</v>
@@ -2223,7 +2260,7 @@
         <v>1</v>
       </c>
       <c r="H18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I18" t="s">
         <v>19</v>
@@ -2235,22 +2272,22 @@
         <v>17</v>
       </c>
       <c r="L18" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
         <v>144</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A19" s="6" t="s">
-        <v>145</v>
       </c>
       <c r="B19" s="6"/>
       <c r="C19" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D19">
         <v>2</v>
       </c>
       <c r="E19" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F19" s="4">
         <v>0</v>
@@ -2271,223 +2308,598 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A20" s="7" t="s">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="D20" s="13">
+        <v>2</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F20" s="14">
+        <v>1</v>
+      </c>
+      <c r="G20" s="13">
+        <v>1</v>
+      </c>
+      <c r="H20" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="I20" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J20" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="K20" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" s="13"/>
+      <c r="C21" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="D21" s="13">
+        <v>2</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F21" s="14">
+        <v>1</v>
+      </c>
+      <c r="G21" s="13">
+        <v>1</v>
+      </c>
+      <c r="H21" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="I21" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J21" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="K21" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="B22" s="13"/>
+      <c r="C22" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="D22" s="13">
+        <v>2</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F22" s="14">
+        <v>1</v>
+      </c>
+      <c r="G22" s="13">
+        <v>1</v>
+      </c>
+      <c r="H22" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="I22" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J22" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="K22" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23" s="13"/>
+      <c r="C23" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="D23" s="13">
+        <v>2</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F23" s="14">
+        <v>0.9</v>
+      </c>
+      <c r="G23" s="13">
+        <v>1</v>
+      </c>
+      <c r="H23" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="I23" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J23" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="K23" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B24" s="13"/>
+      <c r="C24" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="D24" s="13">
+        <v>2</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F24" s="14">
+        <v>0.9</v>
+      </c>
+      <c r="G24" s="13">
+        <v>1</v>
+      </c>
+      <c r="H24" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="I24" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J24" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="K24" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="B25" s="13"/>
+      <c r="C25" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="D25" s="13">
+        <v>2</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F25" s="14">
+        <v>0.9</v>
+      </c>
+      <c r="G25" s="13">
+        <v>1</v>
+      </c>
+      <c r="H25" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="I25" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J25" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="K25" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="13" t="s">
+        <v>205</v>
+      </c>
+      <c r="B26" s="13"/>
+      <c r="C26" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="D26" s="13">
+        <v>2</v>
+      </c>
+      <c r="E26" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F26" s="14">
+        <v>0.75</v>
+      </c>
+      <c r="G26" s="13">
+        <v>1</v>
+      </c>
+      <c r="H26" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="I26" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J26" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="K26" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="13" t="s">
+        <v>206</v>
+      </c>
+      <c r="B27" s="13"/>
+      <c r="C27" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="D27" s="13">
+        <v>2</v>
+      </c>
+      <c r="E27" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F27" s="14">
+        <v>0.75</v>
+      </c>
+      <c r="G27" s="13">
+        <v>1</v>
+      </c>
+      <c r="H27" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="I27" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J27" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="K27" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="13" t="s">
+        <v>207</v>
+      </c>
+      <c r="B28" s="13"/>
+      <c r="C28" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="D28" s="13">
+        <v>2</v>
+      </c>
+      <c r="E28" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F28" s="14">
+        <v>0.75</v>
+      </c>
+      <c r="G28" s="13">
+        <v>1</v>
+      </c>
+      <c r="H28" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="I28" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J28" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="K28" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="13" t="s">
+        <v>208</v>
+      </c>
+      <c r="B29" s="13"/>
+      <c r="C29" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="D29" s="13">
+        <v>2</v>
+      </c>
+      <c r="E29" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F29" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="G29" s="13">
+        <v>1</v>
+      </c>
+      <c r="H29" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="I29" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J29" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="K29" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="13" t="s">
+        <v>209</v>
+      </c>
+      <c r="B30" s="13"/>
+      <c r="C30" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="D30" s="13">
+        <v>2</v>
+      </c>
+      <c r="E30" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F30" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="G30" s="13">
+        <v>1</v>
+      </c>
+      <c r="H30" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="I30" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J30" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="K30" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="13" t="s">
+        <v>210</v>
+      </c>
+      <c r="B31" s="13"/>
+      <c r="C31" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="D31" s="13">
+        <v>2</v>
+      </c>
+      <c r="E31" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F31" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="G31" s="13">
+        <v>1</v>
+      </c>
+      <c r="H31" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="I31" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J31" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="K31" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="B32" s="7"/>
+      <c r="C32" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D32">
+        <v>2</v>
+      </c>
+      <c r="E32" t="s">
+        <v>152</v>
+      </c>
+      <c r="F32" s="4">
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
+      <c r="H32" t="s">
+        <v>58</v>
+      </c>
+      <c r="I32" t="s">
+        <v>19</v>
+      </c>
+      <c r="J32" t="s">
+        <v>27</v>
+      </c>
+      <c r="K32" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A33" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="B20" s="7"/>
-      <c r="C20" s="1" t="s">
+      <c r="B33" s="7"/>
+      <c r="C33" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="D20">
+      <c r="D33">
         <v>2</v>
       </c>
-      <c r="E20" t="s">
-        <v>153</v>
-      </c>
-      <c r="F20" s="4">
+      <c r="E33" t="s">
+        <v>152</v>
+      </c>
+      <c r="F33" s="4">
         <v>0</v>
       </c>
-      <c r="G20">
+      <c r="G33">
         <v>1</v>
       </c>
-      <c r="H20" t="s">
-        <v>59</v>
-      </c>
-      <c r="I20" t="s">
+      <c r="H33" t="s">
+        <v>18</v>
+      </c>
+      <c r="I33" t="s">
         <v>19</v>
       </c>
-      <c r="J20" t="s">
+      <c r="J33" t="s">
         <v>27</v>
       </c>
-      <c r="K20" t="s">
+      <c r="K33" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A21" s="7" t="s">
+    <row r="34" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="B21" s="7"/>
-      <c r="C21" s="1" t="s">
+      <c r="B34" s="7"/>
+      <c r="C34" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="D21">
+      <c r="D34">
         <v>2</v>
       </c>
-      <c r="E21" t="s">
-        <v>153</v>
-      </c>
-      <c r="F21" s="4">
+      <c r="E34" t="s">
+        <v>152</v>
+      </c>
+      <c r="F34" s="4">
         <v>0</v>
       </c>
-      <c r="G21">
+      <c r="G34">
         <v>1</v>
       </c>
-      <c r="H21" t="s">
+      <c r="H34" t="s">
+        <v>15</v>
+      </c>
+      <c r="I34" t="s">
+        <v>19</v>
+      </c>
+      <c r="J34" t="s">
+        <v>27</v>
+      </c>
+      <c r="K34" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A35" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="B35" s="7"/>
+      <c r="C35" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D35">
+        <v>2</v>
+      </c>
+      <c r="E35" t="s">
+        <v>152</v>
+      </c>
+      <c r="F35" s="4">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>1</v>
+      </c>
+      <c r="H35" t="s">
+        <v>58</v>
+      </c>
+      <c r="I35" t="s">
+        <v>19</v>
+      </c>
+      <c r="J35" t="s">
+        <v>27</v>
+      </c>
+      <c r="K35" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A36" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="B36" s="7"/>
+      <c r="C36" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D36">
+        <v>2</v>
+      </c>
+      <c r="E36" t="s">
+        <v>152</v>
+      </c>
+      <c r="F36" s="4">
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <v>1</v>
+      </c>
+      <c r="H36" t="s">
         <v>18</v>
       </c>
-      <c r="I21" t="s">
+      <c r="I36" t="s">
         <v>19</v>
       </c>
-      <c r="J21" t="s">
+      <c r="J36" t="s">
         <v>27</v>
       </c>
-      <c r="K21" t="s">
+      <c r="K36" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A22" s="7" t="s">
-        <v>194</v>
-      </c>
-      <c r="B22" s="7"/>
-      <c r="C22" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="D22">
+    <row r="37" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="B37" s="7"/>
+      <c r="C37" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="D37">
         <v>2</v>
       </c>
-      <c r="E22" t="s">
-        <v>153</v>
-      </c>
-      <c r="F22" s="4">
+      <c r="E37" t="s">
+        <v>152</v>
+      </c>
+      <c r="F37" s="4">
         <v>0</v>
       </c>
-      <c r="G22">
+      <c r="G37">
         <v>1</v>
       </c>
-      <c r="H22" t="s">
-        <v>15</v>
-      </c>
-      <c r="I22" t="s">
+      <c r="H37" t="s">
+        <v>15</v>
+      </c>
+      <c r="I37" t="s">
         <v>19</v>
       </c>
-      <c r="J22" t="s">
+      <c r="J37" t="s">
         <v>27</v>
       </c>
-      <c r="K22" t="s">
+      <c r="K37" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A23" s="7" t="s">
-        <v>201</v>
-      </c>
-      <c r="B23" s="7"/>
-      <c r="C23" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="D23">
-        <v>2</v>
-      </c>
-      <c r="E23" t="s">
-        <v>153</v>
-      </c>
-      <c r="F23" s="4">
-        <v>0</v>
-      </c>
-      <c r="G23">
-        <v>1</v>
-      </c>
-      <c r="H23" t="s">
-        <v>59</v>
-      </c>
-      <c r="I23" t="s">
-        <v>19</v>
-      </c>
-      <c r="J23" t="s">
-        <v>27</v>
-      </c>
-      <c r="K23" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A24" s="7" t="s">
-        <v>202</v>
-      </c>
-      <c r="B24" s="7"/>
-      <c r="C24" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="D24">
-        <v>2</v>
-      </c>
-      <c r="E24" t="s">
-        <v>153</v>
-      </c>
-      <c r="F24" s="4">
-        <v>0</v>
-      </c>
-      <c r="G24">
-        <v>1</v>
-      </c>
-      <c r="H24" t="s">
-        <v>18</v>
-      </c>
-      <c r="I24" t="s">
-        <v>19</v>
-      </c>
-      <c r="J24" t="s">
-        <v>27</v>
-      </c>
-      <c r="K24" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A25" s="7" t="s">
-        <v>203</v>
-      </c>
-      <c r="B25" s="7"/>
-      <c r="C25" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="D25">
-        <v>2</v>
-      </c>
-      <c r="E25" t="s">
-        <v>153</v>
-      </c>
-      <c r="F25" s="4">
-        <v>0</v>
-      </c>
-      <c r="G25">
-        <v>1</v>
-      </c>
-      <c r="H25" t="s">
-        <v>15</v>
-      </c>
-      <c r="I25" t="s">
-        <v>19</v>
-      </c>
-      <c r="J25" t="s">
-        <v>27</v>
-      </c>
-      <c r="K25" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>10</v>
-      </c>
-      <c r="C34" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>12</v>
-      </c>
-      <c r="C35" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -2504,23 +2916,23 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="52.6640625" customWidth="1"/>
-    <col min="2" max="2" width="47.6640625" customWidth="1"/>
-    <col min="3" max="3" width="21.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="47.6640625" customWidth="1"/>
-    <col min="5" max="5" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="26.6640625" customWidth="1"/>
-    <col min="8" max="8" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.6640625" customWidth="1"/>
-    <col min="10" max="12" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="26.109375" customWidth="1"/>
-    <col min="14" max="14" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="34.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="52.7109375" customWidth="1"/>
+    <col min="2" max="2" width="47.7109375" customWidth="1"/>
+    <col min="3" max="3" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="47.7109375" customWidth="1"/>
+    <col min="5" max="5" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="26.7109375" customWidth="1"/>
+    <col min="8" max="8" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.7109375" customWidth="1"/>
+    <col min="10" max="12" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="26.140625" customWidth="1"/>
+    <col min="14" max="14" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="34.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2528,33 +2940,33 @@
         <v>46</v>
       </c>
       <c r="C1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E1" t="s">
         <v>47</v>
       </c>
       <c r="F1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H1" t="s">
         <v>48</v>
       </c>
       <c r="I1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J1" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>37</v>
@@ -2568,87 +2980,87 @@
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>40</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M3" s="1"/>
       <c r="O3" s="1"/>
     </row>
-    <row r="4" spans="1:15" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>41</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G4" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="I4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="J4" s="1" t="s">
+    </row>
+    <row r="5" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="B5" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>181</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>182</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -2656,7 +3068,7 @@
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -2668,7 +3080,7 @@
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -2680,7 +3092,7 @@
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -2692,7 +3104,7 @@
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -2704,7 +3116,7 @@
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -2716,7 +3128,7 @@
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -2728,7 +3140,7 @@
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -2740,7 +3152,7 @@
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -2752,7 +3164,7 @@
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -2764,7 +3176,7 @@
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -2776,7 +3188,7 @@
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -2788,7 +3200,7 @@
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -2800,7 +3212,7 @@
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -2812,7 +3224,7 @@
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -2824,7 +3236,7 @@
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -2836,7 +3248,7 @@
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -2848,7 +3260,7 @@
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -2860,7 +3272,7 @@
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -2872,7 +3284,7 @@
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -2884,7 +3296,7 @@
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -2896,7 +3308,7 @@
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -2908,7 +3320,7 @@
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -2920,7 +3332,7 @@
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -2932,7 +3344,7 @@
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -2944,7 +3356,7 @@
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -2956,7 +3368,7 @@
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -2968,7 +3380,7 @@
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -2980,7 +3392,7 @@
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -2992,7 +3404,7 @@
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -3004,7 +3416,7 @@
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -3016,7 +3428,7 @@
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -3028,7 +3440,7 @@
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -3040,7 +3452,7 @@
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -3052,7 +3464,7 @@
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -3064,7 +3476,7 @@
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -3076,7 +3488,7 @@
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -3088,7 +3500,7 @@
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -3100,7 +3512,7 @@
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -3112,7 +3524,7 @@
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -3124,7 +3536,7 @@
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -3136,7 +3548,7 @@
       <c r="I45" s="1"/>
       <c r="J45" s="1"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -3148,7 +3560,7 @@
       <c r="I46" s="1"/>
       <c r="J46" s="1"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -3160,7 +3572,7 @@
       <c r="I47" s="1"/>
       <c r="J47" s="1"/>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -3172,7 +3584,7 @@
       <c r="I48" s="1"/>
       <c r="J48" s="1"/>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -3184,7 +3596,7 @@
       <c r="I49" s="1"/>
       <c r="J49" s="1"/>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -3196,7 +3608,7 @@
       <c r="I50" s="1"/>
       <c r="J50" s="1"/>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -3208,7 +3620,7 @@
       <c r="I51" s="1"/>
       <c r="J51" s="1"/>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -3220,7 +3632,7 @@
       <c r="I52" s="1"/>
       <c r="J52" s="1"/>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -3232,7 +3644,7 @@
       <c r="I53" s="1"/>
       <c r="J53" s="1"/>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -3244,7 +3656,7 @@
       <c r="I54" s="1"/>
       <c r="J54" s="1"/>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -3256,7 +3668,7 @@
       <c r="I55" s="1"/>
       <c r="J55" s="1"/>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -3268,7 +3680,7 @@
       <c r="I56" s="1"/>
       <c r="J56" s="1"/>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -3280,7 +3692,7 @@
       <c r="I57" s="1"/>
       <c r="J57" s="1"/>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -3292,7 +3704,7 @@
       <c r="I58" s="1"/>
       <c r="J58" s="1"/>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -3304,7 +3716,7 @@
       <c r="I59" s="1"/>
       <c r="J59" s="1"/>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -3316,7 +3728,7 @@
       <c r="I60" s="1"/>
       <c r="J60" s="1"/>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -3328,7 +3740,7 @@
       <c r="I61" s="1"/>
       <c r="J61" s="1"/>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -3340,7 +3752,7 @@
       <c r="I62" s="1"/>
       <c r="J62" s="1"/>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -3352,7 +3764,7 @@
       <c r="I63" s="1"/>
       <c r="J63" s="1"/>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -3364,7 +3776,7 @@
       <c r="I64" s="1"/>
       <c r="J64" s="1"/>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -3376,7 +3788,7 @@
       <c r="I65" s="1"/>
       <c r="J65" s="1"/>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -3388,7 +3800,7 @@
       <c r="I66" s="1"/>
       <c r="J66" s="1"/>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -3400,7 +3812,7 @@
       <c r="I67" s="1"/>
       <c r="J67" s="1"/>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -3412,7 +3824,7 @@
       <c r="I68" s="1"/>
       <c r="J68" s="1"/>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -3424,7 +3836,7 @@
       <c r="I69" s="1"/>
       <c r="J69" s="1"/>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -3436,7 +3848,7 @@
       <c r="I70" s="1"/>
       <c r="J70" s="1"/>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -3448,7 +3860,7 @@
       <c r="I71" s="1"/>
       <c r="J71" s="1"/>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -3460,7 +3872,7 @@
       <c r="I72" s="1"/>
       <c r="J72" s="1"/>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -3472,7 +3884,7 @@
       <c r="I73" s="1"/>
       <c r="J73" s="1"/>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -3484,7 +3896,7 @@
       <c r="I74" s="1"/>
       <c r="J74" s="1"/>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -3496,7 +3908,7 @@
       <c r="I75" s="1"/>
       <c r="J75" s="1"/>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -3508,7 +3920,7 @@
       <c r="I76" s="1"/>
       <c r="J76" s="1"/>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -3520,7 +3932,7 @@
       <c r="I77" s="1"/>
       <c r="J77" s="1"/>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -3532,7 +3944,7 @@
       <c r="I78" s="1"/>
       <c r="J78" s="1"/>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -3544,7 +3956,7 @@
       <c r="I79" s="1"/>
       <c r="J79" s="1"/>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -3556,7 +3968,7 @@
       <c r="I80" s="1"/>
       <c r="J80" s="1"/>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -3568,7 +3980,7 @@
       <c r="I81" s="1"/>
       <c r="J81" s="1"/>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -3580,7 +3992,7 @@
       <c r="I82" s="1"/>
       <c r="J82" s="1"/>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -3592,7 +4004,7 @@
       <c r="I83" s="1"/>
       <c r="J83" s="1"/>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -3604,7 +4016,7 @@
       <c r="I84" s="1"/>
       <c r="J84" s="1"/>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -3616,7 +4028,7 @@
       <c r="I85" s="1"/>
       <c r="J85" s="1"/>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -3628,7 +4040,7 @@
       <c r="I86" s="1"/>
       <c r="J86" s="1"/>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -3640,7 +4052,7 @@
       <c r="I87" s="1"/>
       <c r="J87" s="1"/>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -3652,7 +4064,7 @@
       <c r="I88" s="1"/>
       <c r="J88" s="1"/>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -3664,7 +4076,7 @@
       <c r="I89" s="1"/>
       <c r="J89" s="1"/>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
@@ -3676,7 +4088,7 @@
       <c r="I90" s="1"/>
       <c r="J90" s="1"/>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
@@ -3688,7 +4100,7 @@
       <c r="I91" s="1"/>
       <c r="J91" s="1"/>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -3700,7 +4112,7 @@
       <c r="I92" s="1"/>
       <c r="J92" s="1"/>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
@@ -3712,7 +4124,7 @@
       <c r="I93" s="1"/>
       <c r="J93" s="1"/>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
@@ -3724,7 +4136,7 @@
       <c r="I94" s="1"/>
       <c r="J94" s="1"/>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
@@ -3736,7 +4148,7 @@
       <c r="I95" s="1"/>
       <c r="J95" s="1"/>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
@@ -3748,7 +4160,7 @@
       <c r="I96" s="1"/>
       <c r="J96" s="1"/>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
@@ -3760,7 +4172,7 @@
       <c r="I97" s="1"/>
       <c r="J97" s="1"/>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
@@ -3772,7 +4184,7 @@
       <c r="I98" s="1"/>
       <c r="J98" s="1"/>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
@@ -3784,7 +4196,7 @@
       <c r="I99" s="1"/>
       <c r="J99" s="1"/>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
@@ -3796,7 +4208,7 @@
       <c r="I100" s="1"/>
       <c r="J100" s="1"/>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
@@ -3808,7 +4220,7 @@
       <c r="I101" s="1"/>
       <c r="J101" s="1"/>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
@@ -3820,7 +4232,7 @@
       <c r="I102" s="1"/>
       <c r="J102" s="1"/>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
@@ -3832,7 +4244,7 @@
       <c r="I103" s="1"/>
       <c r="J103" s="1"/>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
@@ -3844,7 +4256,7 @@
       <c r="I104" s="1"/>
       <c r="J104" s="1"/>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" s="1"/>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
@@ -3856,7 +4268,7 @@
       <c r="I105" s="1"/>
       <c r="J105" s="1"/>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
@@ -3868,7 +4280,7 @@
       <c r="I106" s="1"/>
       <c r="J106" s="1"/>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
@@ -3880,7 +4292,7 @@
       <c r="I107" s="1"/>
       <c r="J107" s="1"/>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" s="1"/>
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
@@ -3892,7 +4304,7 @@
       <c r="I108" s="1"/>
       <c r="J108" s="1"/>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" s="1"/>
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
@@ -3917,20 +4329,20 @@
       <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.5546875" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5546875" customWidth="1"/>
-    <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="72.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.5703125" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="72.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>36</v>
       </c>
@@ -3959,7 +4371,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -3988,7 +4400,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -4017,7 +4429,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -4046,7 +4458,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>40</v>
       </c>
@@ -4072,7 +4484,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>41</v>
       </c>
@@ -4101,7 +4513,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>42</v>
       </c>
@@ -4130,7 +4542,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>43</v>
       </c>
@@ -4156,7 +4568,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>44</v>
       </c>
@@ -4182,7 +4594,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>45</v>
       </c>
@@ -4190,12 +4602,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>10</v>
       </c>
@@ -4203,7 +4615,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>12</v>
       </c>
@@ -4224,152 +4636,152 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="79.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="98.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="62.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="79.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="98.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="62.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="69" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="77.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="77.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="8" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.88671875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="17" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="41.5546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="41.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" t="s">
         <v>62</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>63</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>64</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>65</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>66</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>67</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>68</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>69</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>70</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>71</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>72</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>73</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>74</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>75</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>76</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>77</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>78</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>79</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>80</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>81</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>82</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>83</v>
       </c>
-      <c r="W1" t="s">
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>85</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>86</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
         <v>87</v>
-      </c>
-      <c r="D2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" t="s">
-        <v>88</v>
       </c>
       <c r="G2" s="5">
         <v>44754</v>
       </c>
       <c r="H2" t="s">
+        <v>88</v>
+      </c>
+      <c r="I2" t="s">
         <v>89</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L2" t="s">
+        <v>88</v>
+      </c>
+      <c r="M2" t="s">
+        <v>89</v>
+      </c>
+      <c r="N2" t="s">
         <v>90</v>
       </c>
-      <c r="J2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K2" t="s">
-        <v>15</v>
-      </c>
-      <c r="L2" t="s">
-        <v>89</v>
-      </c>
-      <c r="M2" t="s">
-        <v>90</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>91</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>92</v>
-      </c>
-      <c r="P2" t="s">
-        <v>93</v>
       </c>
       <c r="Q2">
         <v>20</v>
@@ -4390,57 +4802,57 @@
         <v>15</v>
       </c>
       <c r="W2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
         <v>95</v>
-      </c>
-      <c r="B3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C3" t="s">
-        <v>87</v>
-      </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" t="s">
-        <v>96</v>
       </c>
       <c r="G3" s="5">
         <v>44754</v>
       </c>
       <c r="H3" t="s">
+        <v>89</v>
+      </c>
+      <c r="I3" t="s">
+        <v>89</v>
+      </c>
+      <c r="J3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L3" t="s">
+        <v>88</v>
+      </c>
+      <c r="M3" t="s">
+        <v>89</v>
+      </c>
+      <c r="N3" t="s">
         <v>90</v>
       </c>
-      <c r="I3" t="s">
-        <v>90</v>
-      </c>
-      <c r="J3" t="s">
-        <v>15</v>
-      </c>
-      <c r="K3" t="s">
-        <v>15</v>
-      </c>
-      <c r="L3" t="s">
-        <v>89</v>
-      </c>
-      <c r="M3" t="s">
-        <v>90</v>
-      </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>91</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>92</v>
-      </c>
-      <c r="P3" t="s">
-        <v>93</v>
       </c>
       <c r="Q3">
         <v>20</v>
@@ -4461,57 +4873,57 @@
         <v>15</v>
       </c>
       <c r="W3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
         <v>97</v>
-      </c>
-      <c r="B4" t="s">
-        <v>86</v>
-      </c>
-      <c r="C4" t="s">
-        <v>87</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" t="s">
-        <v>98</v>
       </c>
       <c r="G4" s="5">
         <v>44755</v>
       </c>
       <c r="H4" t="s">
+        <v>89</v>
+      </c>
+      <c r="I4" t="s">
+        <v>89</v>
+      </c>
+      <c r="J4" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L4" t="s">
+        <v>89</v>
+      </c>
+      <c r="M4" t="s">
+        <v>89</v>
+      </c>
+      <c r="N4" t="s">
         <v>90</v>
       </c>
-      <c r="I4" t="s">
-        <v>90</v>
-      </c>
-      <c r="J4" t="s">
-        <v>15</v>
-      </c>
-      <c r="K4" t="s">
-        <v>15</v>
-      </c>
-      <c r="L4" t="s">
-        <v>90</v>
-      </c>
-      <c r="M4" t="s">
-        <v>90</v>
-      </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>91</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>92</v>
-      </c>
-      <c r="P4" t="s">
-        <v>93</v>
       </c>
       <c r="Q4">
         <v>20</v>
@@ -4532,57 +4944,57 @@
         <v>15</v>
       </c>
       <c r="W4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C5" t="s">
         <v>99</v>
       </c>
-      <c r="B5" t="s">
-        <v>86</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" t="s">
         <v>100</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" t="s">
-        <v>101</v>
       </c>
       <c r="G5" s="5">
         <v>44755</v>
       </c>
       <c r="H5" t="s">
+        <v>88</v>
+      </c>
+      <c r="I5" t="s">
         <v>89</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L5" t="s">
+        <v>88</v>
+      </c>
+      <c r="M5" t="s">
+        <v>89</v>
+      </c>
+      <c r="N5" t="s">
         <v>90</v>
       </c>
-      <c r="J5" t="s">
-        <v>15</v>
-      </c>
-      <c r="K5" t="s">
-        <v>15</v>
-      </c>
-      <c r="L5" t="s">
-        <v>89</v>
-      </c>
-      <c r="M5" t="s">
-        <v>90</v>
-      </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>91</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>92</v>
-      </c>
-      <c r="P5" t="s">
-        <v>93</v>
       </c>
       <c r="Q5">
         <v>20</v>
@@ -4603,57 +5015,57 @@
         <v>15</v>
       </c>
       <c r="W5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C6" t="s">
+        <v>99</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" t="s">
         <v>102</v>
-      </c>
-      <c r="B6" t="s">
-        <v>86</v>
-      </c>
-      <c r="C6" t="s">
-        <v>100</v>
-      </c>
-      <c r="D6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" t="s">
-        <v>103</v>
       </c>
       <c r="G6" s="5">
         <v>44755</v>
       </c>
       <c r="H6" t="s">
+        <v>89</v>
+      </c>
+      <c r="I6" t="s">
+        <v>89</v>
+      </c>
+      <c r="J6" t="s">
+        <v>15</v>
+      </c>
+      <c r="K6" t="s">
+        <v>15</v>
+      </c>
+      <c r="L6" t="s">
+        <v>88</v>
+      </c>
+      <c r="M6" t="s">
+        <v>89</v>
+      </c>
+      <c r="N6" t="s">
         <v>90</v>
       </c>
-      <c r="I6" t="s">
-        <v>90</v>
-      </c>
-      <c r="J6" t="s">
-        <v>15</v>
-      </c>
-      <c r="K6" t="s">
-        <v>15</v>
-      </c>
-      <c r="L6" t="s">
-        <v>89</v>
-      </c>
-      <c r="M6" t="s">
-        <v>90</v>
-      </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>91</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>92</v>
-      </c>
-      <c r="P6" t="s">
-        <v>93</v>
       </c>
       <c r="Q6">
         <v>20</v>
@@ -4674,57 +5086,57 @@
         <v>15</v>
       </c>
       <c r="W6" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C7" t="s">
+        <v>99</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" t="s">
         <v>104</v>
-      </c>
-      <c r="B7" t="s">
-        <v>86</v>
-      </c>
-      <c r="C7" t="s">
-        <v>100</v>
-      </c>
-      <c r="D7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" t="s">
-        <v>105</v>
       </c>
       <c r="G7" s="5">
         <v>44755</v>
       </c>
       <c r="H7" t="s">
+        <v>89</v>
+      </c>
+      <c r="I7" t="s">
+        <v>89</v>
+      </c>
+      <c r="J7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K7" t="s">
+        <v>15</v>
+      </c>
+      <c r="L7" t="s">
+        <v>89</v>
+      </c>
+      <c r="M7" t="s">
+        <v>89</v>
+      </c>
+      <c r="N7" t="s">
         <v>90</v>
       </c>
-      <c r="I7" t="s">
-        <v>90</v>
-      </c>
-      <c r="J7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K7" t="s">
-        <v>15</v>
-      </c>
-      <c r="L7" t="s">
-        <v>90</v>
-      </c>
-      <c r="M7" t="s">
-        <v>90</v>
-      </c>
-      <c r="N7" t="s">
+      <c r="O7" t="s">
         <v>91</v>
       </c>
-      <c r="O7" t="s">
+      <c r="P7" t="s">
         <v>92</v>
-      </c>
-      <c r="P7" t="s">
-        <v>93</v>
       </c>
       <c r="Q7">
         <v>20</v>
@@ -4745,57 +5157,57 @@
         <v>15</v>
       </c>
       <c r="W7" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>105</v>
+      </c>
+      <c r="B8" t="s">
         <v>106</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>107</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>108</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" t="s">
         <v>109</v>
-      </c>
-      <c r="E8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" t="s">
-        <v>110</v>
       </c>
       <c r="G8" s="5">
         <v>44755</v>
       </c>
       <c r="H8" t="s">
+        <v>88</v>
+      </c>
+      <c r="I8" t="s">
         <v>89</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
+        <v>15</v>
+      </c>
+      <c r="K8" t="s">
+        <v>15</v>
+      </c>
+      <c r="L8" t="s">
+        <v>88</v>
+      </c>
+      <c r="M8" t="s">
+        <v>89</v>
+      </c>
+      <c r="N8" t="s">
         <v>90</v>
       </c>
-      <c r="J8" t="s">
-        <v>15</v>
-      </c>
-      <c r="K8" t="s">
-        <v>15</v>
-      </c>
-      <c r="L8" t="s">
-        <v>89</v>
-      </c>
-      <c r="M8" t="s">
-        <v>90</v>
-      </c>
-      <c r="N8" t="s">
+      <c r="O8" t="s">
         <v>91</v>
       </c>
-      <c r="O8" t="s">
+      <c r="P8" t="s">
         <v>92</v>
-      </c>
-      <c r="P8" t="s">
-        <v>93</v>
       </c>
       <c r="Q8">
         <v>20</v>
@@ -4816,57 +5228,57 @@
         <v>15</v>
       </c>
       <c r="W8" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>110</v>
+      </c>
+      <c r="B9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C9" t="s">
+        <v>107</v>
+      </c>
+      <c r="D9" t="s">
+        <v>108</v>
+      </c>
+      <c r="E9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" t="s">
         <v>111</v>
-      </c>
-      <c r="B9" t="s">
-        <v>107</v>
-      </c>
-      <c r="C9" t="s">
-        <v>108</v>
-      </c>
-      <c r="D9" t="s">
-        <v>109</v>
-      </c>
-      <c r="E9" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" t="s">
-        <v>112</v>
       </c>
       <c r="G9" s="5">
         <v>44755</v>
       </c>
       <c r="H9" t="s">
+        <v>89</v>
+      </c>
+      <c r="I9" t="s">
+        <v>89</v>
+      </c>
+      <c r="J9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K9" t="s">
+        <v>15</v>
+      </c>
+      <c r="L9" t="s">
+        <v>88</v>
+      </c>
+      <c r="M9" t="s">
+        <v>89</v>
+      </c>
+      <c r="N9" t="s">
         <v>90</v>
       </c>
-      <c r="I9" t="s">
-        <v>90</v>
-      </c>
-      <c r="J9" t="s">
-        <v>15</v>
-      </c>
-      <c r="K9" t="s">
-        <v>15</v>
-      </c>
-      <c r="L9" t="s">
-        <v>89</v>
-      </c>
-      <c r="M9" t="s">
-        <v>90</v>
-      </c>
-      <c r="N9" t="s">
+      <c r="O9" t="s">
         <v>91</v>
       </c>
-      <c r="O9" t="s">
+      <c r="P9" t="s">
         <v>92</v>
-      </c>
-      <c r="P9" t="s">
-        <v>93</v>
       </c>
       <c r="Q9">
         <v>20</v>
@@ -4887,57 +5299,57 @@
         <v>15</v>
       </c>
       <c r="W9" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>112</v>
+      </c>
+      <c r="B10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C10" t="s">
+        <v>107</v>
+      </c>
+      <c r="D10" t="s">
+        <v>108</v>
+      </c>
+      <c r="E10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" t="s">
         <v>113</v>
-      </c>
-      <c r="B10" t="s">
-        <v>107</v>
-      </c>
-      <c r="C10" t="s">
-        <v>108</v>
-      </c>
-      <c r="D10" t="s">
-        <v>109</v>
-      </c>
-      <c r="E10" t="s">
-        <v>15</v>
-      </c>
-      <c r="F10" t="s">
-        <v>114</v>
       </c>
       <c r="G10" s="5">
         <v>44755</v>
       </c>
       <c r="H10" t="s">
+        <v>89</v>
+      </c>
+      <c r="I10" t="s">
+        <v>89</v>
+      </c>
+      <c r="J10" t="s">
+        <v>15</v>
+      </c>
+      <c r="K10" t="s">
+        <v>15</v>
+      </c>
+      <c r="L10" t="s">
+        <v>89</v>
+      </c>
+      <c r="M10" t="s">
+        <v>89</v>
+      </c>
+      <c r="N10" t="s">
         <v>90</v>
       </c>
-      <c r="I10" t="s">
-        <v>90</v>
-      </c>
-      <c r="J10" t="s">
-        <v>15</v>
-      </c>
-      <c r="K10" t="s">
-        <v>15</v>
-      </c>
-      <c r="L10" t="s">
-        <v>90</v>
-      </c>
-      <c r="M10" t="s">
-        <v>90</v>
-      </c>
-      <c r="N10" t="s">
+      <c r="O10" t="s">
         <v>91</v>
       </c>
-      <c r="O10" t="s">
+      <c r="P10" t="s">
         <v>92</v>
-      </c>
-      <c r="P10" t="s">
-        <v>93</v>
       </c>
       <c r="Q10">
         <v>20</v>
@@ -4958,57 +5370,57 @@
         <v>15</v>
       </c>
       <c r="W10" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>114</v>
+      </c>
+      <c r="B11" t="s">
+        <v>106</v>
+      </c>
+      <c r="C11" t="s">
+        <v>107</v>
+      </c>
+      <c r="D11" t="s">
+        <v>108</v>
+      </c>
+      <c r="E11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" t="s">
         <v>115</v>
-      </c>
-      <c r="B11" t="s">
-        <v>107</v>
-      </c>
-      <c r="C11" t="s">
-        <v>108</v>
-      </c>
-      <c r="D11" t="s">
-        <v>109</v>
-      </c>
-      <c r="E11" t="s">
-        <v>15</v>
-      </c>
-      <c r="F11" t="s">
-        <v>116</v>
       </c>
       <c r="G11" s="5">
         <v>44755</v>
       </c>
       <c r="H11" t="s">
+        <v>89</v>
+      </c>
+      <c r="I11" t="s">
+        <v>89</v>
+      </c>
+      <c r="J11" t="s">
+        <v>15</v>
+      </c>
+      <c r="K11" t="s">
+        <v>15</v>
+      </c>
+      <c r="L11" t="s">
+        <v>89</v>
+      </c>
+      <c r="M11" t="s">
+        <v>89</v>
+      </c>
+      <c r="N11" t="s">
         <v>90</v>
       </c>
-      <c r="I11" t="s">
-        <v>90</v>
-      </c>
-      <c r="J11" t="s">
-        <v>15</v>
-      </c>
-      <c r="K11" t="s">
-        <v>15</v>
-      </c>
-      <c r="L11" t="s">
-        <v>90</v>
-      </c>
-      <c r="M11" t="s">
-        <v>90</v>
-      </c>
-      <c r="N11" t="s">
-        <v>91</v>
-      </c>
       <c r="O11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="P11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Q11">
         <v>20</v>
@@ -5029,57 +5441,57 @@
         <v>15</v>
       </c>
       <c r="W11" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>117</v>
+      </c>
+      <c r="B12" t="s">
+        <v>106</v>
+      </c>
+      <c r="C12" t="s">
+        <v>107</v>
+      </c>
+      <c r="D12" t="s">
+        <v>108</v>
+      </c>
+      <c r="E12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" t="s">
         <v>118</v>
-      </c>
-      <c r="B12" t="s">
-        <v>107</v>
-      </c>
-      <c r="C12" t="s">
-        <v>108</v>
-      </c>
-      <c r="D12" t="s">
-        <v>109</v>
-      </c>
-      <c r="E12" t="s">
-        <v>15</v>
-      </c>
-      <c r="F12" t="s">
-        <v>119</v>
       </c>
       <c r="G12" s="5">
         <v>44755</v>
       </c>
       <c r="H12" t="s">
+        <v>88</v>
+      </c>
+      <c r="I12" t="s">
         <v>89</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
+        <v>15</v>
+      </c>
+      <c r="K12" t="s">
+        <v>15</v>
+      </c>
+      <c r="L12" t="s">
+        <v>88</v>
+      </c>
+      <c r="M12" t="s">
+        <v>89</v>
+      </c>
+      <c r="N12" t="s">
         <v>90</v>
       </c>
-      <c r="J12" t="s">
-        <v>15</v>
-      </c>
-      <c r="K12" t="s">
-        <v>15</v>
-      </c>
-      <c r="L12" t="s">
-        <v>89</v>
-      </c>
-      <c r="M12" t="s">
-        <v>90</v>
-      </c>
-      <c r="N12" t="s">
-        <v>91</v>
-      </c>
       <c r="O12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="P12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Q12">
         <v>20</v>
@@ -5100,57 +5512,57 @@
         <v>15</v>
       </c>
       <c r="W12" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>119</v>
+      </c>
+      <c r="B13" t="s">
+        <v>106</v>
+      </c>
+      <c r="C13" t="s">
+        <v>107</v>
+      </c>
+      <c r="D13" t="s">
+        <v>108</v>
+      </c>
+      <c r="E13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" t="s">
         <v>120</v>
-      </c>
-      <c r="B13" t="s">
-        <v>107</v>
-      </c>
-      <c r="C13" t="s">
-        <v>108</v>
-      </c>
-      <c r="D13" t="s">
-        <v>109</v>
-      </c>
-      <c r="E13" t="s">
-        <v>15</v>
-      </c>
-      <c r="F13" t="s">
-        <v>121</v>
       </c>
       <c r="G13" s="5">
         <v>44755</v>
       </c>
       <c r="H13" t="s">
+        <v>88</v>
+      </c>
+      <c r="I13" t="s">
         <v>89</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" t="s">
+        <v>15</v>
+      </c>
+      <c r="K13" t="s">
+        <v>15</v>
+      </c>
+      <c r="L13" t="s">
+        <v>88</v>
+      </c>
+      <c r="M13" t="s">
+        <v>89</v>
+      </c>
+      <c r="N13" t="s">
         <v>90</v>
       </c>
-      <c r="J13" t="s">
-        <v>15</v>
-      </c>
-      <c r="K13" t="s">
-        <v>15</v>
-      </c>
-      <c r="L13" t="s">
-        <v>89</v>
-      </c>
-      <c r="M13" t="s">
-        <v>90</v>
-      </c>
-      <c r="N13" t="s">
-        <v>91</v>
-      </c>
       <c r="O13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="P13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Q13">
         <v>20</v>
@@ -5171,57 +5583,57 @@
         <v>15</v>
       </c>
       <c r="W13" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>121</v>
+      </c>
+      <c r="B14" t="s">
+        <v>106</v>
+      </c>
+      <c r="C14" t="s">
+        <v>107</v>
+      </c>
+      <c r="D14" t="s">
+        <v>108</v>
+      </c>
+      <c r="E14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" t="s">
         <v>122</v>
-      </c>
-      <c r="B14" t="s">
-        <v>107</v>
-      </c>
-      <c r="C14" t="s">
-        <v>108</v>
-      </c>
-      <c r="D14" t="s">
-        <v>109</v>
-      </c>
-      <c r="E14" t="s">
-        <v>15</v>
-      </c>
-      <c r="F14" t="s">
-        <v>123</v>
       </c>
       <c r="G14" s="5">
         <v>44755</v>
       </c>
       <c r="H14" t="s">
+        <v>89</v>
+      </c>
+      <c r="I14" t="s">
+        <v>89</v>
+      </c>
+      <c r="J14" t="s">
+        <v>15</v>
+      </c>
+      <c r="K14" t="s">
+        <v>15</v>
+      </c>
+      <c r="L14" t="s">
+        <v>88</v>
+      </c>
+      <c r="M14" t="s">
+        <v>89</v>
+      </c>
+      <c r="N14" t="s">
         <v>90</v>
       </c>
-      <c r="I14" t="s">
-        <v>90</v>
-      </c>
-      <c r="J14" t="s">
-        <v>15</v>
-      </c>
-      <c r="K14" t="s">
-        <v>15</v>
-      </c>
-      <c r="L14" t="s">
-        <v>89</v>
-      </c>
-      <c r="M14" t="s">
-        <v>90</v>
-      </c>
-      <c r="N14" t="s">
-        <v>91</v>
-      </c>
       <c r="O14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="P14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Q14">
         <v>20</v>
@@ -5242,57 +5654,57 @@
         <v>15</v>
       </c>
       <c r="W14" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>123</v>
+      </c>
+      <c r="B15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C15" t="s">
+        <v>107</v>
+      </c>
+      <c r="D15" t="s">
+        <v>108</v>
+      </c>
+      <c r="E15" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" t="s">
         <v>124</v>
-      </c>
-      <c r="B15" t="s">
-        <v>107</v>
-      </c>
-      <c r="C15" t="s">
-        <v>108</v>
-      </c>
-      <c r="D15" t="s">
-        <v>109</v>
-      </c>
-      <c r="E15" t="s">
-        <v>15</v>
-      </c>
-      <c r="F15" t="s">
-        <v>125</v>
       </c>
       <c r="G15" s="5">
         <v>44755</v>
       </c>
       <c r="H15" t="s">
+        <v>89</v>
+      </c>
+      <c r="I15" t="s">
+        <v>89</v>
+      </c>
+      <c r="J15" t="s">
+        <v>15</v>
+      </c>
+      <c r="K15" t="s">
+        <v>15</v>
+      </c>
+      <c r="L15" t="s">
+        <v>88</v>
+      </c>
+      <c r="M15" t="s">
+        <v>89</v>
+      </c>
+      <c r="N15" t="s">
         <v>90</v>
       </c>
-      <c r="I15" t="s">
-        <v>90</v>
-      </c>
-      <c r="J15" t="s">
-        <v>15</v>
-      </c>
-      <c r="K15" t="s">
-        <v>15</v>
-      </c>
-      <c r="L15" t="s">
-        <v>89</v>
-      </c>
-      <c r="M15" t="s">
-        <v>90</v>
-      </c>
-      <c r="N15" t="s">
-        <v>91</v>
-      </c>
       <c r="O15" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="P15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Q15">
         <v>20</v>
@@ -5313,57 +5725,57 @@
         <v>15</v>
       </c>
       <c r="W15" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>125</v>
+      </c>
+      <c r="B16" t="s">
+        <v>106</v>
+      </c>
+      <c r="C16" t="s">
+        <v>107</v>
+      </c>
+      <c r="D16" t="s">
+        <v>108</v>
+      </c>
+      <c r="E16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" t="s">
         <v>126</v>
-      </c>
-      <c r="B16" t="s">
-        <v>107</v>
-      </c>
-      <c r="C16" t="s">
-        <v>108</v>
-      </c>
-      <c r="D16" t="s">
-        <v>109</v>
-      </c>
-      <c r="E16" t="s">
-        <v>15</v>
-      </c>
-      <c r="F16" t="s">
-        <v>127</v>
       </c>
       <c r="G16" s="5">
         <v>44755</v>
       </c>
       <c r="H16" t="s">
+        <v>89</v>
+      </c>
+      <c r="I16" t="s">
+        <v>89</v>
+      </c>
+      <c r="J16" t="s">
+        <v>15</v>
+      </c>
+      <c r="K16" t="s">
+        <v>15</v>
+      </c>
+      <c r="L16" t="s">
+        <v>89</v>
+      </c>
+      <c r="M16" t="s">
+        <v>89</v>
+      </c>
+      <c r="N16" t="s">
         <v>90</v>
       </c>
-      <c r="I16" t="s">
-        <v>90</v>
-      </c>
-      <c r="J16" t="s">
-        <v>15</v>
-      </c>
-      <c r="K16" t="s">
-        <v>15</v>
-      </c>
-      <c r="L16" t="s">
-        <v>90</v>
-      </c>
-      <c r="M16" t="s">
-        <v>90</v>
-      </c>
-      <c r="N16" t="s">
-        <v>91</v>
-      </c>
       <c r="O16" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="P16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Q16">
         <v>20</v>
@@ -5384,57 +5796,57 @@
         <v>15</v>
       </c>
       <c r="W16" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>127</v>
+      </c>
+      <c r="B17" t="s">
+        <v>106</v>
+      </c>
+      <c r="C17" t="s">
+        <v>107</v>
+      </c>
+      <c r="D17" t="s">
+        <v>108</v>
+      </c>
+      <c r="E17" t="s">
         <v>128</v>
       </c>
-      <c r="B17" t="s">
-        <v>107</v>
-      </c>
-      <c r="C17" t="s">
-        <v>108</v>
-      </c>
-      <c r="D17" t="s">
-        <v>109</v>
-      </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>129</v>
-      </c>
-      <c r="F17" t="s">
-        <v>130</v>
       </c>
       <c r="G17" s="5">
         <v>44756</v>
       </c>
       <c r="H17" t="s">
+        <v>89</v>
+      </c>
+      <c r="I17" t="s">
+        <v>89</v>
+      </c>
+      <c r="J17" t="s">
+        <v>15</v>
+      </c>
+      <c r="K17" t="s">
+        <v>15</v>
+      </c>
+      <c r="L17" t="s">
+        <v>89</v>
+      </c>
+      <c r="M17" t="s">
+        <v>89</v>
+      </c>
+      <c r="N17" t="s">
         <v>90</v>
       </c>
-      <c r="I17" t="s">
-        <v>90</v>
-      </c>
-      <c r="J17" t="s">
-        <v>15</v>
-      </c>
-      <c r="K17" t="s">
-        <v>15</v>
-      </c>
-      <c r="L17" t="s">
-        <v>90</v>
-      </c>
-      <c r="M17" t="s">
-        <v>90</v>
-      </c>
-      <c r="N17" t="s">
-        <v>91</v>
-      </c>
       <c r="O17" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="P17" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Q17">
         <v>20</v>
@@ -5455,57 +5867,57 @@
         <v>15</v>
       </c>
       <c r="W17" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>130</v>
+      </c>
+      <c r="B18" t="s">
+        <v>106</v>
+      </c>
+      <c r="C18" t="s">
+        <v>107</v>
+      </c>
+      <c r="D18" t="s">
+        <v>108</v>
+      </c>
+      <c r="E18" t="s">
+        <v>128</v>
+      </c>
+      <c r="F18" t="s">
         <v>131</v>
-      </c>
-      <c r="B18" t="s">
-        <v>107</v>
-      </c>
-      <c r="C18" t="s">
-        <v>108</v>
-      </c>
-      <c r="D18" t="s">
-        <v>109</v>
-      </c>
-      <c r="E18" t="s">
-        <v>129</v>
-      </c>
-      <c r="F18" t="s">
-        <v>132</v>
       </c>
       <c r="G18" s="5">
         <v>44756</v>
       </c>
       <c r="H18" t="s">
+        <v>89</v>
+      </c>
+      <c r="I18" t="s">
+        <v>89</v>
+      </c>
+      <c r="J18" t="s">
+        <v>15</v>
+      </c>
+      <c r="K18" t="s">
+        <v>15</v>
+      </c>
+      <c r="L18" t="s">
+        <v>88</v>
+      </c>
+      <c r="M18" t="s">
+        <v>89</v>
+      </c>
+      <c r="N18" t="s">
         <v>90</v>
       </c>
-      <c r="I18" t="s">
-        <v>90</v>
-      </c>
-      <c r="J18" t="s">
-        <v>15</v>
-      </c>
-      <c r="K18" t="s">
-        <v>15</v>
-      </c>
-      <c r="L18" t="s">
-        <v>89</v>
-      </c>
-      <c r="M18" t="s">
-        <v>90</v>
-      </c>
-      <c r="N18" t="s">
-        <v>91</v>
-      </c>
       <c r="O18" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="P18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Q18">
         <v>20</v>
@@ -5526,57 +5938,57 @@
         <v>15</v>
       </c>
       <c r="W18" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>132</v>
+      </c>
+      <c r="B19" t="s">
+        <v>106</v>
+      </c>
+      <c r="C19" t="s">
+        <v>107</v>
+      </c>
+      <c r="D19" t="s">
+        <v>108</v>
+      </c>
+      <c r="E19" t="s">
+        <v>128</v>
+      </c>
+      <c r="F19" t="s">
         <v>133</v>
-      </c>
-      <c r="B19" t="s">
-        <v>107</v>
-      </c>
-      <c r="C19" t="s">
-        <v>108</v>
-      </c>
-      <c r="D19" t="s">
-        <v>109</v>
-      </c>
-      <c r="E19" t="s">
-        <v>129</v>
-      </c>
-      <c r="F19" t="s">
-        <v>134</v>
       </c>
       <c r="G19" s="5">
         <v>44756</v>
       </c>
       <c r="H19" t="s">
+        <v>88</v>
+      </c>
+      <c r="I19" t="s">
         <v>89</v>
       </c>
-      <c r="I19" t="s">
+      <c r="J19" t="s">
+        <v>15</v>
+      </c>
+      <c r="K19" t="s">
+        <v>15</v>
+      </c>
+      <c r="L19" t="s">
+        <v>88</v>
+      </c>
+      <c r="M19" t="s">
+        <v>89</v>
+      </c>
+      <c r="N19" t="s">
         <v>90</v>
       </c>
-      <c r="J19" t="s">
-        <v>15</v>
-      </c>
-      <c r="K19" t="s">
-        <v>15</v>
-      </c>
-      <c r="L19" t="s">
-        <v>89</v>
-      </c>
-      <c r="M19" t="s">
-        <v>90</v>
-      </c>
-      <c r="N19" t="s">
-        <v>91</v>
-      </c>
       <c r="O19" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="P19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Q19">
         <v>20</v>
@@ -5597,57 +6009,57 @@
         <v>15</v>
       </c>
       <c r="W19" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>134</v>
+      </c>
+      <c r="B20" t="s">
+        <v>106</v>
+      </c>
+      <c r="C20" t="s">
+        <v>107</v>
+      </c>
+      <c r="D20" t="s">
+        <v>108</v>
+      </c>
+      <c r="E20" t="s">
+        <v>128</v>
+      </c>
+      <c r="F20" t="s">
         <v>135</v>
-      </c>
-      <c r="B20" t="s">
-        <v>107</v>
-      </c>
-      <c r="C20" t="s">
-        <v>108</v>
-      </c>
-      <c r="D20" t="s">
-        <v>109</v>
-      </c>
-      <c r="E20" t="s">
-        <v>129</v>
-      </c>
-      <c r="F20" t="s">
-        <v>136</v>
       </c>
       <c r="G20" s="5">
         <v>44757</v>
       </c>
       <c r="H20" t="s">
+        <v>89</v>
+      </c>
+      <c r="I20" t="s">
+        <v>89</v>
+      </c>
+      <c r="J20" t="s">
+        <v>15</v>
+      </c>
+      <c r="K20" t="s">
+        <v>15</v>
+      </c>
+      <c r="L20" t="s">
+        <v>89</v>
+      </c>
+      <c r="M20" t="s">
+        <v>89</v>
+      </c>
+      <c r="N20" t="s">
         <v>90</v>
       </c>
-      <c r="I20" t="s">
-        <v>90</v>
-      </c>
-      <c r="J20" t="s">
-        <v>15</v>
-      </c>
-      <c r="K20" t="s">
-        <v>15</v>
-      </c>
-      <c r="L20" t="s">
-        <v>90</v>
-      </c>
-      <c r="M20" t="s">
-        <v>90</v>
-      </c>
-      <c r="N20" t="s">
-        <v>91</v>
-      </c>
       <c r="O20" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="P20" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Q20">
         <v>20</v>
@@ -5668,57 +6080,57 @@
         <v>15</v>
       </c>
       <c r="W20" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>136</v>
+      </c>
+      <c r="B21" t="s">
+        <v>106</v>
+      </c>
+      <c r="C21" t="s">
+        <v>107</v>
+      </c>
+      <c r="D21" t="s">
+        <v>108</v>
+      </c>
+      <c r="E21" t="s">
+        <v>128</v>
+      </c>
+      <c r="F21" t="s">
         <v>137</v>
-      </c>
-      <c r="B21" t="s">
-        <v>107</v>
-      </c>
-      <c r="C21" t="s">
-        <v>108</v>
-      </c>
-      <c r="D21" t="s">
-        <v>109</v>
-      </c>
-      <c r="E21" t="s">
-        <v>129</v>
-      </c>
-      <c r="F21" t="s">
-        <v>138</v>
       </c>
       <c r="G21" s="5">
         <v>44757</v>
       </c>
       <c r="H21" t="s">
+        <v>89</v>
+      </c>
+      <c r="I21" t="s">
+        <v>89</v>
+      </c>
+      <c r="J21" t="s">
+        <v>15</v>
+      </c>
+      <c r="K21" t="s">
+        <v>15</v>
+      </c>
+      <c r="L21" t="s">
+        <v>88</v>
+      </c>
+      <c r="M21" t="s">
+        <v>89</v>
+      </c>
+      <c r="N21" t="s">
         <v>90</v>
       </c>
-      <c r="I21" t="s">
-        <v>90</v>
-      </c>
-      <c r="J21" t="s">
-        <v>15</v>
-      </c>
-      <c r="K21" t="s">
-        <v>15</v>
-      </c>
-      <c r="L21" t="s">
-        <v>89</v>
-      </c>
-      <c r="M21" t="s">
-        <v>90</v>
-      </c>
-      <c r="N21" t="s">
-        <v>91</v>
-      </c>
       <c r="O21" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="P21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Q21">
         <v>20</v>
@@ -5739,57 +6151,57 @@
         <v>15</v>
       </c>
       <c r="W21" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>138</v>
+      </c>
+      <c r="B22" t="s">
+        <v>106</v>
+      </c>
+      <c r="C22" t="s">
+        <v>107</v>
+      </c>
+      <c r="D22" t="s">
+        <v>108</v>
+      </c>
+      <c r="E22" t="s">
+        <v>128</v>
+      </c>
+      <c r="F22" t="s">
         <v>139</v>
-      </c>
-      <c r="B22" t="s">
-        <v>107</v>
-      </c>
-      <c r="C22" t="s">
-        <v>108</v>
-      </c>
-      <c r="D22" t="s">
-        <v>109</v>
-      </c>
-      <c r="E22" t="s">
-        <v>129</v>
-      </c>
-      <c r="F22" t="s">
-        <v>140</v>
       </c>
       <c r="G22" s="5">
         <v>44757</v>
       </c>
       <c r="H22" t="s">
+        <v>88</v>
+      </c>
+      <c r="I22" t="s">
         <v>89</v>
       </c>
-      <c r="I22" t="s">
+      <c r="J22" t="s">
+        <v>15</v>
+      </c>
+      <c r="K22" t="s">
+        <v>15</v>
+      </c>
+      <c r="L22" t="s">
+        <v>88</v>
+      </c>
+      <c r="M22" t="s">
+        <v>89</v>
+      </c>
+      <c r="N22" t="s">
         <v>90</v>
       </c>
-      <c r="J22" t="s">
-        <v>15</v>
-      </c>
-      <c r="K22" t="s">
-        <v>15</v>
-      </c>
-      <c r="L22" t="s">
-        <v>89</v>
-      </c>
-      <c r="M22" t="s">
-        <v>90</v>
-      </c>
-      <c r="N22" t="s">
-        <v>91</v>
-      </c>
       <c r="O22" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="P22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Q22">
         <v>20</v>
@@ -5810,7 +6222,7 @@
         <v>15</v>
       </c>
       <c r="W22" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Major updates: update skipped-breeding scripts and data viz.
</commit_message>
<xml_diff>
--- a/Simulation_log_key.xlsx
+++ b/Simulation_log_key.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zeus\Documents\R\working_directory\LemonSharkCKMR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4CF8340-DE81-4178-8AC3-6E04FC435323}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{162D298E-7AF6-4E7A-81C2-C3709C1F2B12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,6 +19,7 @@
     <sheet name="model_settings_old" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -67,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="805" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="979" uniqueCount="229">
   <si>
     <t>Objective</t>
   </si>
@@ -709,6 +710,57 @@
   </si>
   <si>
     <t>Conformists</t>
+  </si>
+  <si>
+    <t>Old runs - replaced with runs that are not highlighted in green</t>
+  </si>
+  <si>
+    <t>scenario_3.6.1</t>
+  </si>
+  <si>
+    <t>scenario_3.6.2</t>
+  </si>
+  <si>
+    <t>scenario_3.6.3</t>
+  </si>
+  <si>
+    <t>scenario_3.7.1</t>
+  </si>
+  <si>
+    <t>scenario_3.7.2</t>
+  </si>
+  <si>
+    <t>scenario_3.7.3</t>
+  </si>
+  <si>
+    <t>scenario_3.8.1</t>
+  </si>
+  <si>
+    <t>scenario_3.8.2</t>
+  </si>
+  <si>
+    <t>scenario_3.8.3</t>
+  </si>
+  <si>
+    <t>scenario_3.9.1</t>
+  </si>
+  <si>
+    <t>scenario_3.9.2</t>
+  </si>
+  <si>
+    <t>scenario_3.9.3</t>
+  </si>
+  <si>
+    <t>Psi prior</t>
+  </si>
+  <si>
+    <t>Uniform 0-1</t>
+  </si>
+  <si>
+    <t>Fixed to 1</t>
+  </si>
+  <si>
+    <t>Can't run bc probabilities of odd comparisons are 0</t>
   </si>
 </sst>
 </file>
@@ -1634,10 +1686,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L37"/>
+  <dimension ref="A1:M61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1651,12 +1703,13 @@
     <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="43.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="72.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.85546875" customWidth="1"/>
+    <col min="11" max="11" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="72.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>36</v>
       </c>
@@ -1685,17 +1738,20 @@
         <v>5</v>
       </c>
       <c r="J1" t="s">
+        <v>225</v>
+      </c>
+      <c r="K1" t="s">
         <v>24</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>2</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>37</v>
       </c>
       <c r="B2" s="7"/>
@@ -1720,18 +1776,18 @@
       <c r="I2" t="s">
         <v>32</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>25</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>17</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>38</v>
       </c>
       <c r="B3" s="7"/>
@@ -1756,18 +1812,18 @@
       <c r="I3" t="s">
         <v>19</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>25</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+    <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>54</v>
       </c>
       <c r="B4" s="6"/>
@@ -1792,18 +1848,18 @@
       <c r="I4" t="s">
         <v>19</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>25</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>17</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="M4" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+    <row r="5" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>55</v>
       </c>
       <c r="B5" s="6"/>
@@ -1828,18 +1884,18 @@
       <c r="I5" t="s">
         <v>19</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>25</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="M5" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>40</v>
       </c>
       <c r="B6" s="8"/>
@@ -1864,18 +1920,18 @@
       <c r="I6" t="s">
         <v>19</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>26</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>17</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="M6" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+    <row r="7" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>41</v>
       </c>
       <c r="B7" s="6"/>
@@ -1900,18 +1956,18 @@
       <c r="I7" t="s">
         <v>19</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>26</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>17</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="M7" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+    <row r="8" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>140</v>
       </c>
       <c r="B8" s="10" t="s">
@@ -1935,13 +1991,13 @@
       <c r="H8" t="s">
         <v>18</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>17</v>
       </c>
-      <c r="L8" s="1"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="M8" s="1"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>141</v>
       </c>
       <c r="B9" s="6"/>
@@ -1963,13 +2019,13 @@
       <c r="H9" t="s">
         <v>18</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>17</v>
       </c>
-      <c r="L9" s="1"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="M9" s="1"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>49</v>
       </c>
       <c r="B10" s="6"/>
@@ -1995,14 +2051,17 @@
         <v>19</v>
       </c>
       <c r="J10" t="s">
+        <v>15</v>
+      </c>
+      <c r="K10" t="s">
         <v>25</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>50</v>
       </c>
       <c r="B11" s="9" t="s">
@@ -2030,14 +2089,17 @@
         <v>19</v>
       </c>
       <c r="J11" t="s">
+        <v>15</v>
+      </c>
+      <c r="K11" t="s">
         <v>26</v>
       </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>182</v>
       </c>
       <c r="B12" s="9" t="s">
@@ -2065,13 +2127,16 @@
         <v>19</v>
       </c>
       <c r="J12" t="s">
+        <v>15</v>
+      </c>
+      <c r="K12" t="s">
         <v>26</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>51</v>
       </c>
@@ -2097,15 +2162,16 @@
       <c r="I13" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J13" s="2" t="s">
+      <c r="J13" s="2"/>
+      <c r="K13" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="K13" s="2" t="s">
+      <c r="L13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L13" s="2"/>
-    </row>
-    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M13" s="2"/>
+    </row>
+    <row r="14" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>52</v>
       </c>
@@ -2131,15 +2197,16 @@
       <c r="I14" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J14" s="2" t="s">
+      <c r="J14" s="2"/>
+      <c r="K14" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="K14" s="2" t="s">
+      <c r="L14" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L14" s="2"/>
-    </row>
-    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M14" s="2"/>
+    </row>
+    <row r="15" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>186</v>
       </c>
@@ -2165,15 +2232,16 @@
       <c r="I15" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J15" s="2" t="s">
+      <c r="J15" s="2"/>
+      <c r="K15" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="K15" s="2" t="s">
+      <c r="L15" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L15" s="2"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M15" s="2"/>
+    </row>
+    <row r="16" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>56</v>
       </c>
@@ -2199,14 +2267,17 @@
       <c r="I16" t="s">
         <v>19</v>
       </c>
-      <c r="J16" t="s">
+      <c r="K16" t="s">
         <v>53</v>
       </c>
-      <c r="K16" t="s">
+      <c r="L16" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M16" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>57</v>
       </c>
@@ -2232,14 +2303,14 @@
       <c r="I17" t="s">
         <v>19</v>
       </c>
-      <c r="J17" t="s">
+      <c r="K17" t="s">
         <v>27</v>
       </c>
-      <c r="K17" t="s">
+      <c r="L17" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>142</v>
       </c>
@@ -2265,17 +2336,17 @@
       <c r="I18" t="s">
         <v>19</v>
       </c>
-      <c r="J18" t="s">
+      <c r="K18" t="s">
         <v>27</v>
       </c>
-      <c r="K18" t="s">
+      <c r="L18" t="s">
         <v>17</v>
       </c>
-      <c r="L18" t="s">
+      <c r="M18" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>144</v>
       </c>
@@ -2301,14 +2372,14 @@
       <c r="I19" t="s">
         <v>19</v>
       </c>
-      <c r="J19" t="s">
+      <c r="K19" t="s">
         <v>27</v>
       </c>
-      <c r="K19" t="s">
+      <c r="L19" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
         <v>51</v>
       </c>
@@ -2335,13 +2406,13 @@
         <v>19</v>
       </c>
       <c r="J20" s="13" t="s">
-        <v>203</v>
-      </c>
-      <c r="K20" s="13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+      <c r="K20" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
         <v>52</v>
       </c>
@@ -2368,13 +2439,13 @@
         <v>19</v>
       </c>
       <c r="J21" s="13" t="s">
-        <v>204</v>
-      </c>
-      <c r="K21" s="13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+      <c r="K21" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
         <v>186</v>
       </c>
@@ -2401,13 +2472,13 @@
         <v>19</v>
       </c>
       <c r="J22" s="13" t="s">
-        <v>204</v>
-      </c>
-      <c r="K22" s="13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+      <c r="K22" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
         <v>56</v>
       </c>
@@ -2434,13 +2505,13 @@
         <v>19</v>
       </c>
       <c r="J23" s="13" t="s">
-        <v>203</v>
-      </c>
-      <c r="K23" s="13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+      <c r="K23" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
         <v>57</v>
       </c>
@@ -2467,13 +2538,13 @@
         <v>19</v>
       </c>
       <c r="J24" s="13" t="s">
-        <v>204</v>
-      </c>
-      <c r="K24" s="13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+      <c r="K24" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
         <v>142</v>
       </c>
@@ -2500,13 +2571,13 @@
         <v>19</v>
       </c>
       <c r="J25" s="13" t="s">
-        <v>204</v>
-      </c>
-      <c r="K25" s="13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+      <c r="K25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
         <v>205</v>
       </c>
@@ -2533,13 +2604,13 @@
         <v>19</v>
       </c>
       <c r="J26" s="13" t="s">
-        <v>203</v>
-      </c>
-      <c r="K26" s="13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+      <c r="K26" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
         <v>206</v>
       </c>
@@ -2566,13 +2637,13 @@
         <v>19</v>
       </c>
       <c r="J27" s="13" t="s">
-        <v>204</v>
-      </c>
-      <c r="K27" s="13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+      <c r="K27" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
         <v>207</v>
       </c>
@@ -2599,13 +2670,13 @@
         <v>19</v>
       </c>
       <c r="J28" s="13" t="s">
-        <v>204</v>
-      </c>
-      <c r="K28" s="13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+      <c r="K28" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
         <v>208</v>
       </c>
@@ -2632,13 +2703,13 @@
         <v>19</v>
       </c>
       <c r="J29" s="13" t="s">
-        <v>203</v>
-      </c>
-      <c r="K29" s="13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+      <c r="K29" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
         <v>209</v>
       </c>
@@ -2665,13 +2736,13 @@
         <v>19</v>
       </c>
       <c r="J30" s="13" t="s">
-        <v>204</v>
-      </c>
-      <c r="K30" s="13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+      <c r="K30" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
         <v>210</v>
       </c>
@@ -2698,207 +2769,1014 @@
         <v>19</v>
       </c>
       <c r="J31" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="K31" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" s="13" t="s">
+        <v>213</v>
+      </c>
+      <c r="B32" s="13"/>
+      <c r="C32" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="D32" s="13">
+        <v>2</v>
+      </c>
+      <c r="E32" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F32" s="14">
+        <v>1</v>
+      </c>
+      <c r="G32" s="13">
+        <v>1</v>
+      </c>
+      <c r="H32" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="I32" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J32" s="13" t="s">
+        <v>227</v>
+      </c>
+      <c r="K32" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="B33" s="13"/>
+      <c r="C33" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="D33" s="13">
+        <v>2</v>
+      </c>
+      <c r="E33" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F33" s="14">
+        <v>1</v>
+      </c>
+      <c r="G33" s="13">
+        <v>1</v>
+      </c>
+      <c r="H33" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="I33" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J33" s="13" t="s">
+        <v>227</v>
+      </c>
+      <c r="K33" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" s="13" t="s">
+        <v>215</v>
+      </c>
+      <c r="B34" s="13"/>
+      <c r="C34" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="D34" s="13">
+        <v>2</v>
+      </c>
+      <c r="E34" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F34" s="14">
+        <v>1</v>
+      </c>
+      <c r="G34" s="13">
+        <v>1</v>
+      </c>
+      <c r="H34" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="I34" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J34" s="13" t="s">
+        <v>227</v>
+      </c>
+      <c r="K34" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="13" t="s">
+        <v>216</v>
+      </c>
+      <c r="B35" s="13"/>
+      <c r="C35" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="D35" s="13">
+        <v>2</v>
+      </c>
+      <c r="E35" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F35" s="14">
+        <v>0.9</v>
+      </c>
+      <c r="G35" s="13">
+        <v>1</v>
+      </c>
+      <c r="H35" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="I35" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J35" s="13" t="s">
+        <v>227</v>
+      </c>
+      <c r="K35" t="s">
+        <v>27</v>
+      </c>
+      <c r="L35" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="13" t="s">
+        <v>217</v>
+      </c>
+      <c r="B36" s="13"/>
+      <c r="C36" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="D36" s="13">
+        <v>2</v>
+      </c>
+      <c r="E36" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F36" s="14">
+        <v>0.9</v>
+      </c>
+      <c r="G36" s="13">
+        <v>1</v>
+      </c>
+      <c r="H36" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="I36" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J36" s="13" t="s">
+        <v>227</v>
+      </c>
+      <c r="K36" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="13" t="s">
+        <v>218</v>
+      </c>
+      <c r="B37" s="13"/>
+      <c r="C37" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="D37" s="13">
+        <v>2</v>
+      </c>
+      <c r="E37" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F37" s="14">
+        <v>0.9</v>
+      </c>
+      <c r="G37" s="13">
+        <v>1</v>
+      </c>
+      <c r="H37" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="I37" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J37" s="13" t="s">
+        <v>227</v>
+      </c>
+      <c r="K37" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="13" t="s">
+        <v>219</v>
+      </c>
+      <c r="B38" s="13"/>
+      <c r="C38" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="D38" s="13">
+        <v>2</v>
+      </c>
+      <c r="E38" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F38" s="14">
+        <v>0.75</v>
+      </c>
+      <c r="G38" s="13">
+        <v>1</v>
+      </c>
+      <c r="H38" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="I38" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J38" s="13" t="s">
+        <v>227</v>
+      </c>
+      <c r="K38" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B39" s="13"/>
+      <c r="C39" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="D39" s="13">
+        <v>2</v>
+      </c>
+      <c r="E39" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F39" s="14">
+        <v>0.75</v>
+      </c>
+      <c r="G39" s="13">
+        <v>1</v>
+      </c>
+      <c r="H39" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="I39" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J39" s="13" t="s">
+        <v>227</v>
+      </c>
+      <c r="K39" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="13" t="s">
+        <v>221</v>
+      </c>
+      <c r="B40" s="13"/>
+      <c r="C40" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="D40" s="13">
+        <v>2</v>
+      </c>
+      <c r="E40" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F40" s="14">
+        <v>0.75</v>
+      </c>
+      <c r="G40" s="13">
+        <v>1</v>
+      </c>
+      <c r="H40" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="I40" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J40" s="13" t="s">
+        <v>227</v>
+      </c>
+      <c r="K40" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="13" t="s">
+        <v>222</v>
+      </c>
+      <c r="B41" s="13"/>
+      <c r="C41" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="D41" s="13">
+        <v>2</v>
+      </c>
+      <c r="E41" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F41" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="G41" s="13">
+        <v>1</v>
+      </c>
+      <c r="H41" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="I41" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J41" s="13" t="s">
+        <v>227</v>
+      </c>
+      <c r="K41" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="13" t="s">
+        <v>223</v>
+      </c>
+      <c r="B42" s="13"/>
+      <c r="C42" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="D42" s="13">
+        <v>2</v>
+      </c>
+      <c r="E42" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F42" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="G42" s="13">
+        <v>1</v>
+      </c>
+      <c r="H42" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="I42" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J42" s="13" t="s">
+        <v>227</v>
+      </c>
+      <c r="K42" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="13" t="s">
+        <v>224</v>
+      </c>
+      <c r="B43" s="13"/>
+      <c r="C43" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="D43" s="13">
+        <v>2</v>
+      </c>
+      <c r="E43" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F43" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="G43" s="13">
+        <v>1</v>
+      </c>
+      <c r="H43" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="I43" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J43" s="13" t="s">
+        <v>227</v>
+      </c>
+      <c r="K43" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B44" s="13"/>
+      <c r="C44" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="D44" s="13">
+        <v>2</v>
+      </c>
+      <c r="E44" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F44" s="14">
+        <v>1</v>
+      </c>
+      <c r="G44" s="13">
+        <v>1</v>
+      </c>
+      <c r="H44" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="I44" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J44" s="13"/>
+      <c r="K44" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="L44" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="B45" s="13"/>
+      <c r="C45" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="D45" s="13">
+        <v>2</v>
+      </c>
+      <c r="E45" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F45" s="14">
+        <v>1</v>
+      </c>
+      <c r="G45" s="13">
+        <v>1</v>
+      </c>
+      <c r="H45" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="I45" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J45" s="13"/>
+      <c r="K45" s="13" t="s">
         <v>204</v>
       </c>
-      <c r="K31" s="13" t="s">
+      <c r="L45" s="13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A32" s="7" t="s">
+    <row r="46" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="B46" s="13"/>
+      <c r="C46" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="D46" s="13">
+        <v>2</v>
+      </c>
+      <c r="E46" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F46" s="14">
+        <v>1</v>
+      </c>
+      <c r="G46" s="13">
+        <v>1</v>
+      </c>
+      <c r="H46" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="I46" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J46" s="13"/>
+      <c r="K46" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="L46" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B47" s="13"/>
+      <c r="C47" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="D47" s="13">
+        <v>2</v>
+      </c>
+      <c r="E47" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F47" s="14">
+        <v>0.9</v>
+      </c>
+      <c r="G47" s="13">
+        <v>1</v>
+      </c>
+      <c r="H47" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="I47" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J47" s="13"/>
+      <c r="K47" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="L47" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B48" s="13"/>
+      <c r="C48" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="D48" s="13">
+        <v>2</v>
+      </c>
+      <c r="E48" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F48" s="14">
+        <v>0.9</v>
+      </c>
+      <c r="G48" s="13">
+        <v>1</v>
+      </c>
+      <c r="H48" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="I48" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J48" s="13"/>
+      <c r="K48" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="L48" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="B49" s="13"/>
+      <c r="C49" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="D49" s="13">
+        <v>2</v>
+      </c>
+      <c r="E49" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F49" s="14">
+        <v>0.9</v>
+      </c>
+      <c r="G49" s="13">
+        <v>1</v>
+      </c>
+      <c r="H49" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="I49" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J49" s="13"/>
+      <c r="K49" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="L49" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="13" t="s">
+        <v>205</v>
+      </c>
+      <c r="B50" s="13"/>
+      <c r="C50" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="D50" s="13">
+        <v>2</v>
+      </c>
+      <c r="E50" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F50" s="14">
+        <v>0.75</v>
+      </c>
+      <c r="G50" s="13">
+        <v>1</v>
+      </c>
+      <c r="H50" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="I50" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J50" s="13"/>
+      <c r="K50" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="L50" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="13" t="s">
+        <v>206</v>
+      </c>
+      <c r="B51" s="13"/>
+      <c r="C51" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="D51" s="13">
+        <v>2</v>
+      </c>
+      <c r="E51" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F51" s="14">
+        <v>0.75</v>
+      </c>
+      <c r="G51" s="13">
+        <v>1</v>
+      </c>
+      <c r="H51" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="I51" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J51" s="13"/>
+      <c r="K51" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="L51" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="13" t="s">
+        <v>207</v>
+      </c>
+      <c r="B52" s="13"/>
+      <c r="C52" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="D52" s="13">
+        <v>2</v>
+      </c>
+      <c r="E52" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F52" s="14">
+        <v>0.75</v>
+      </c>
+      <c r="G52" s="13">
+        <v>1</v>
+      </c>
+      <c r="H52" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="I52" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J52" s="13"/>
+      <c r="K52" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="L52" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="13" t="s">
+        <v>208</v>
+      </c>
+      <c r="B53" s="13"/>
+      <c r="C53" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="D53" s="13">
+        <v>2</v>
+      </c>
+      <c r="E53" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F53" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="G53" s="13">
+        <v>1</v>
+      </c>
+      <c r="H53" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="I53" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J53" s="13"/>
+      <c r="K53" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="L53" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="13" t="s">
+        <v>209</v>
+      </c>
+      <c r="B54" s="13"/>
+      <c r="C54" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="D54" s="13">
+        <v>2</v>
+      </c>
+      <c r="E54" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F54" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="G54" s="13">
+        <v>1</v>
+      </c>
+      <c r="H54" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="I54" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J54" s="13"/>
+      <c r="K54" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="L54" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="13" t="s">
+        <v>210</v>
+      </c>
+      <c r="B55" s="13"/>
+      <c r="C55" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="D55" s="13">
+        <v>2</v>
+      </c>
+      <c r="E55" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F55" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="G55" s="13">
+        <v>1</v>
+      </c>
+      <c r="H55" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="I55" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J55" s="13"/>
+      <c r="K55" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="L55" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A56" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="B32" s="7"/>
-      <c r="C32" s="1" t="s">
+      <c r="B56" s="7"/>
+      <c r="C56" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="D32">
+      <c r="D56">
         <v>2</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E56" t="s">
         <v>152</v>
       </c>
-      <c r="F32" s="4">
-        <v>0</v>
-      </c>
-      <c r="G32">
-        <v>1</v>
-      </c>
-      <c r="H32" t="s">
+      <c r="F56" s="14">
+        <v>1</v>
+      </c>
+      <c r="G56">
+        <v>1</v>
+      </c>
+      <c r="H56" t="s">
         <v>58</v>
       </c>
-      <c r="I32" t="s">
+      <c r="I56" t="s">
         <v>19</v>
       </c>
-      <c r="J32" t="s">
+      <c r="K56" t="s">
         <v>27</v>
       </c>
-      <c r="K32" t="s">
+      <c r="L56" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A33" s="7" t="s">
+    <row r="57" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A57" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="B33" s="7"/>
-      <c r="C33" s="1" t="s">
+      <c r="B57" s="7"/>
+      <c r="C57" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="D33">
+      <c r="D57">
         <v>2</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E57" t="s">
         <v>152</v>
       </c>
-      <c r="F33" s="4">
-        <v>0</v>
-      </c>
-      <c r="G33">
-        <v>1</v>
-      </c>
-      <c r="H33" t="s">
+      <c r="F57" s="14">
+        <v>1</v>
+      </c>
+      <c r="G57">
+        <v>1</v>
+      </c>
+      <c r="H57" t="s">
         <v>18</v>
       </c>
-      <c r="I33" t="s">
+      <c r="I57" t="s">
         <v>19</v>
       </c>
-      <c r="J33" t="s">
+      <c r="K57" t="s">
         <v>27</v>
       </c>
-      <c r="K33" t="s">
+      <c r="L57" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="7" t="s">
+    <row r="58" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A58" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="B34" s="7"/>
-      <c r="C34" s="1" t="s">
+      <c r="B58" s="7"/>
+      <c r="C58" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="D34">
+      <c r="D58">
         <v>2</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E58" t="s">
         <v>152</v>
       </c>
-      <c r="F34" s="4">
-        <v>0</v>
-      </c>
-      <c r="G34">
-        <v>1</v>
-      </c>
-      <c r="H34" t="s">
-        <v>15</v>
-      </c>
-      <c r="I34" t="s">
+      <c r="F58" s="14">
+        <v>1</v>
+      </c>
+      <c r="G58">
+        <v>1</v>
+      </c>
+      <c r="H58" t="s">
+        <v>15</v>
+      </c>
+      <c r="I58" t="s">
         <v>19</v>
       </c>
-      <c r="J34" t="s">
+      <c r="K58" t="s">
         <v>27</v>
       </c>
-      <c r="K34" t="s">
+      <c r="L58" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A35" s="7" t="s">
+    <row r="59" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A59" s="7" t="s">
         <v>200</v>
       </c>
-      <c r="B35" s="7"/>
-      <c r="C35" s="1" t="s">
+      <c r="B59" s="7"/>
+      <c r="C59" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="D35">
+      <c r="D59">
         <v>2</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E59" t="s">
         <v>152</v>
       </c>
-      <c r="F35" s="4">
-        <v>0</v>
-      </c>
-      <c r="G35">
-        <v>1</v>
-      </c>
-      <c r="H35" t="s">
+      <c r="F59" s="14">
+        <v>1</v>
+      </c>
+      <c r="G59">
+        <v>1</v>
+      </c>
+      <c r="H59" t="s">
         <v>58</v>
       </c>
-      <c r="I35" t="s">
+      <c r="I59" t="s">
         <v>19</v>
       </c>
-      <c r="J35" t="s">
+      <c r="K59" t="s">
         <v>27</v>
       </c>
-      <c r="K35" t="s">
+      <c r="L59" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A36" s="7" t="s">
+    <row r="60" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A60" s="7" t="s">
         <v>201</v>
       </c>
-      <c r="B36" s="7"/>
-      <c r="C36" s="1" t="s">
+      <c r="B60" s="7"/>
+      <c r="C60" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="D36">
+      <c r="D60">
         <v>2</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E60" t="s">
         <v>152</v>
       </c>
-      <c r="F36" s="4">
-        <v>0</v>
-      </c>
-      <c r="G36">
-        <v>1</v>
-      </c>
-      <c r="H36" t="s">
+      <c r="F60" s="14">
+        <v>1</v>
+      </c>
+      <c r="G60">
+        <v>1</v>
+      </c>
+      <c r="H60" t="s">
         <v>18</v>
       </c>
-      <c r="I36" t="s">
+      <c r="I60" t="s">
         <v>19</v>
       </c>
-      <c r="J36" t="s">
+      <c r="K60" t="s">
         <v>27</v>
       </c>
-      <c r="K36" t="s">
+      <c r="L60" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="7" t="s">
+    <row r="61" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A61" s="7" t="s">
         <v>202</v>
       </c>
-      <c r="B37" s="7"/>
-      <c r="C37" s="1" t="s">
+      <c r="B61" s="7"/>
+      <c r="C61" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="D37">
+      <c r="D61">
         <v>2</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E61" t="s">
         <v>152</v>
       </c>
-      <c r="F37" s="4">
-        <v>0</v>
-      </c>
-      <c r="G37">
-        <v>1</v>
-      </c>
-      <c r="H37" t="s">
-        <v>15</v>
-      </c>
-      <c r="I37" t="s">
+      <c r="F61" s="14">
+        <v>1</v>
+      </c>
+      <c r="G61">
+        <v>1</v>
+      </c>
+      <c r="H61" t="s">
+        <v>15</v>
+      </c>
+      <c r="I61" t="s">
         <v>19</v>
       </c>
-      <c r="J37" t="s">
+      <c r="K61" t="s">
         <v>27</v>
       </c>
-      <c r="K37" t="s">
+      <c r="L61" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update all the aging error scripts
</commit_message>
<xml_diff>
--- a/Simulation_log_key.xlsx
+++ b/Simulation_log_key.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zeus\Documents\R\working_directory\LemonSharkCKMR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\Documents\R\working_directory\LemonSharkCKMR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{162D298E-7AF6-4E7A-81C2-C3709C1F2B12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08F7170F-2C19-4FD2-A86F-78FF07139412}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,6 @@
     <sheet name="model_settings_old" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -68,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="979" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1001" uniqueCount="233">
   <si>
     <t>Objective</t>
   </si>
@@ -761,6 +760,18 @@
   </si>
   <si>
     <t>Can't run bc probabilities of odd comparisons are 0</t>
+  </si>
+  <si>
+    <t>scenario_4.3.1</t>
+  </si>
+  <si>
+    <t>scenario_4.3.2</t>
+  </si>
+  <si>
+    <t>scenario_4.3.3</t>
+  </si>
+  <si>
+    <t>age miss CV</t>
   </si>
 </sst>
 </file>
@@ -1686,30 +1697,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M61"/>
+  <dimension ref="A1:N64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="K64" sqref="K64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="56.7109375" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="28.7109375" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.85546875" customWidth="1"/>
-    <col min="11" max="11" width="43.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="72.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.109375" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="56.6640625" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="28.6640625" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5546875" customWidth="1"/>
+    <col min="7" max="7" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="16.88671875" customWidth="1"/>
+    <col min="12" max="12" width="43.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="72.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>36</v>
       </c>
@@ -1741,16 +1752,19 @@
         <v>225</v>
       </c>
       <c r="K1" t="s">
+        <v>232</v>
+      </c>
+      <c r="L1" t="s">
         <v>24</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>2</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -1776,17 +1790,20 @@
       <c r="I2" t="s">
         <v>32</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2" t="s">
         <v>25</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>17</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -1812,17 +1829,20 @@
       <c r="I3" t="s">
         <v>19</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3" t="s">
         <v>25</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>17</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>54</v>
       </c>
@@ -1848,17 +1868,20 @@
       <c r="I4" t="s">
         <v>19</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4" t="s">
         <v>25</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="N4" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>55</v>
       </c>
@@ -1884,17 +1907,20 @@
       <c r="I5" t="s">
         <v>19</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5" t="s">
         <v>25</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>17</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="N5" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -1920,17 +1946,20 @@
       <c r="I6" t="s">
         <v>19</v>
       </c>
-      <c r="K6" t="s">
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6" t="s">
         <v>26</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>17</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="N6" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>41</v>
       </c>
@@ -1956,17 +1985,20 @@
       <c r="I7" t="s">
         <v>19</v>
       </c>
-      <c r="K7" t="s">
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7" t="s">
         <v>26</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>17</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="N7" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>140</v>
       </c>
@@ -1991,12 +2023,15 @@
       <c r="H8" t="s">
         <v>18</v>
       </c>
-      <c r="L8" t="s">
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="M8" t="s">
         <v>17</v>
       </c>
-      <c r="M8" s="1"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N8" s="1"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>141</v>
       </c>
@@ -2019,12 +2054,15 @@
       <c r="H9" t="s">
         <v>18</v>
       </c>
-      <c r="L9" t="s">
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="M9" t="s">
         <v>17</v>
       </c>
-      <c r="M9" s="1"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N9" s="1"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>49</v>
       </c>
@@ -2053,14 +2091,17 @@
       <c r="J10" t="s">
         <v>15</v>
       </c>
-      <c r="K10" t="s">
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10" t="s">
         <v>25</v>
       </c>
-      <c r="L10" t="s">
+      <c r="M10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>50</v>
       </c>
@@ -2091,14 +2132,17 @@
       <c r="J11" t="s">
         <v>15</v>
       </c>
-      <c r="K11" t="s">
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11" t="s">
         <v>26</v>
       </c>
-      <c r="L11" t="s">
+      <c r="M11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>182</v>
       </c>
@@ -2129,14 +2173,17 @@
       <c r="J12" t="s">
         <v>15</v>
       </c>
-      <c r="K12" t="s">
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12" t="s">
         <v>26</v>
       </c>
-      <c r="L12" t="s">
+      <c r="M12" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>51</v>
       </c>
@@ -2163,15 +2210,16 @@
         <v>19</v>
       </c>
       <c r="J13" s="2"/>
-      <c r="K13" s="2" t="s">
+      <c r="K13" s="2"/>
+      <c r="L13" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="L13" s="2" t="s">
+      <c r="M13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="M13" s="2"/>
-    </row>
-    <row r="14" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="N13" s="2"/>
+    </row>
+    <row r="14" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>52</v>
       </c>
@@ -2198,15 +2246,16 @@
         <v>19</v>
       </c>
       <c r="J14" s="2"/>
-      <c r="K14" s="2" t="s">
+      <c r="K14" s="2"/>
+      <c r="L14" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="L14" s="2" t="s">
+      <c r="M14" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="M14" s="2"/>
-    </row>
-    <row r="15" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="N14" s="2"/>
+    </row>
+    <row r="15" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>186</v>
       </c>
@@ -2233,15 +2282,16 @@
         <v>19</v>
       </c>
       <c r="J15" s="2"/>
-      <c r="K15" s="2" t="s">
+      <c r="K15" s="2"/>
+      <c r="L15" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="L15" s="2" t="s">
+      <c r="M15" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="M15" s="2"/>
-    </row>
-    <row r="16" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="N15" s="2"/>
+    </row>
+    <row r="16" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>56</v>
       </c>
@@ -2267,17 +2317,17 @@
       <c r="I16" t="s">
         <v>19</v>
       </c>
-      <c r="K16" t="s">
+      <c r="L16" t="s">
         <v>53</v>
       </c>
-      <c r="L16" t="s">
+      <c r="M16" t="s">
         <v>17</v>
       </c>
-      <c r="M16" t="s">
+      <c r="N16" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="17" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
         <v>57</v>
       </c>
@@ -2303,14 +2353,14 @@
       <c r="I17" t="s">
         <v>19</v>
       </c>
-      <c r="K17" t="s">
+      <c r="L17" t="s">
         <v>27</v>
       </c>
-      <c r="L17" t="s">
+      <c r="M17" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
         <v>142</v>
       </c>
@@ -2336,17 +2386,17 @@
       <c r="I18" t="s">
         <v>19</v>
       </c>
-      <c r="K18" t="s">
+      <c r="L18" t="s">
         <v>27</v>
       </c>
-      <c r="L18" t="s">
+      <c r="M18" t="s">
         <v>17</v>
       </c>
-      <c r="M18" t="s">
+      <c r="N18" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="19" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
         <v>144</v>
       </c>
@@ -2372,14 +2422,14 @@
       <c r="I19" t="s">
         <v>19</v>
       </c>
-      <c r="K19" t="s">
+      <c r="L19" t="s">
         <v>27</v>
       </c>
-      <c r="L19" t="s">
+      <c r="M19" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" s="13" t="s">
         <v>51</v>
       </c>
@@ -2408,11 +2458,14 @@
       <c r="J20" s="13" t="s">
         <v>226</v>
       </c>
-      <c r="K20" t="s">
+      <c r="K20" s="13">
+        <v>0</v>
+      </c>
+      <c r="L20" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" s="13" t="s">
         <v>52</v>
       </c>
@@ -2441,11 +2494,14 @@
       <c r="J21" s="13" t="s">
         <v>226</v>
       </c>
-      <c r="K21" t="s">
+      <c r="K21" s="13">
+        <v>0</v>
+      </c>
+      <c r="L21" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" s="13" t="s">
         <v>186</v>
       </c>
@@ -2474,11 +2530,14 @@
       <c r="J22" s="13" t="s">
         <v>226</v>
       </c>
-      <c r="K22" t="s">
+      <c r="K22" s="13">
+        <v>0</v>
+      </c>
+      <c r="L22" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" s="13" t="s">
         <v>56</v>
       </c>
@@ -2507,11 +2566,14 @@
       <c r="J23" s="13" t="s">
         <v>226</v>
       </c>
-      <c r="K23" t="s">
+      <c r="K23" s="13">
+        <v>0</v>
+      </c>
+      <c r="L23" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" s="13" t="s">
         <v>57</v>
       </c>
@@ -2540,11 +2602,14 @@
       <c r="J24" s="13" t="s">
         <v>226</v>
       </c>
-      <c r="K24" t="s">
+      <c r="K24" s="13">
+        <v>0</v>
+      </c>
+      <c r="L24" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" s="13" t="s">
         <v>142</v>
       </c>
@@ -2573,11 +2638,14 @@
       <c r="J25" s="13" t="s">
         <v>226</v>
       </c>
-      <c r="K25" t="s">
+      <c r="K25" s="13">
+        <v>0</v>
+      </c>
+      <c r="L25" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" s="13" t="s">
         <v>205</v>
       </c>
@@ -2606,11 +2674,14 @@
       <c r="J26" s="13" t="s">
         <v>226</v>
       </c>
-      <c r="K26" t="s">
+      <c r="K26" s="13">
+        <v>0</v>
+      </c>
+      <c r="L26" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" s="13" t="s">
         <v>206</v>
       </c>
@@ -2639,11 +2710,14 @@
       <c r="J27" s="13" t="s">
         <v>226</v>
       </c>
-      <c r="K27" t="s">
+      <c r="K27" s="13">
+        <v>0</v>
+      </c>
+      <c r="L27" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" s="13" t="s">
         <v>207</v>
       </c>
@@ -2672,11 +2746,14 @@
       <c r="J28" s="13" t="s">
         <v>226</v>
       </c>
-      <c r="K28" t="s">
+      <c r="K28" s="13">
+        <v>0</v>
+      </c>
+      <c r="L28" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" s="13" t="s">
         <v>208</v>
       </c>
@@ -2705,11 +2782,14 @@
       <c r="J29" s="13" t="s">
         <v>226</v>
       </c>
-      <c r="K29" t="s">
+      <c r="K29" s="13">
+        <v>0</v>
+      </c>
+      <c r="L29" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" s="13" t="s">
         <v>209</v>
       </c>
@@ -2738,11 +2818,14 @@
       <c r="J30" s="13" t="s">
         <v>226</v>
       </c>
-      <c r="K30" t="s">
+      <c r="K30" s="13">
+        <v>0</v>
+      </c>
+      <c r="L30" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" s="13" t="s">
         <v>210</v>
       </c>
@@ -2771,11 +2854,14 @@
       <c r="J31" s="13" t="s">
         <v>226</v>
       </c>
-      <c r="K31" t="s">
+      <c r="K31" s="13">
+        <v>0</v>
+      </c>
+      <c r="L31" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" s="13" t="s">
         <v>213</v>
       </c>
@@ -2804,11 +2890,14 @@
       <c r="J32" s="13" t="s">
         <v>227</v>
       </c>
-      <c r="K32" t="s">
+      <c r="K32" s="13">
+        <v>0</v>
+      </c>
+      <c r="L32" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="13" t="s">
         <v>214</v>
       </c>
@@ -2837,11 +2926,14 @@
       <c r="J33" s="13" t="s">
         <v>227</v>
       </c>
-      <c r="K33" t="s">
+      <c r="K33" s="13">
+        <v>0</v>
+      </c>
+      <c r="L33" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="13" t="s">
         <v>215</v>
       </c>
@@ -2870,11 +2962,14 @@
       <c r="J34" s="13" t="s">
         <v>227</v>
       </c>
-      <c r="K34" t="s">
+      <c r="K34" s="13">
+        <v>0</v>
+      </c>
+      <c r="L34" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" s="13" t="s">
         <v>216</v>
       </c>
@@ -2903,14 +2998,15 @@
       <c r="J35" s="13" t="s">
         <v>227</v>
       </c>
-      <c r="K35" t="s">
+      <c r="K35" s="13"/>
+      <c r="L35" t="s">
         <v>27</v>
       </c>
-      <c r="L35" t="s">
+      <c r="M35" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="36" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" s="13" t="s">
         <v>217</v>
       </c>
@@ -2939,11 +3035,12 @@
       <c r="J36" s="13" t="s">
         <v>227</v>
       </c>
-      <c r="K36" t="s">
+      <c r="K36" s="13"/>
+      <c r="L36" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="37" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" s="13" t="s">
         <v>218</v>
       </c>
@@ -2972,11 +3069,12 @@
       <c r="J37" s="13" t="s">
         <v>227</v>
       </c>
-      <c r="K37" t="s">
+      <c r="K37" s="13"/>
+      <c r="L37" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="38" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" s="13" t="s">
         <v>219</v>
       </c>
@@ -3005,11 +3103,12 @@
       <c r="J38" s="13" t="s">
         <v>227</v>
       </c>
-      <c r="K38" t="s">
+      <c r="K38" s="13"/>
+      <c r="L38" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="39" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" s="13" t="s">
         <v>220</v>
       </c>
@@ -3038,11 +3137,12 @@
       <c r="J39" s="13" t="s">
         <v>227</v>
       </c>
-      <c r="K39" t="s">
+      <c r="K39" s="13"/>
+      <c r="L39" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="40" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" s="13" t="s">
         <v>221</v>
       </c>
@@ -3071,11 +3171,12 @@
       <c r="J40" s="13" t="s">
         <v>227</v>
       </c>
-      <c r="K40" t="s">
+      <c r="K40" s="13"/>
+      <c r="L40" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="41" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" s="13" t="s">
         <v>222</v>
       </c>
@@ -3104,11 +3205,12 @@
       <c r="J41" s="13" t="s">
         <v>227</v>
       </c>
-      <c r="K41" t="s">
+      <c r="K41" s="13"/>
+      <c r="L41" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="42" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" s="13" t="s">
         <v>223</v>
       </c>
@@ -3137,11 +3239,12 @@
       <c r="J42" s="13" t="s">
         <v>227</v>
       </c>
-      <c r="K42" t="s">
+      <c r="K42" s="13"/>
+      <c r="L42" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="43" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" s="13" t="s">
         <v>224</v>
       </c>
@@ -3170,11 +3273,12 @@
       <c r="J43" s="13" t="s">
         <v>227</v>
       </c>
-      <c r="K43" t="s">
+      <c r="K43" s="13"/>
+      <c r="L43" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="44" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" s="13" t="s">
         <v>51</v>
       </c>
@@ -3201,14 +3305,15 @@
         <v>19</v>
       </c>
       <c r="J44" s="13"/>
-      <c r="K44" s="13" t="s">
+      <c r="K44" s="13"/>
+      <c r="L44" s="13" t="s">
         <v>203</v>
       </c>
-      <c r="L44" s="13" t="s">
+      <c r="M44" s="13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="45" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" s="13" t="s">
         <v>52</v>
       </c>
@@ -3235,14 +3340,15 @@
         <v>19</v>
       </c>
       <c r="J45" s="13"/>
-      <c r="K45" s="13" t="s">
+      <c r="K45" s="13"/>
+      <c r="L45" s="13" t="s">
         <v>204</v>
       </c>
-      <c r="L45" s="13" t="s">
+      <c r="M45" s="13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="46" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" s="13" t="s">
         <v>186</v>
       </c>
@@ -3269,14 +3375,15 @@
         <v>19</v>
       </c>
       <c r="J46" s="13"/>
-      <c r="K46" s="13" t="s">
+      <c r="K46" s="13"/>
+      <c r="L46" s="13" t="s">
         <v>204</v>
       </c>
-      <c r="L46" s="13" t="s">
+      <c r="M46" s="13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="47" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" s="13" t="s">
         <v>56</v>
       </c>
@@ -3303,14 +3410,15 @@
         <v>19</v>
       </c>
       <c r="J47" s="13"/>
-      <c r="K47" s="13" t="s">
+      <c r="K47" s="13"/>
+      <c r="L47" s="13" t="s">
         <v>203</v>
       </c>
-      <c r="L47" s="13" t="s">
+      <c r="M47" s="13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="48" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" s="13" t="s">
         <v>57</v>
       </c>
@@ -3337,14 +3445,15 @@
         <v>19</v>
       </c>
       <c r="J48" s="13"/>
-      <c r="K48" s="13" t="s">
+      <c r="K48" s="13"/>
+      <c r="L48" s="13" t="s">
         <v>204</v>
       </c>
-      <c r="L48" s="13" t="s">
+      <c r="M48" s="13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="49" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" s="13" t="s">
         <v>142</v>
       </c>
@@ -3371,14 +3480,15 @@
         <v>19</v>
       </c>
       <c r="J49" s="13"/>
-      <c r="K49" s="13" t="s">
+      <c r="K49" s="13"/>
+      <c r="L49" s="13" t="s">
         <v>204</v>
       </c>
-      <c r="L49" s="13" t="s">
+      <c r="M49" s="13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="50" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" s="13" t="s">
         <v>205</v>
       </c>
@@ -3405,14 +3515,15 @@
         <v>19</v>
       </c>
       <c r="J50" s="13"/>
-      <c r="K50" s="13" t="s">
+      <c r="K50" s="13"/>
+      <c r="L50" s="13" t="s">
         <v>203</v>
       </c>
-      <c r="L50" s="13" t="s">
+      <c r="M50" s="13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="51" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" s="13" t="s">
         <v>206</v>
       </c>
@@ -3439,14 +3550,15 @@
         <v>19</v>
       </c>
       <c r="J51" s="13"/>
-      <c r="K51" s="13" t="s">
+      <c r="K51" s="13"/>
+      <c r="L51" s="13" t="s">
         <v>204</v>
       </c>
-      <c r="L51" s="13" t="s">
+      <c r="M51" s="13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="52" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" s="13" t="s">
         <v>207</v>
       </c>
@@ -3473,14 +3585,15 @@
         <v>19</v>
       </c>
       <c r="J52" s="13"/>
-      <c r="K52" s="13" t="s">
+      <c r="K52" s="13"/>
+      <c r="L52" s="13" t="s">
         <v>204</v>
       </c>
-      <c r="L52" s="13" t="s">
+      <c r="M52" s="13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="53" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" s="13" t="s">
         <v>208</v>
       </c>
@@ -3507,14 +3620,15 @@
         <v>19</v>
       </c>
       <c r="J53" s="13"/>
-      <c r="K53" s="13" t="s">
+      <c r="K53" s="13"/>
+      <c r="L53" s="13" t="s">
         <v>203</v>
       </c>
-      <c r="L53" s="13" t="s">
+      <c r="M53" s="13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="54" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" s="13" t="s">
         <v>209</v>
       </c>
@@ -3541,14 +3655,15 @@
         <v>19</v>
       </c>
       <c r="J54" s="13"/>
-      <c r="K54" s="13" t="s">
+      <c r="K54" s="13"/>
+      <c r="L54" s="13" t="s">
         <v>204</v>
       </c>
-      <c r="L54" s="13" t="s">
+      <c r="M54" s="13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="55" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" s="13" t="s">
         <v>210</v>
       </c>
@@ -3575,14 +3690,15 @@
         <v>19</v>
       </c>
       <c r="J55" s="13"/>
-      <c r="K55" s="13" t="s">
+      <c r="K55" s="13"/>
+      <c r="L55" s="13" t="s">
         <v>204</v>
       </c>
-      <c r="L55" s="13" t="s">
+      <c r="M55" s="13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="56" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A56" s="7" t="s">
         <v>191</v>
       </c>
@@ -3608,14 +3724,17 @@
       <c r="I56" t="s">
         <v>19</v>
       </c>
-      <c r="K56" t="s">
+      <c r="K56">
+        <v>0.05</v>
+      </c>
+      <c r="L56" t="s">
         <v>27</v>
       </c>
-      <c r="L56" t="s">
+      <c r="M56" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="57" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A57" s="7" t="s">
         <v>192</v>
       </c>
@@ -3641,14 +3760,17 @@
       <c r="I57" t="s">
         <v>19</v>
       </c>
-      <c r="K57" t="s">
+      <c r="K57">
+        <v>0.05</v>
+      </c>
+      <c r="L57" t="s">
         <v>27</v>
       </c>
-      <c r="L57" t="s">
+      <c r="M57" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="58" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A58" s="7" t="s">
         <v>193</v>
       </c>
@@ -3674,14 +3796,17 @@
       <c r="I58" t="s">
         <v>19</v>
       </c>
-      <c r="K58" t="s">
+      <c r="K58">
+        <v>0.05</v>
+      </c>
+      <c r="L58" t="s">
         <v>27</v>
       </c>
-      <c r="L58" t="s">
+      <c r="M58" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="59" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A59" s="7" t="s">
         <v>200</v>
       </c>
@@ -3707,14 +3832,17 @@
       <c r="I59" t="s">
         <v>19</v>
       </c>
-      <c r="K59" t="s">
+      <c r="K59">
+        <v>0.1</v>
+      </c>
+      <c r="L59" t="s">
         <v>27</v>
       </c>
-      <c r="L59" t="s">
+      <c r="M59" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="60" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A60" s="7" t="s">
         <v>201</v>
       </c>
@@ -3740,14 +3868,17 @@
       <c r="I60" t="s">
         <v>19</v>
       </c>
-      <c r="K60" t="s">
+      <c r="K60">
+        <v>0.1</v>
+      </c>
+      <c r="L60" t="s">
         <v>27</v>
       </c>
-      <c r="L60" t="s">
+      <c r="M60" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="61" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A61" s="7" t="s">
         <v>202</v>
       </c>
@@ -3773,10 +3904,121 @@
       <c r="I61" t="s">
         <v>19</v>
       </c>
-      <c r="K61" t="s">
+      <c r="K61">
+        <v>0.1</v>
+      </c>
+      <c r="L61" t="s">
         <v>27</v>
       </c>
-      <c r="L61" t="s">
+      <c r="M61" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A62" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="B62" s="7"/>
+      <c r="C62" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D62">
+        <v>2</v>
+      </c>
+      <c r="E62" t="s">
+        <v>152</v>
+      </c>
+      <c r="F62" s="14">
+        <v>1</v>
+      </c>
+      <c r="G62">
+        <v>1</v>
+      </c>
+      <c r="H62" t="s">
+        <v>58</v>
+      </c>
+      <c r="I62" t="s">
+        <v>19</v>
+      </c>
+      <c r="K62">
+        <v>0.2</v>
+      </c>
+      <c r="L62" t="s">
+        <v>27</v>
+      </c>
+      <c r="M62" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A63" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="B63" s="7"/>
+      <c r="C63" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D63">
+        <v>2</v>
+      </c>
+      <c r="E63" t="s">
+        <v>152</v>
+      </c>
+      <c r="F63" s="14">
+        <v>1</v>
+      </c>
+      <c r="G63">
+        <v>1</v>
+      </c>
+      <c r="H63" t="s">
+        <v>18</v>
+      </c>
+      <c r="I63" t="s">
+        <v>19</v>
+      </c>
+      <c r="K63">
+        <v>0.2</v>
+      </c>
+      <c r="L63" t="s">
+        <v>27</v>
+      </c>
+      <c r="M63" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A64" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="B64" s="7"/>
+      <c r="C64" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="D64">
+        <v>2</v>
+      </c>
+      <c r="E64" t="s">
+        <v>152</v>
+      </c>
+      <c r="F64" s="14">
+        <v>1</v>
+      </c>
+      <c r="G64">
+        <v>1</v>
+      </c>
+      <c r="H64" t="s">
+        <v>15</v>
+      </c>
+      <c r="I64" t="s">
+        <v>19</v>
+      </c>
+      <c r="K64">
+        <v>0.2</v>
+      </c>
+      <c r="L64" t="s">
+        <v>27</v>
+      </c>
+      <c r="M64" t="s">
         <v>17</v>
       </c>
     </row>
@@ -3794,23 +4036,23 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="52.7109375" customWidth="1"/>
-    <col min="2" max="2" width="47.7109375" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="47.7109375" customWidth="1"/>
-    <col min="5" max="5" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="26.7109375" customWidth="1"/>
-    <col min="8" max="8" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.7109375" customWidth="1"/>
-    <col min="10" max="12" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="26.140625" customWidth="1"/>
-    <col min="14" max="14" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="52.6640625" customWidth="1"/>
+    <col min="2" max="2" width="47.6640625" customWidth="1"/>
+    <col min="3" max="3" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="47.6640625" customWidth="1"/>
+    <col min="5" max="5" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="26.6640625" customWidth="1"/>
+    <col min="8" max="8" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.6640625" customWidth="1"/>
+    <col min="10" max="12" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="26.109375" customWidth="1"/>
+    <col min="14" max="14" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="34.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3842,7 +4084,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>159</v>
       </c>
@@ -3858,7 +4100,7 @@
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>171</v>
       </c>
@@ -3892,7 +4134,7 @@
       <c r="M3" s="1"/>
       <c r="O3" s="1"/>
     </row>
-    <row r="4" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>170</v>
       </c>
@@ -3924,7 +4166,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>178</v>
       </c>
@@ -3946,7 +4188,7 @@
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -3958,7 +4200,7 @@
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -3970,7 +4212,7 @@
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -3982,7 +4224,7 @@
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -3994,7 +4236,7 @@
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -4006,7 +4248,7 @@
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -4018,7 +4260,7 @@
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -4030,7 +4272,7 @@
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -4042,7 +4284,7 @@
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -4054,7 +4296,7 @@
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -4066,7 +4308,7 @@
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -4078,7 +4320,7 @@
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -4090,7 +4332,7 @@
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -4102,7 +4344,7 @@
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -4114,7 +4356,7 @@
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -4126,7 +4368,7 @@
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -4138,7 +4380,7 @@
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -4150,7 +4392,7 @@
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -4162,7 +4404,7 @@
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -4174,7 +4416,7 @@
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -4186,7 +4428,7 @@
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -4198,7 +4440,7 @@
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -4210,7 +4452,7 @@
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -4222,7 +4464,7 @@
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -4234,7 +4476,7 @@
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -4246,7 +4488,7 @@
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -4258,7 +4500,7 @@
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -4270,7 +4512,7 @@
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -4282,7 +4524,7 @@
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -4294,7 +4536,7 @@
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -4306,7 +4548,7 @@
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -4318,7 +4560,7 @@
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -4330,7 +4572,7 @@
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -4342,7 +4584,7 @@
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -4354,7 +4596,7 @@
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -4366,7 +4608,7 @@
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -4378,7 +4620,7 @@
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -4390,7 +4632,7 @@
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -4402,7 +4644,7 @@
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -4414,7 +4656,7 @@
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -4426,7 +4668,7 @@
       <c r="I45" s="1"/>
       <c r="J45" s="1"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -4438,7 +4680,7 @@
       <c r="I46" s="1"/>
       <c r="J46" s="1"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -4450,7 +4692,7 @@
       <c r="I47" s="1"/>
       <c r="J47" s="1"/>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -4462,7 +4704,7 @@
       <c r="I48" s="1"/>
       <c r="J48" s="1"/>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -4474,7 +4716,7 @@
       <c r="I49" s="1"/>
       <c r="J49" s="1"/>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -4486,7 +4728,7 @@
       <c r="I50" s="1"/>
       <c r="J50" s="1"/>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -4498,7 +4740,7 @@
       <c r="I51" s="1"/>
       <c r="J51" s="1"/>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -4510,7 +4752,7 @@
       <c r="I52" s="1"/>
       <c r="J52" s="1"/>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -4522,7 +4764,7 @@
       <c r="I53" s="1"/>
       <c r="J53" s="1"/>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -4534,7 +4776,7 @@
       <c r="I54" s="1"/>
       <c r="J54" s="1"/>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -4546,7 +4788,7 @@
       <c r="I55" s="1"/>
       <c r="J55" s="1"/>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -4558,7 +4800,7 @@
       <c r="I56" s="1"/>
       <c r="J56" s="1"/>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -4570,7 +4812,7 @@
       <c r="I57" s="1"/>
       <c r="J57" s="1"/>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -4582,7 +4824,7 @@
       <c r="I58" s="1"/>
       <c r="J58" s="1"/>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -4594,7 +4836,7 @@
       <c r="I59" s="1"/>
       <c r="J59" s="1"/>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -4606,7 +4848,7 @@
       <c r="I60" s="1"/>
       <c r="J60" s="1"/>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -4618,7 +4860,7 @@
       <c r="I61" s="1"/>
       <c r="J61" s="1"/>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -4630,7 +4872,7 @@
       <c r="I62" s="1"/>
       <c r="J62" s="1"/>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -4642,7 +4884,7 @@
       <c r="I63" s="1"/>
       <c r="J63" s="1"/>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -4654,7 +4896,7 @@
       <c r="I64" s="1"/>
       <c r="J64" s="1"/>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -4666,7 +4908,7 @@
       <c r="I65" s="1"/>
       <c r="J65" s="1"/>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -4678,7 +4920,7 @@
       <c r="I66" s="1"/>
       <c r="J66" s="1"/>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -4690,7 +4932,7 @@
       <c r="I67" s="1"/>
       <c r="J67" s="1"/>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -4702,7 +4944,7 @@
       <c r="I68" s="1"/>
       <c r="J68" s="1"/>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -4714,7 +4956,7 @@
       <c r="I69" s="1"/>
       <c r="J69" s="1"/>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -4726,7 +4968,7 @@
       <c r="I70" s="1"/>
       <c r="J70" s="1"/>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -4738,7 +4980,7 @@
       <c r="I71" s="1"/>
       <c r="J71" s="1"/>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -4750,7 +4992,7 @@
       <c r="I72" s="1"/>
       <c r="J72" s="1"/>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -4762,7 +5004,7 @@
       <c r="I73" s="1"/>
       <c r="J73" s="1"/>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -4774,7 +5016,7 @@
       <c r="I74" s="1"/>
       <c r="J74" s="1"/>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -4786,7 +5028,7 @@
       <c r="I75" s="1"/>
       <c r="J75" s="1"/>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -4798,7 +5040,7 @@
       <c r="I76" s="1"/>
       <c r="J76" s="1"/>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -4810,7 +5052,7 @@
       <c r="I77" s="1"/>
       <c r="J77" s="1"/>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -4822,7 +5064,7 @@
       <c r="I78" s="1"/>
       <c r="J78" s="1"/>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -4834,7 +5076,7 @@
       <c r="I79" s="1"/>
       <c r="J79" s="1"/>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -4846,7 +5088,7 @@
       <c r="I80" s="1"/>
       <c r="J80" s="1"/>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -4858,7 +5100,7 @@
       <c r="I81" s="1"/>
       <c r="J81" s="1"/>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -4870,7 +5112,7 @@
       <c r="I82" s="1"/>
       <c r="J82" s="1"/>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -4882,7 +5124,7 @@
       <c r="I83" s="1"/>
       <c r="J83" s="1"/>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -4894,7 +5136,7 @@
       <c r="I84" s="1"/>
       <c r="J84" s="1"/>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -4906,7 +5148,7 @@
       <c r="I85" s="1"/>
       <c r="J85" s="1"/>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -4918,7 +5160,7 @@
       <c r="I86" s="1"/>
       <c r="J86" s="1"/>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -4930,7 +5172,7 @@
       <c r="I87" s="1"/>
       <c r="J87" s="1"/>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -4942,7 +5184,7 @@
       <c r="I88" s="1"/>
       <c r="J88" s="1"/>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -4954,7 +5196,7 @@
       <c r="I89" s="1"/>
       <c r="J89" s="1"/>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
@@ -4966,7 +5208,7 @@
       <c r="I90" s="1"/>
       <c r="J90" s="1"/>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
@@ -4978,7 +5220,7 @@
       <c r="I91" s="1"/>
       <c r="J91" s="1"/>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -4990,7 +5232,7 @@
       <c r="I92" s="1"/>
       <c r="J92" s="1"/>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
@@ -5002,7 +5244,7 @@
       <c r="I93" s="1"/>
       <c r="J93" s="1"/>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
@@ -5014,7 +5256,7 @@
       <c r="I94" s="1"/>
       <c r="J94" s="1"/>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
@@ -5026,7 +5268,7 @@
       <c r="I95" s="1"/>
       <c r="J95" s="1"/>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
@@ -5038,7 +5280,7 @@
       <c r="I96" s="1"/>
       <c r="J96" s="1"/>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
@@ -5050,7 +5292,7 @@
       <c r="I97" s="1"/>
       <c r="J97" s="1"/>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
@@ -5062,7 +5304,7 @@
       <c r="I98" s="1"/>
       <c r="J98" s="1"/>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
@@ -5074,7 +5316,7 @@
       <c r="I99" s="1"/>
       <c r="J99" s="1"/>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
@@ -5086,7 +5328,7 @@
       <c r="I100" s="1"/>
       <c r="J100" s="1"/>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
@@ -5098,7 +5340,7 @@
       <c r="I101" s="1"/>
       <c r="J101" s="1"/>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
@@ -5110,7 +5352,7 @@
       <c r="I102" s="1"/>
       <c r="J102" s="1"/>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
@@ -5122,7 +5364,7 @@
       <c r="I103" s="1"/>
       <c r="J103" s="1"/>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
@@ -5134,7 +5376,7 @@
       <c r="I104" s="1"/>
       <c r="J104" s="1"/>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A105" s="1"/>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
@@ -5146,7 +5388,7 @@
       <c r="I105" s="1"/>
       <c r="J105" s="1"/>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
@@ -5158,7 +5400,7 @@
       <c r="I106" s="1"/>
       <c r="J106" s="1"/>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
@@ -5170,7 +5412,7 @@
       <c r="I107" s="1"/>
       <c r="J107" s="1"/>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A108" s="1"/>
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
@@ -5182,7 +5424,7 @@
       <c r="I108" s="1"/>
       <c r="J108" s="1"/>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A109" s="1"/>
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
@@ -5207,20 +5449,20 @@
       <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.5703125" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="43.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="72.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.5546875" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="43.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="72.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>36</v>
       </c>
@@ -5249,7 +5491,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -5278,7 +5520,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -5307,7 +5549,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -5336,7 +5578,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>40</v>
       </c>
@@ -5362,7 +5604,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>41</v>
       </c>
@@ -5391,7 +5633,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>42</v>
       </c>
@@ -5420,7 +5662,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>43</v>
       </c>
@@ -5446,7 +5688,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>44</v>
       </c>
@@ -5472,7 +5714,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>45</v>
       </c>
@@ -5480,12 +5722,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>10</v>
       </c>
@@ -5493,7 +5735,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>12</v>
       </c>
@@ -5514,34 +5756,34 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="79.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="98.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="62.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="79.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="98.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="62.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="69" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="77.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="77.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="8" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.88671875" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="17" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="41.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="41.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>61</v>
       </c>
@@ -5612,7 +5854,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>84</v>
       </c>
@@ -5683,7 +5925,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>94</v>
       </c>
@@ -5754,7 +5996,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>96</v>
       </c>
@@ -5825,7 +6067,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>98</v>
       </c>
@@ -5896,7 +6138,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>101</v>
       </c>
@@ -5967,7 +6209,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>103</v>
       </c>
@@ -6038,7 +6280,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>105</v>
       </c>
@@ -6109,7 +6351,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>110</v>
       </c>
@@ -6180,7 +6422,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>112</v>
       </c>
@@ -6251,7 +6493,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>114</v>
       </c>
@@ -6322,7 +6564,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>117</v>
       </c>
@@ -6393,7 +6635,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>119</v>
       </c>
@@ -6464,7 +6706,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>121</v>
       </c>
@@ -6535,7 +6777,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>123</v>
       </c>
@@ -6606,7 +6848,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>125</v>
       </c>
@@ -6677,7 +6919,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>127</v>
       </c>
@@ -6748,7 +6990,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>130</v>
       </c>
@@ -6819,7 +7061,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>132</v>
       </c>
@@ -6890,7 +7132,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>134</v>
       </c>
@@ -6961,7 +7203,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>136</v>
       </c>
@@ -7032,7 +7274,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>138</v>
       </c>

</xml_diff>

<commit_message>
Update viz scripts and simulation log
</commit_message>
<xml_diff>
--- a/Simulation_log_key.xlsx
+++ b/Simulation_log_key.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\Documents\R\working_directory\LemonSharkCKMR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08F7170F-2C19-4FD2-A86F-78FF07139412}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F546B0E-F4E0-481D-816D-FBED2E971E61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Simulation_log_key" sheetId="1" r:id="rId1"/>
@@ -1699,17 +1699,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="K64" sqref="K64"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="32.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.109375" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="56.6640625" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5546875" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="28.6640625" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="19.109375" customWidth="1"/>
+    <col min="3" max="3" width="56.6640625" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" customWidth="1"/>
+    <col min="5" max="5" width="28.6640625" customWidth="1"/>
     <col min="6" max="6" width="16.5546875" customWidth="1"/>
     <col min="7" max="7" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.109375" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
Update file organization and fix bugs in population simulation script.
</commit_message>
<xml_diff>
--- a/Simulation_log_key.xlsx
+++ b/Simulation_log_key.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\Documents\R\working_directory\LemonSharkCKMR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F546B0E-F4E0-481D-816D-FBED2E971E61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8687C4B8-FB18-4961-BD38-C6295EA6950F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5085" yWindow="-11640" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Simulation_log_key" sheetId="1" r:id="rId1"/>
@@ -1699,8 +1699,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>